<commit_message>
Update RS for MS-OXWSATT_R527.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$421</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$422</definedName>
     <definedName name="Appendix_A_1" localSheetId="0">Requirements!$B$403</definedName>
     <definedName name="Appendix_A_2" localSheetId="0">Requirements!$B$405</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="952">
   <si>
     <t>Req ID</t>
   </si>
@@ -2997,12 +2997,6 @@
 &lt;/xs:complexType&gt;</t>
   </si>
   <si>
-    <t>[In t:ItemAttachmentType Complex Type][The type of Item element is] t:ItemType ([MS-OXWSCORE] section 2.2.4.24).</t>
-  </si>
-  <si>
-    <t>[In t:ItemAttachmentType Complex Type][The Item element] Represents a generic item in the server store.&lt;3&gt;</t>
-  </si>
-  <si>
     <t>[In t:ItemAttachmentType Complex Type][The type of CalendarItem element is] t:CalendarItemType ([MS-OXWSMTGS] section 2.2.4.9)</t>
   </si>
   <si>
@@ -3484,18 +3478,12 @@
     <t>MS-OXWSATT_R346:i</t>
   </si>
   <si>
-    <t>MS-OXWSATT_R81:i</t>
-  </si>
-  <si>
     <t>MS-OXWSATT_R99006:i</t>
   </si>
   <si>
     <t>MS-OXWSATT_R104002:i</t>
   </si>
   <si>
-    <t>MS-OXWSATT_R309:i</t>
-  </si>
-  <si>
     <t>MS-OXWSATT_R311:i</t>
   </si>
   <si>
@@ -3521,9 +3509,6 @@
   </si>
   <si>
     <t>Verified by derived requirement: MS-OXWSATT_R318013.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXWSATT_R318014.</t>
   </si>
   <si>
     <t xml:space="preserve">[t:ReferenceAttachmentType Complex Type]This type extends the AttachmentType complex type (section 2.2.4.4). &lt;8&gt;
@@ -3549,6 +3534,27 @@
      &lt;/xs:extension&gt;
    &lt;/xs:complexContent&gt;
  &lt;/xs:complexType&gt;</t>
+  </si>
+  <si>
+    <t>MS-OXWSATT_R401:i</t>
+  </si>
+  <si>
+    <t>[In t:ItemAttachmentType Complex Type][The type of Item element is] t:ItemType ([MS-OXWSCORE] section 2.2.4.24).&lt;3&gt;</t>
+  </si>
+  <si>
+    <t>[In t:ItemAttachmentType Complex Type][The Item element] Represents a generic item in the server store.</t>
+  </si>
+  <si>
+    <t>MS-OXWSATT_R318015</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Exchange2007 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSATT_R318014, Ms-OXWSATT_R318015.</t>
+  </si>
+  <si>
+    <t>MS-OXWSATT_R527:i</t>
   </si>
 </sst>
 </file>
@@ -3861,27 +3867,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3906,11 +3891,76 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="147">
+  <dxfs count="113">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -4326,216 +4376,6 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5034,34 +4874,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I421" tableType="xml" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" connectionId="1">
-  <autoFilter ref="A19:I421"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I422" tableType="xml" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111" connectionId="1">
+  <autoFilter ref="A19:I422"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="144">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="110">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="143">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="109">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="142">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="108">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="141">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="107">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="140">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="106">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="139">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="105">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="138">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="104">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="137">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="103">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="136">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="102">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5070,12 +4910,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="135" dataDxfId="133" headerRowBorderDxfId="134" tableBorderDxfId="132" totalsRowBorderDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98" totalsRowBorderDxfId="97">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="130"/>
-    <tableColumn id="2" name="Test" dataDxfId="129"/>
-    <tableColumn id="3" name="Description" dataDxfId="128"/>
+    <tableColumn id="1" name="Scope" dataDxfId="96"/>
+    <tableColumn id="2" name="Test" dataDxfId="95"/>
+    <tableColumn id="3" name="Description" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5369,10 +5209,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M423"/>
+  <dimension ref="A1:M424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H138" sqref="H138"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C409" sqref="C409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5438,16 +5278,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -5459,13 +5299,13 @@
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -5473,16 +5313,16 @@
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -5490,16 +5330,16 @@
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -5507,16 +5347,16 @@
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -5524,16 +5364,16 @@
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -5541,16 +5381,16 @@
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="56" t="s">
         <v>749</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -5558,16 +5398,16 @@
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>748</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -5651,16 +5491,16 @@
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -5668,16 +5508,16 @@
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -5685,16 +5525,16 @@
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>750</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -7076,7 +6916,7 @@
     </row>
     <row r="73" spans="1:9" ht="30">
       <c r="A73" s="28" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B73" s="29" t="s">
         <v>393</v>
@@ -7923,7 +7763,7 @@
         <v>395</v>
       </c>
       <c r="C106" s="30" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D106" s="28"/>
       <c r="E106" s="28" t="s">
@@ -7939,7 +7779,7 @@
         <v>17</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="30">
@@ -8125,7 +7965,7 @@
         <v>396</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D114" s="28"/>
       <c r="E114" s="28" t="s">
@@ -8141,7 +7981,7 @@
         <v>17</v>
       </c>
       <c r="I114" s="30" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="30">
@@ -8293,7 +8133,7 @@
         <v>17</v>
       </c>
       <c r="I120" s="30" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="45">
@@ -8371,7 +8211,7 @@
       </c>
       <c r="I123" s="30"/>
     </row>
-    <row r="124" spans="1:9" ht="30">
+    <row r="124" spans="1:9" ht="60">
       <c r="A124" s="28" t="s">
         <v>136</v>
       </c>
@@ -8379,7 +8219,7 @@
         <v>397</v>
       </c>
       <c r="C124" s="30" t="s">
-        <v>780</v>
+        <v>946</v>
       </c>
       <c r="D124" s="28"/>
       <c r="E124" s="28" t="s">
@@ -8392,11 +8232,13 @@
         <v>15</v>
       </c>
       <c r="H124" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="I124" s="30"/>
-    </row>
-    <row r="125" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I124" s="30" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="28" t="s">
         <v>137</v>
       </c>
@@ -8404,7 +8246,7 @@
         <v>397</v>
       </c>
       <c r="C125" s="30" t="s">
-        <v>781</v>
+        <v>947</v>
       </c>
       <c r="D125" s="28"/>
       <c r="E125" s="28" t="s">
@@ -8417,11 +8259,9 @@
         <v>15</v>
       </c>
       <c r="H125" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I125" s="30" t="s">
-        <v>946</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I125" s="30"/>
     </row>
     <row r="126" spans="1:9" ht="30">
       <c r="A126" s="28" t="s">
@@ -8481,7 +8321,7 @@
         <v>397</v>
       </c>
       <c r="C128" s="30" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D128" s="28"/>
       <c r="E128" s="28" t="s">
@@ -8531,7 +8371,7 @@
         <v>397</v>
       </c>
       <c r="C130" s="30" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D130" s="28"/>
       <c r="E130" s="28" t="s">
@@ -8581,7 +8421,7 @@
         <v>397</v>
       </c>
       <c r="C132" s="30" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D132" s="28"/>
       <c r="E132" s="28" t="s">
@@ -8631,7 +8471,7 @@
         <v>397</v>
       </c>
       <c r="C134" s="30" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D134" s="28"/>
       <c r="E134" s="28" t="s">
@@ -8681,7 +8521,7 @@
         <v>397</v>
       </c>
       <c r="C136" s="30" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D136" s="28"/>
       <c r="E136" s="28" t="s">
@@ -8731,7 +8571,7 @@
         <v>397</v>
       </c>
       <c r="C138" s="30" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D138" s="28"/>
       <c r="E138" s="28" t="s">
@@ -8781,7 +8621,7 @@
         <v>397</v>
       </c>
       <c r="C140" s="30" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D140" s="28"/>
       <c r="E140" s="28" t="s">
@@ -8875,13 +8715,13 @@
     </row>
     <row r="144" spans="1:9" ht="30">
       <c r="A144" s="28" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B144" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C144" s="30" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D144" s="28"/>
       <c r="E144" s="28" t="s">
@@ -8900,13 +8740,13 @@
     </row>
     <row r="145" spans="1:9" ht="30">
       <c r="A145" s="28" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B145" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C145" s="30" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D145" s="28"/>
       <c r="E145" s="28" t="s">
@@ -8925,13 +8765,13 @@
     </row>
     <row r="146" spans="1:9" ht="30">
       <c r="A146" s="28" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B146" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C146" s="30" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D146" s="28"/>
       <c r="E146" s="28" t="s">
@@ -8950,13 +8790,13 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="28" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B147" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C147" s="30" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D147" s="28"/>
       <c r="E147" s="28" t="s">
@@ -8975,13 +8815,13 @@
     </row>
     <row r="148" spans="1:9" ht="30">
       <c r="A148" s="28" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B148" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C148" s="30" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D148" s="28"/>
       <c r="E148" s="28" t="s">
@@ -9000,13 +8840,13 @@
     </row>
     <row r="149" spans="1:9" ht="45">
       <c r="A149" s="28" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B149" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C149" s="30" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D149" s="28"/>
       <c r="E149" s="28" t="s">
@@ -9022,18 +8862,18 @@
         <v>17</v>
       </c>
       <c r="I149" s="30" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="30">
       <c r="A150" s="28" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B150" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C150" s="30" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D150" s="28"/>
       <c r="E150" s="28" t="s">
@@ -9052,13 +8892,13 @@
     </row>
     <row r="151" spans="1:9">
       <c r="A151" s="28" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B151" s="29" t="s">
         <v>397</v>
       </c>
       <c r="C151" s="30" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D151" s="28"/>
       <c r="E151" s="28" t="s">
@@ -9158,7 +8998,7 @@
         <v>398</v>
       </c>
       <c r="C155" s="30" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D155" s="28"/>
       <c r="E155" s="28" t="s">
@@ -9202,13 +9042,13 @@
     </row>
     <row r="157" spans="1:9" ht="30">
       <c r="A157" s="28" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B157" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C157" s="30" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D157" s="28"/>
       <c r="E157" s="28" t="s">
@@ -9227,13 +9067,13 @@
     </row>
     <row r="158" spans="1:9" ht="45">
       <c r="A158" s="28" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B158" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C158" s="30" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="D158" s="28"/>
       <c r="E158" s="28" t="s">
@@ -9249,18 +9089,18 @@
         <v>17</v>
       </c>
       <c r="I158" s="30" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="330">
       <c r="A159" s="28" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="B159" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C159" s="30" t="s">
-        <v>949</v>
+        <v>944</v>
       </c>
       <c r="D159" s="28"/>
       <c r="E159" s="28" t="s">
@@ -9279,13 +9119,13 @@
     </row>
     <row r="160" spans="1:9" ht="30">
       <c r="A160" s="28" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B160" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C160" s="30" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D160" s="28"/>
       <c r="E160" s="28" t="s">
@@ -9304,13 +9144,13 @@
     </row>
     <row r="161" spans="1:9" ht="30">
       <c r="A161" s="28" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B161" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C161" s="30" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D161" s="28"/>
       <c r="E161" s="28" t="s">
@@ -9329,13 +9169,13 @@
     </row>
     <row r="162" spans="1:9" ht="30">
       <c r="A162" s="28" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B162" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C162" s="30" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D162" s="28"/>
       <c r="E162" s="28" t="s">
@@ -9354,13 +9194,13 @@
     </row>
     <row r="163" spans="1:9" ht="30">
       <c r="A163" s="28" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B163" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C163" s="30" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D163" s="28"/>
       <c r="E163" s="28" t="s">
@@ -9379,13 +9219,13 @@
     </row>
     <row r="164" spans="1:9" ht="30">
       <c r="A164" s="28" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B164" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C164" s="30" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D164" s="28"/>
       <c r="E164" s="28" t="s">
@@ -9404,13 +9244,13 @@
     </row>
     <row r="165" spans="1:9" ht="30">
       <c r="A165" s="28" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B165" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C165" s="30" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D165" s="28"/>
       <c r="E165" s="28" t="s">
@@ -9429,13 +9269,13 @@
     </row>
     <row r="166" spans="1:9" ht="30">
       <c r="A166" s="28" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B166" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C166" s="30" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D166" s="28"/>
       <c r="E166" s="28" t="s">
@@ -9454,13 +9294,13 @@
     </row>
     <row r="167" spans="1:9" ht="30">
       <c r="A167" s="28" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B167" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C167" s="30" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D167" s="28"/>
       <c r="E167" s="28" t="s">
@@ -9479,13 +9319,13 @@
     </row>
     <row r="168" spans="1:9" ht="30">
       <c r="A168" s="28" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B168" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C168" s="30" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D168" s="28"/>
       <c r="E168" s="28" t="s">
@@ -9504,13 +9344,13 @@
     </row>
     <row r="169" spans="1:9" ht="30">
       <c r="A169" s="28" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B169" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C169" s="30" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D169" s="28"/>
       <c r="E169" s="28" t="s">
@@ -9529,13 +9369,13 @@
     </row>
     <row r="170" spans="1:9" ht="30">
       <c r="A170" s="28" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B170" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C170" s="30" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D170" s="28"/>
       <c r="E170" s="28" t="s">
@@ -9554,13 +9394,13 @@
     </row>
     <row r="171" spans="1:9" ht="30">
       <c r="A171" s="28" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C171" s="30" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D171" s="28"/>
       <c r="E171" s="28" t="s">
@@ -9579,13 +9419,13 @@
     </row>
     <row r="172" spans="1:9" ht="30">
       <c r="A172" s="28" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B172" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C172" s="30" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D172" s="28"/>
       <c r="E172" s="28" t="s">
@@ -9604,13 +9444,13 @@
     </row>
     <row r="173" spans="1:9" ht="30">
       <c r="A173" s="28" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B173" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C173" s="30" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D173" s="28"/>
       <c r="E173" s="28" t="s">
@@ -9629,13 +9469,13 @@
     </row>
     <row r="174" spans="1:9" ht="30">
       <c r="A174" s="28" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B174" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C174" s="30" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D174" s="28"/>
       <c r="E174" s="28" t="s">
@@ -9685,7 +9525,7 @@
         <v>400</v>
       </c>
       <c r="C176" s="30" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D176" s="28"/>
       <c r="E176" s="28" t="s">
@@ -9960,7 +9800,7 @@
         <v>405</v>
       </c>
       <c r="C187" s="30" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D187" s="28"/>
       <c r="E187" s="28" t="s">
@@ -10460,7 +10300,7 @@
         <v>32</v>
       </c>
       <c r="C207" s="30" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="D207" s="28"/>
       <c r="E207" s="28" t="s">
@@ -10739,7 +10579,7 @@
         <v>410</v>
       </c>
       <c r="C218" s="30" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D218" s="28"/>
       <c r="E218" s="28" t="s">
@@ -10789,7 +10629,7 @@
         <v>410</v>
       </c>
       <c r="C220" s="30" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D220" s="28"/>
       <c r="E220" s="28" t="s">
@@ -10864,7 +10704,7 @@
         <v>410</v>
       </c>
       <c r="C223" s="30" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D223" s="28"/>
       <c r="E223" s="28" t="s">
@@ -11089,7 +10929,7 @@
         <v>411</v>
       </c>
       <c r="C232" s="30" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D232" s="28"/>
       <c r="E232" s="28" t="s">
@@ -11139,7 +10979,7 @@
         <v>411</v>
       </c>
       <c r="C234" s="30" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D234" s="28"/>
       <c r="E234" s="28" t="s">
@@ -11183,13 +11023,13 @@
     </row>
     <row r="236" spans="1:9" ht="45">
       <c r="A236" s="28" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B236" s="29" t="s">
         <v>411</v>
       </c>
       <c r="C236" s="30" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D236" s="28"/>
       <c r="E236" s="28" t="s">
@@ -11208,13 +11048,13 @@
     </row>
     <row r="237" spans="1:9" ht="60">
       <c r="A237" s="28" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B237" s="29" t="s">
         <v>411</v>
       </c>
       <c r="C237" s="30" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="D237" s="28"/>
       <c r="E237" s="28" t="s">
@@ -11339,7 +11179,7 @@
         <v>414</v>
       </c>
       <c r="C242" s="30" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D242" s="28"/>
       <c r="E242" s="28" t="s">
@@ -11464,7 +11304,7 @@
         <v>416</v>
       </c>
       <c r="C247" s="30" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D247" s="28"/>
       <c r="E247" s="28" t="s">
@@ -11539,7 +11379,7 @@
         <v>417</v>
       </c>
       <c r="C250" s="30" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D250" s="28"/>
       <c r="E250" s="28" t="s">
@@ -11614,7 +11454,7 @@
         <v>417</v>
       </c>
       <c r="C253" s="30" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D253" s="28"/>
       <c r="E253" s="28" t="s">
@@ -11689,7 +11529,7 @@
         <v>417</v>
       </c>
       <c r="C256" s="30" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D256" s="28"/>
       <c r="E256" s="28" t="s">
@@ -11714,7 +11554,7 @@
         <v>417</v>
       </c>
       <c r="C257" s="30" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D257" s="28"/>
       <c r="E257" s="28" t="s">
@@ -11764,7 +11604,7 @@
         <v>33</v>
       </c>
       <c r="C259" s="30" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D259" s="28"/>
       <c r="E259" s="28" t="s">
@@ -11941,7 +11781,7 @@
         <v>33</v>
       </c>
       <c r="C266" s="30" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D266" s="28" t="s">
         <v>732</v>
@@ -11993,7 +11833,7 @@
         <v>33</v>
       </c>
       <c r="C268" s="30" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D268" s="28"/>
       <c r="E268" s="28" t="s">
@@ -12518,7 +12358,7 @@
         <v>420</v>
       </c>
       <c r="C289" s="30" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D289" s="28"/>
       <c r="E289" s="28" t="s">
@@ -12612,13 +12452,13 @@
     </row>
     <row r="293" spans="1:9" ht="45">
       <c r="A293" s="28" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B293" s="29" t="s">
         <v>420</v>
       </c>
       <c r="C293" s="30" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D293" s="28"/>
       <c r="E293" s="28" t="s">
@@ -12637,13 +12477,13 @@
     </row>
     <row r="294" spans="1:9" ht="60">
       <c r="A294" s="28" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B294" s="29" t="s">
         <v>420</v>
       </c>
       <c r="C294" s="30" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="D294" s="28"/>
       <c r="E294" s="28" t="s">
@@ -12843,7 +12683,7 @@
         <v>424</v>
       </c>
       <c r="C302" s="30" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D302" s="28"/>
       <c r="E302" s="28" t="s">
@@ -12912,13 +12752,13 @@
     </row>
     <row r="305" spans="1:9" ht="30">
       <c r="A305" s="28" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B305" s="29" t="s">
         <v>424</v>
       </c>
       <c r="C305" s="30" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D305" s="28"/>
       <c r="E305" s="28" t="s">
@@ -12937,13 +12777,13 @@
     </row>
     <row r="306" spans="1:9" ht="30">
       <c r="A306" s="28" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B306" s="29" t="s">
         <v>424</v>
       </c>
       <c r="C306" s="30" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D306" s="28"/>
       <c r="E306" s="28" t="s">
@@ -12993,7 +12833,7 @@
         <v>425</v>
       </c>
       <c r="C308" s="30" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D308" s="28"/>
       <c r="E308" s="28" t="s">
@@ -13068,7 +12908,7 @@
         <v>425</v>
       </c>
       <c r="C311" s="30" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D311" s="28"/>
       <c r="E311" s="28" t="s">
@@ -13143,7 +12983,7 @@
         <v>426</v>
       </c>
       <c r="C314" s="30" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D314" s="28"/>
       <c r="E314" s="28" t="s">
@@ -13218,7 +13058,7 @@
         <v>427</v>
       </c>
       <c r="C317" s="30" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D317" s="28"/>
       <c r="E317" s="28" t="s">
@@ -13318,7 +13158,7 @@
         <v>427</v>
       </c>
       <c r="C321" s="30" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D321" s="28"/>
       <c r="E321" s="28" t="s">
@@ -13340,7 +13180,7 @@
         <v>168</v>
       </c>
       <c r="B322" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C322" s="30" t="s">
         <v>547</v>
@@ -13365,10 +13205,10 @@
         <v>169</v>
       </c>
       <c r="B323" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C323" s="30" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="D323" s="28"/>
       <c r="E323" s="28" t="s">
@@ -13390,7 +13230,7 @@
         <v>170</v>
       </c>
       <c r="B324" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C324" s="30" t="s">
         <v>548</v>
@@ -13415,7 +13255,7 @@
         <v>171</v>
       </c>
       <c r="B325" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C325" s="30" t="s">
         <v>549</v>
@@ -13440,7 +13280,7 @@
         <v>172</v>
       </c>
       <c r="B326" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C326" s="30" t="s">
         <v>550</v>
@@ -13465,7 +13305,7 @@
         <v>173</v>
       </c>
       <c r="B327" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C327" s="30" t="s">
         <v>551</v>
@@ -13490,7 +13330,7 @@
         <v>174</v>
       </c>
       <c r="B328" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C328" s="30" t="s">
         <v>552</v>
@@ -13517,7 +13357,7 @@
         <v>175</v>
       </c>
       <c r="B329" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C329" s="30" t="s">
         <v>553</v>
@@ -13544,7 +13384,7 @@
         <v>176</v>
       </c>
       <c r="B330" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C330" s="30" t="s">
         <v>554</v>
@@ -13569,7 +13409,7 @@
         <v>177</v>
       </c>
       <c r="B331" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C331" s="30" t="s">
         <v>555</v>
@@ -13594,7 +13434,7 @@
         <v>178</v>
       </c>
       <c r="B332" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C332" s="30" t="s">
         <v>556</v>
@@ -13621,7 +13461,7 @@
         <v>179</v>
       </c>
       <c r="B333" s="29" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C333" s="30" t="s">
         <v>557</v>
@@ -13651,7 +13491,7 @@
         <v>428</v>
       </c>
       <c r="C334" s="30" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D334" s="28"/>
       <c r="E334" s="28" t="s">
@@ -13976,7 +13816,7 @@
         <v>430</v>
       </c>
       <c r="C347" s="30" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D347" s="28"/>
       <c r="E347" s="28" t="s">
@@ -14026,7 +13866,7 @@
         <v>430</v>
       </c>
       <c r="C349" s="30" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D349" s="28"/>
       <c r="E349" s="28" t="s">
@@ -14101,7 +13941,7 @@
         <v>430</v>
       </c>
       <c r="C352" s="30" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D352" s="28"/>
       <c r="E352" s="28" t="s">
@@ -14326,7 +14166,7 @@
         <v>431</v>
       </c>
       <c r="C361" s="30" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D361" s="28"/>
       <c r="E361" s="28" t="s">
@@ -14376,7 +14216,7 @@
         <v>431</v>
       </c>
       <c r="C363" s="30" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D363" s="28"/>
       <c r="E363" s="28" t="s">
@@ -14420,13 +14260,13 @@
     </row>
     <row r="365" spans="1:9" ht="45">
       <c r="A365" s="28" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B365" s="29" t="s">
         <v>431</v>
       </c>
       <c r="C365" s="30" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D365" s="28"/>
       <c r="E365" s="28" t="s">
@@ -14445,13 +14285,13 @@
     </row>
     <row r="366" spans="1:9" ht="60">
       <c r="A366" s="28" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B366" s="29" t="s">
         <v>431</v>
       </c>
       <c r="C366" s="30" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D366" s="28"/>
       <c r="E366" s="28" t="s">
@@ -14726,7 +14566,7 @@
         <v>436</v>
       </c>
       <c r="C377" s="30" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D377" s="28"/>
       <c r="E377" s="28" t="s">
@@ -14776,7 +14616,7 @@
         <v>437</v>
       </c>
       <c r="C379" s="30" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D379" s="28"/>
       <c r="E379" s="28" t="s">
@@ -14951,7 +14791,7 @@
         <v>438</v>
       </c>
       <c r="C386" s="30" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D386" s="28"/>
       <c r="E386" s="28" t="s">
@@ -15017,7 +14857,7 @@
         <v>17</v>
       </c>
       <c r="I388" s="30" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
     </row>
     <row r="389" spans="1:9" ht="90">
@@ -15028,7 +14868,7 @@
         <v>438</v>
       </c>
       <c r="C389" s="30" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="D389" s="28"/>
       <c r="E389" s="28" t="s">
@@ -15044,7 +14884,7 @@
         <v>17</v>
       </c>
       <c r="I389" s="30" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="390" spans="1:9" ht="30">
@@ -15082,7 +14922,7 @@
         <v>438</v>
       </c>
       <c r="C391" s="30" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D391" s="28"/>
       <c r="E391" s="28" t="s">
@@ -15148,7 +14988,7 @@
         <v>17</v>
       </c>
       <c r="I393" s="30" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="394" spans="1:9" ht="60">
@@ -15175,18 +15015,18 @@
         <v>17</v>
       </c>
       <c r="I394" s="30" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
     </row>
     <row r="395" spans="1:9" ht="45">
       <c r="A395" s="28" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B395" s="29" t="s">
         <v>438</v>
       </c>
       <c r="C395" s="30" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="D395" s="28"/>
       <c r="E395" s="28" t="s">
@@ -15205,16 +15045,16 @@
     </row>
     <row r="396" spans="1:9" ht="45">
       <c r="A396" s="28" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B396" s="29" t="s">
         <v>438</v>
       </c>
       <c r="C396" s="30" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D396" s="28" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E396" s="28" t="s">
         <v>19</v>
@@ -15238,7 +15078,7 @@
         <v>438</v>
       </c>
       <c r="C397" s="30" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D397" s="28"/>
       <c r="E397" s="28" t="s">
@@ -15370,7 +15210,7 @@
         <v>778</v>
       </c>
       <c r="D402" s="28" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="E402" s="28" t="s">
         <v>22</v>
@@ -15390,16 +15230,16 @@
     </row>
     <row r="403" spans="1:9" ht="30">
       <c r="A403" s="28" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B403" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C403" s="19" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="D403" s="28" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E403" s="28" t="s">
         <v>22</v>
@@ -15417,16 +15257,16 @@
     </row>
     <row r="404" spans="1:9" ht="45">
       <c r="A404" s="28" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B404" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C404" s="19" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D404" s="28" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E404" s="28" t="s">
         <v>22</v>
@@ -15446,16 +15286,16 @@
     </row>
     <row r="405" spans="1:9" ht="30">
       <c r="A405" s="28" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B405" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C405" s="19" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D405" s="21" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E405" s="28" t="s">
         <v>22</v>
@@ -15473,16 +15313,16 @@
     </row>
     <row r="406" spans="1:9" ht="45">
       <c r="A406" s="28" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B406" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C406" s="19" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D406" s="28" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E406" s="28" t="s">
         <v>22</v>
@@ -15502,16 +15342,16 @@
     </row>
     <row r="407" spans="1:9" ht="45">
       <c r="A407" s="28" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B407" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C407" s="30" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D407" s="28" t="s">
-        <v>933</v>
+        <v>951</v>
       </c>
       <c r="E407" s="28" t="s">
         <v>22</v>
@@ -15523,24 +15363,24 @@
         <v>15</v>
       </c>
       <c r="H407" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I407" s="30" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="408" spans="1:9" ht="45">
+    <row r="408" spans="1:9" ht="30">
       <c r="A408" s="28" t="s">
-        <v>909</v>
+        <v>948</v>
       </c>
       <c r="B408" s="29" t="s">
         <v>439</v>
       </c>
-      <c r="C408" s="19" t="s">
-        <v>897</v>
-      </c>
-      <c r="D408" s="21" t="s">
-        <v>934</v>
+      <c r="C408" s="30" t="s">
+        <v>949</v>
+      </c>
+      <c r="D408" s="28" t="s">
+        <v>951</v>
       </c>
       <c r="E408" s="28" t="s">
         <v>22</v>
@@ -15551,23 +15391,23 @@
       <c r="G408" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H408" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I408" s="19"/>
+      <c r="H408" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I408" s="30"/>
     </row>
     <row r="409" spans="1:9" ht="45">
       <c r="A409" s="28" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="B409" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C409" s="19" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="D409" s="21" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="E409" s="28" t="s">
         <v>22</v>
@@ -15575,28 +15415,26 @@
       <c r="F409" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G409" s="21" t="s">
+      <c r="G409" s="28" t="s">
         <v>15</v>
       </c>
       <c r="H409" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="I409" s="30" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="410" spans="1:9" ht="60">
+        <v>18</v>
+      </c>
+      <c r="I409" s="19"/>
+    </row>
+    <row r="410" spans="1:9" ht="45">
       <c r="A410" s="28" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="B410" s="29" t="s">
         <v>439</v>
       </c>
-      <c r="C410" s="30" t="s">
-        <v>942</v>
-      </c>
-      <c r="D410" s="28" t="s">
-        <v>935</v>
+      <c r="C410" s="19" t="s">
+        <v>896</v>
+      </c>
+      <c r="D410" s="21" t="s">
+        <v>931</v>
       </c>
       <c r="E410" s="28" t="s">
         <v>22</v>
@@ -15604,26 +15442,28 @@
       <c r="F410" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G410" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="H410" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I410" s="30"/>
-    </row>
-    <row r="411" spans="1:9" ht="45">
+      <c r="G410" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H410" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I410" s="30" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9" ht="60">
       <c r="A411" s="28" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="B411" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C411" s="30" t="s">
-        <v>943</v>
+        <v>938</v>
       </c>
       <c r="D411" s="28" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="E411" s="28" t="s">
         <v>22</v>
@@ -15635,51 +15475,51 @@
         <v>15</v>
       </c>
       <c r="H411" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="I411" s="30" t="s">
-        <v>745</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I411" s="30"/>
     </row>
     <row r="412" spans="1:9" ht="45">
       <c r="A412" s="28" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="B412" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C412" s="30" t="s">
-        <v>900</v>
+        <v>939</v>
       </c>
       <c r="D412" s="28" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="E412" s="28" t="s">
         <v>22</v>
       </c>
       <c r="F412" s="28" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G412" s="28" t="s">
         <v>15</v>
       </c>
       <c r="H412" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I412" s="30"/>
+        <v>21</v>
+      </c>
+      <c r="I412" s="30" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="413" spans="1:9" ht="45">
       <c r="A413" s="28" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="B413" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C413" s="30" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D413" s="28" t="s">
-        <v>936</v>
+        <v>945</v>
       </c>
       <c r="E413" s="28" t="s">
         <v>22</v>
@@ -15691,24 +15531,22 @@
         <v>15</v>
       </c>
       <c r="H413" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="I413" s="30" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="414" spans="1:9" ht="75">
+        <v>18</v>
+      </c>
+      <c r="I413" s="30"/>
+    </row>
+    <row r="414" spans="1:9" ht="45">
       <c r="A414" s="28" t="s">
-        <v>369</v>
+        <v>912</v>
       </c>
       <c r="B414" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C414" s="30" t="s">
-        <v>923</v>
+        <v>897</v>
       </c>
       <c r="D414" s="28" t="s">
-        <v>937</v>
+        <v>945</v>
       </c>
       <c r="E414" s="28" t="s">
         <v>22</v>
@@ -15720,7 +15558,7 @@
         <v>15</v>
       </c>
       <c r="H414" s="28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I414" s="30" t="s">
         <v>745</v>
@@ -15728,16 +15566,16 @@
     </row>
     <row r="415" spans="1:9" ht="75">
       <c r="A415" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B415" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C415" s="30" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="D415" s="28" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="E415" s="28" t="s">
         <v>22</v>
@@ -15757,16 +15595,16 @@
     </row>
     <row r="416" spans="1:9" ht="75">
       <c r="A416" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B416" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C416" s="30" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="D416" s="28" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="E416" s="28" t="s">
         <v>22</v>
@@ -15784,18 +15622,18 @@
         <v>745</v>
       </c>
     </row>
-    <row r="417" spans="1:9" ht="105">
+    <row r="417" spans="1:9" ht="75">
       <c r="A417" s="28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B417" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C417" s="30" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="D417" s="28" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="E417" s="28" t="s">
         <v>22</v>
@@ -15813,18 +15651,18 @@
         <v>745</v>
       </c>
     </row>
-    <row r="418" spans="1:9" ht="30">
+    <row r="418" spans="1:9" ht="105">
       <c r="A418" s="28" t="s">
-        <v>921</v>
+        <v>372</v>
       </c>
       <c r="B418" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C418" s="30" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
       <c r="D418" s="28" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="E418" s="28" t="s">
         <v>22</v>
@@ -15836,44 +15674,48 @@
         <v>15</v>
       </c>
       <c r="H418" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I418" s="30"/>
-    </row>
-    <row r="419" spans="1:9" ht="45">
+        <v>20</v>
+      </c>
+      <c r="I418" s="30" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9" ht="30">
       <c r="A419" s="28" t="s">
+        <v>919</v>
+      </c>
+      <c r="B419" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="C419" s="30" t="s">
+        <v>924</v>
+      </c>
+      <c r="D419" s="28" t="s">
+        <v>933</v>
+      </c>
+      <c r="E419" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F419" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G419" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H419" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I419" s="30"/>
+    </row>
+    <row r="420" spans="1:9" ht="45">
+      <c r="A420" s="28" t="s">
         <v>382</v>
       </c>
-      <c r="B419" s="29" t="s">
+      <c r="B420" s="29" t="s">
         <v>440</v>
       </c>
-      <c r="C419" s="30" t="s">
+      <c r="C420" s="30" t="s">
         <v>721</v>
-      </c>
-      <c r="D419" s="28"/>
-      <c r="E419" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F419" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="G419" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="H419" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="I419" s="30"/>
-    </row>
-    <row r="420" spans="1:9" ht="30">
-      <c r="A420" s="28" t="s">
-        <v>383</v>
-      </c>
-      <c r="B420" s="29" t="s">
-        <v>441</v>
-      </c>
-      <c r="C420" s="30" t="s">
-        <v>722</v>
       </c>
       <c r="D420" s="28"/>
       <c r="E420" s="28" t="s">
@@ -15890,15 +15732,15 @@
       </c>
       <c r="I420" s="30"/>
     </row>
-    <row r="421" spans="1:9" ht="360">
+    <row r="421" spans="1:9" ht="30">
       <c r="A421" s="28" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B421" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C421" s="30" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D421" s="28"/>
       <c r="E421" s="28" t="s">
@@ -15911,322 +15753,347 @@
         <v>15</v>
       </c>
       <c r="H421" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I421" s="30"/>
+    </row>
+    <row r="422" spans="1:9" ht="360">
+      <c r="A422" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="B422" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="C422" s="30" t="s">
+        <v>723</v>
+      </c>
+      <c r="D422" s="28"/>
+      <c r="E422" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F422" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G422" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H422" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I421" s="30"/>
-    </row>
-    <row r="422" spans="1:9">
-      <c r="A422" s="3"/>
-      <c r="B422" s="10"/>
+      <c r="I422" s="30"/>
     </row>
     <row r="423" spans="1:9">
       <c r="A423" s="3"/>
       <c r="B423" s="10"/>
     </row>
+    <row r="424" spans="1:9">
+      <c r="A424" s="3"/>
+      <c r="B424" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A396:I421 A20:I233">
-    <cfRule type="expression" dxfId="85" priority="133">
+  <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A126:I233 A125:H125 A20:I124 A396:I422">
+    <cfRule type="expression" dxfId="93" priority="133">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="134">
+    <cfRule type="expression" dxfId="92" priority="134">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="141">
+    <cfRule type="expression" dxfId="91" priority="141">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A396:I421 A20:I233">
-    <cfRule type="expression" dxfId="82" priority="87">
+  <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A126:I233 A125:H125 A20:I124 A396:I422">
+    <cfRule type="expression" dxfId="90" priority="87">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="88">
+    <cfRule type="expression" dxfId="89" priority="88">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="89">
+    <cfRule type="expression" dxfId="88" priority="89">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F233 F238:F290 F293:F362 F365:F421">
-    <cfRule type="expression" dxfId="79" priority="93">
+  <conditionalFormatting sqref="F20:F233 F238:F290 F293:F362 F365:F422">
+    <cfRule type="expression" dxfId="87" priority="93">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="94">
+    <cfRule type="expression" dxfId="86" priority="94">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A363:A364 C363:I364">
-    <cfRule type="expression" dxfId="77" priority="78">
+    <cfRule type="expression" dxfId="85" priority="78">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="79">
+    <cfRule type="expression" dxfId="84" priority="79">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="80">
+    <cfRule type="expression" dxfId="83" priority="80">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A363:A364 C363:I364">
-    <cfRule type="expression" dxfId="74" priority="73">
+    <cfRule type="expression" dxfId="82" priority="73">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="74">
+    <cfRule type="expression" dxfId="81" priority="74">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="75">
+    <cfRule type="expression" dxfId="80" priority="75">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F363:F364">
-    <cfRule type="expression" dxfId="71" priority="76">
+    <cfRule type="expression" dxfId="79" priority="76">
       <formula>NOT(VLOOKUP(F363,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="77">
+    <cfRule type="expression" dxfId="78" priority="77">
       <formula>(VLOOKUP(F363,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I363:I364">
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="77" priority="70">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="71">
+    <cfRule type="expression" dxfId="76" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="72">
+    <cfRule type="expression" dxfId="75" priority="72">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I363:I364">
-    <cfRule type="expression" dxfId="66" priority="67">
+    <cfRule type="expression" dxfId="74" priority="67">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="68">
+    <cfRule type="expression" dxfId="73" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="69">
+    <cfRule type="expression" dxfId="72" priority="69">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234:I237">
-    <cfRule type="expression" dxfId="63" priority="64">
+    <cfRule type="expression" dxfId="71" priority="64">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="65">
+    <cfRule type="expression" dxfId="70" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="66">
+    <cfRule type="expression" dxfId="69" priority="66">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A234:I237">
-    <cfRule type="expression" dxfId="60" priority="59">
+    <cfRule type="expression" dxfId="68" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="60">
+    <cfRule type="expression" dxfId="67" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="61">
+    <cfRule type="expression" dxfId="66" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F234:F237">
-    <cfRule type="expression" dxfId="57" priority="62">
+    <cfRule type="expression" dxfId="65" priority="62">
       <formula>NOT(VLOOKUP(F234,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="63">
+    <cfRule type="expression" dxfId="64" priority="63">
       <formula>(VLOOKUP(F234,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I234:I237">
-    <cfRule type="expression" dxfId="55" priority="56">
+    <cfRule type="expression" dxfId="63" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="57">
+    <cfRule type="expression" dxfId="62" priority="57">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="58">
+    <cfRule type="expression" dxfId="61" priority="58">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I234:I237">
-    <cfRule type="expression" dxfId="52" priority="53">
+    <cfRule type="expression" dxfId="60" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="54">
+    <cfRule type="expression" dxfId="59" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="55">
+    <cfRule type="expression" dxfId="58" priority="55">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A291:A292 C291:I292">
-    <cfRule type="expression" dxfId="49" priority="50">
+    <cfRule type="expression" dxfId="57" priority="50">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="51">
+    <cfRule type="expression" dxfId="56" priority="51">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="52">
+    <cfRule type="expression" dxfId="55" priority="52">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A291:A292 C291:I292">
-    <cfRule type="expression" dxfId="46" priority="45">
+    <cfRule type="expression" dxfId="54" priority="45">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="53" priority="46">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="47">
+    <cfRule type="expression" dxfId="52" priority="47">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F291:F292">
-    <cfRule type="expression" dxfId="43" priority="48">
+    <cfRule type="expression" dxfId="51" priority="48">
       <formula>NOT(VLOOKUP(F291,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="49">
+    <cfRule type="expression" dxfId="50" priority="49">
       <formula>(VLOOKUP(F291,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I291:I292">
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="49" priority="42">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="43">
+    <cfRule type="expression" dxfId="48" priority="43">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="44">
+    <cfRule type="expression" dxfId="47" priority="44">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I291:I292">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="46" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="40">
+    <cfRule type="expression" dxfId="45" priority="40">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="41">
+    <cfRule type="expression" dxfId="44" priority="41">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B292">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="43" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="42" priority="37">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="38">
+    <cfRule type="expression" dxfId="41" priority="38">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B292">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="40" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="34">
+    <cfRule type="expression" dxfId="39" priority="34">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="35">
+    <cfRule type="expression" dxfId="38" priority="35">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B291">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="37" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="31">
+    <cfRule type="expression" dxfId="36" priority="31">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="35" priority="32">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B291">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="34" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="28">
+    <cfRule type="expression" dxfId="33" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="32" priority="29">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B363">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="31" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="25">
+    <cfRule type="expression" dxfId="30" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="29" priority="26">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B363">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="28" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="27" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="23">
+    <cfRule type="expression" dxfId="26" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B364">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="25" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="19">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="20">
+    <cfRule type="expression" dxfId="23" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B364">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="22" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="21" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="17">
+    <cfRule type="expression" dxfId="20" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F421">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F422">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E421">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E422">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G421">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G422">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H421">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H422">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16236,7 +16103,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 C3 B10:B17 B19:B29 B31:B39 B41 B419:B423 B43:B53 B55:B64 B67:B72 B74:B119 B152:B156 B122:B143 B238:B290 B307:B321 B295:B304 B334:B362 B182:B209 B211:B233 B397:B401 B367:B394" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 C3 B10:B17 B19:B29 B31:B39 B41 B420:B424 B43:B53 B55:B64 B67:B72 B74:B119 B152:B156 B122:B143 B238:B290 B307:B321 B295:B304 B334:B362 B182:B209 B211:B233 B397:B401 B367:B394" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -16246,9 +16113,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16301,24 +16171,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16339,9 +16200,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXWSATT] fix watchman error
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source Depot2\Interop-TestSuites-1\ExchangeWebServices\Docs\MS-OXWSATT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="950">
   <si>
     <t>Req ID</t>
   </si>
@@ -3495,9 +3490,6 @@
     <t>Verified by derived requirement: MS-OXWSATT_R318009.</t>
   </si>
   <si>
-    <t>Verified by derived requirements:MS-OXWSATT_R311, MS-OXWSATT_R3111.</t>
-  </si>
-  <si>
     <t>Verified by derived requirements: MS-OXWSATT_R55001, MS-OXWSATT_R55002, MS-OXWSATT_R55003, MS-OXWSATT_R552.</t>
   </si>
   <si>
@@ -3508,9 +3500,6 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does introduce the ReferenceAttachmentType complex type. (This type was introduced in Microsoft Exchange Server 2013 Service Pack 1 (SP1).)</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXWSATT_R479001, MS-OXWSATT_R479002.</t>
   </si>
   <si>
     <t>Verified by derived requirement: MS-OXWSATT_R318013.</t>
@@ -3556,25 +3545,25 @@
     <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Exchange2007 follow this behavior.)</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXWSATT_R318014, Ms-OXWSATT_R318015.</t>
-  </si>
-  <si>
     <t>MS-OXWSATT_R527:i</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSATT_R318014.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3779,7 +3768,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3817,7 +3806,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3858,8 +3847,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3871,27 +3860,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3917,9 +3885,30 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="93">
     <dxf>
@@ -4823,7 +4812,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4898,6 +4887,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4933,6 +4939,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5114,22 +5137,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>746</v>
       </c>
@@ -5141,7 +5164,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
         <v>747</v>
       </c>
@@ -5155,7 +5178,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="36"/>
       <c r="B3" s="37" t="s">
         <v>25</v>
@@ -5176,141 +5199,141 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+    <row r="4" spans="1:11" ht="21">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="78.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="33.75" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="56" t="s">
         <v>749</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>748</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="25" t="s">
         <v>8</v>
       </c>
@@ -5329,7 +5352,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="26" t="s">
         <v>6</v>
       </c>
@@ -5348,7 +5371,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="26" t="s">
         <v>7</v>
       </c>
@@ -5367,7 +5390,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="27" t="s">
         <v>3</v>
       </c>
@@ -5386,59 +5409,59 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="30" customHeight="1">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="64.5" customHeight="1">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="30" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>750</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="30">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -5467,7 +5490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" s="22" customFormat="1" ht="60">
       <c r="A20" s="21" t="s">
         <v>41</v>
       </c>
@@ -5493,7 +5516,7 @@
       <c r="I20" s="23"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" s="22" customFormat="1" ht="45">
       <c r="A21" s="21" t="s">
         <v>42</v>
       </c>
@@ -5519,7 +5542,7 @@
       <c r="I21" s="23"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" s="22" customFormat="1" ht="30">
       <c r="A22" s="21" t="s">
         <v>43</v>
       </c>
@@ -5545,7 +5568,7 @@
       <c r="I22" s="23"/>
       <c r="J22" s="35"/>
     </row>
-    <row r="23" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" s="22" customFormat="1">
       <c r="A23" s="21" t="s">
         <v>44</v>
       </c>
@@ -5571,7 +5594,7 @@
       <c r="I23" s="23"/>
       <c r="J23" s="35"/>
     </row>
-    <row r="24" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" s="22" customFormat="1" ht="30">
       <c r="A24" s="21" t="s">
         <v>45</v>
       </c>
@@ -5597,7 +5620,7 @@
       <c r="I24" s="23"/>
       <c r="J24" s="35"/>
     </row>
-    <row r="25" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" s="22" customFormat="1" ht="30">
       <c r="A25" s="21" t="s">
         <v>46</v>
       </c>
@@ -5623,7 +5646,7 @@
       <c r="I25" s="23"/>
       <c r="J25" s="35"/>
     </row>
-    <row r="26" spans="1:13" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" s="22" customFormat="1" ht="45">
       <c r="A26" s="21" t="s">
         <v>47</v>
       </c>
@@ -5649,7 +5672,7 @@
       <c r="I26" s="23"/>
       <c r="J26" s="35"/>
     </row>
-    <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" s="22" customFormat="1">
       <c r="A27" s="21" t="s">
         <v>48</v>
       </c>
@@ -5675,7 +5698,7 @@
       <c r="I27" s="23"/>
       <c r="J27" s="35"/>
     </row>
-    <row r="28" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" s="22" customFormat="1">
       <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
@@ -5701,7 +5724,7 @@
       <c r="I28" s="23"/>
       <c r="J28" s="35"/>
     </row>
-    <row r="29" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" s="22" customFormat="1" ht="30">
       <c r="A29" s="21" t="s">
         <v>50</v>
       </c>
@@ -5727,7 +5750,7 @@
       <c r="I29" s="23"/>
       <c r="J29" s="35"/>
     </row>
-    <row r="30" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" s="22" customFormat="1">
       <c r="A30" s="21" t="s">
         <v>754</v>
       </c>
@@ -5753,7 +5776,7 @@
       <c r="I30" s="30"/>
       <c r="J30" s="35"/>
     </row>
-    <row r="31" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" s="22" customFormat="1" ht="45">
       <c r="A31" s="21" t="s">
         <v>51</v>
       </c>
@@ -5781,7 +5804,7 @@
       </c>
       <c r="J31" s="35"/>
     </row>
-    <row r="32" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" s="22" customFormat="1" ht="30">
       <c r="A32" s="21" t="s">
         <v>52</v>
       </c>
@@ -5807,7 +5830,7 @@
       <c r="I32" s="23"/>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:10" s="22" customFormat="1" ht="45">
       <c r="A33" s="21" t="s">
         <v>53</v>
       </c>
@@ -5833,7 +5856,7 @@
       <c r="I33" s="23"/>
       <c r="J33" s="35"/>
     </row>
-    <row r="34" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" s="22" customFormat="1" ht="45">
       <c r="A34" s="21" t="s">
         <v>54</v>
       </c>
@@ -5859,7 +5882,7 @@
       <c r="I34" s="23"/>
       <c r="J34" s="35"/>
     </row>
-    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="60">
       <c r="A35" s="28" t="s">
         <v>55</v>
       </c>
@@ -5884,7 +5907,7 @@
       </c>
       <c r="I35" s="30"/>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="30">
       <c r="A36" s="28" t="s">
         <v>56</v>
       </c>
@@ -5909,7 +5932,7 @@
       </c>
       <c r="I36" s="30"/>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="30">
       <c r="A37" s="28" t="s">
         <v>57</v>
       </c>
@@ -5934,7 +5957,7 @@
       </c>
       <c r="I37" s="30"/>
     </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="30">
       <c r="A38" s="28" t="s">
         <v>58</v>
       </c>
@@ -5959,7 +5982,7 @@
       </c>
       <c r="I38" s="30"/>
     </row>
-    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="30">
       <c r="A39" s="28" t="s">
         <v>59</v>
       </c>
@@ -5984,7 +6007,7 @@
       </c>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="30">
       <c r="A40" s="28" t="s">
         <v>756</v>
       </c>
@@ -6009,7 +6032,7 @@
       </c>
       <c r="I40" s="30"/>
     </row>
-    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="30">
       <c r="A41" s="28" t="s">
         <v>60</v>
       </c>
@@ -6034,7 +6057,7 @@
       </c>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="30">
       <c r="A42" s="28" t="s">
         <v>759</v>
       </c>
@@ -6059,7 +6082,7 @@
       </c>
       <c r="I42" s="30"/>
     </row>
-    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="30">
       <c r="A43" s="28" t="s">
         <v>61</v>
       </c>
@@ -6084,7 +6107,7 @@
       </c>
       <c r="I43" s="30"/>
     </row>
-    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="30">
       <c r="A44" s="28" t="s">
         <v>62</v>
       </c>
@@ -6109,7 +6132,7 @@
       </c>
       <c r="I44" s="30"/>
     </row>
-    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="45">
       <c r="A45" s="28" t="s">
         <v>63</v>
       </c>
@@ -6134,7 +6157,7 @@
       </c>
       <c r="I45" s="30"/>
     </row>
-    <row r="46" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="75">
       <c r="A46" s="28" t="s">
         <v>64</v>
       </c>
@@ -6159,7 +6182,7 @@
       </c>
       <c r="I46" s="30"/>
     </row>
-    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="30">
       <c r="A47" s="28" t="s">
         <v>65</v>
       </c>
@@ -6184,7 +6207,7 @@
       </c>
       <c r="I47" s="30"/>
     </row>
-    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="45">
       <c r="A48" s="28" t="s">
         <v>66</v>
       </c>
@@ -6209,7 +6232,7 @@
       </c>
       <c r="I48" s="30"/>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30">
       <c r="A49" s="28" t="s">
         <v>67</v>
       </c>
@@ -6234,7 +6257,7 @@
       </c>
       <c r="I49" s="30"/>
     </row>
-    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="30">
       <c r="A50" s="28" t="s">
         <v>68</v>
       </c>
@@ -6259,7 +6282,7 @@
       </c>
       <c r="I50" s="30"/>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30">
       <c r="A51" s="28" t="s">
         <v>69</v>
       </c>
@@ -6284,7 +6307,7 @@
       </c>
       <c r="I51" s="30"/>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30">
       <c r="A52" s="28" t="s">
         <v>70</v>
       </c>
@@ -6309,7 +6332,7 @@
       </c>
       <c r="I52" s="30"/>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30">
       <c r="A53" s="28" t="s">
         <v>71</v>
       </c>
@@ -6334,7 +6357,7 @@
       </c>
       <c r="I53" s="30"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="28" t="s">
         <v>763</v>
       </c>
@@ -6359,7 +6382,7 @@
       </c>
       <c r="I54" s="30"/>
     </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30">
       <c r="A55" s="28" t="s">
         <v>72</v>
       </c>
@@ -6384,7 +6407,7 @@
       </c>
       <c r="I55" s="30"/>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="30">
       <c r="A56" s="28" t="s">
         <v>73</v>
       </c>
@@ -6409,7 +6432,7 @@
       </c>
       <c r="I56" s="30"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="45">
       <c r="A57" s="28" t="s">
         <v>74</v>
       </c>
@@ -6436,7 +6459,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30">
       <c r="A58" s="28" t="s">
         <v>75</v>
       </c>
@@ -6463,7 +6486,7 @@
       </c>
       <c r="I58" s="30"/>
     </row>
-    <row r="59" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="270">
       <c r="A59" s="28" t="s">
         <v>76</v>
       </c>
@@ -6488,7 +6511,7 @@
       </c>
       <c r="I59" s="30"/>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="45">
       <c r="A60" s="28" t="s">
         <v>77</v>
       </c>
@@ -6513,7 +6536,7 @@
       </c>
       <c r="I60" s="30"/>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30">
       <c r="A61" s="28" t="s">
         <v>78</v>
       </c>
@@ -6538,7 +6561,7 @@
       </c>
       <c r="I61" s="30"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30">
       <c r="A62" s="28" t="s">
         <v>79</v>
       </c>
@@ -6563,7 +6586,7 @@
       </c>
       <c r="I62" s="30"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30">
       <c r="A63" s="28" t="s">
         <v>80</v>
       </c>
@@ -6588,7 +6611,7 @@
       </c>
       <c r="I63" s="30"/>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="30">
       <c r="A64" s="28" t="s">
         <v>81</v>
       </c>
@@ -6613,7 +6636,7 @@
       </c>
       <c r="I64" s="30"/>
     </row>
-    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="28" t="s">
         <v>768</v>
       </c>
@@ -6638,7 +6661,7 @@
       </c>
       <c r="I65" s="30"/>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="28" t="s">
         <v>769</v>
       </c>
@@ -6663,7 +6686,7 @@
       </c>
       <c r="I66" s="30"/>
     </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="30">
       <c r="A67" s="28" t="s">
         <v>82</v>
       </c>
@@ -6688,7 +6711,7 @@
       </c>
       <c r="I67" s="30"/>
     </row>
-    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="28" t="s">
         <v>83</v>
       </c>
@@ -6713,7 +6736,7 @@
       </c>
       <c r="I68" s="30"/>
     </row>
-    <row r="69" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="255">
       <c r="A69" s="28" t="s">
         <v>84</v>
       </c>
@@ -6738,7 +6761,7 @@
       </c>
       <c r="I69" s="30"/>
     </row>
-    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="45">
       <c r="A70" s="28" t="s">
         <v>85</v>
       </c>
@@ -6763,7 +6786,7 @@
       </c>
       <c r="I70" s="30"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30">
       <c r="A71" s="28" t="s">
         <v>86</v>
       </c>
@@ -6788,7 +6811,7 @@
       </c>
       <c r="I71" s="30"/>
     </row>
-    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="28" t="s">
         <v>87</v>
       </c>
@@ -6813,7 +6836,7 @@
       </c>
       <c r="I72" s="30"/>
     </row>
-    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="30">
       <c r="A73" s="28" t="s">
         <v>928</v>
       </c>
@@ -6838,7 +6861,7 @@
       </c>
       <c r="I73" s="30"/>
     </row>
-    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="45">
       <c r="A74" s="28" t="s">
         <v>88</v>
       </c>
@@ -6865,7 +6888,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="30">
       <c r="A75" s="28" t="s">
         <v>89</v>
       </c>
@@ -6892,7 +6915,7 @@
       </c>
       <c r="I75" s="30"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30">
       <c r="A76" s="28" t="s">
         <v>90</v>
       </c>
@@ -6917,7 +6940,7 @@
       </c>
       <c r="I76" s="30"/>
     </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30">
       <c r="A77" s="28" t="s">
         <v>91</v>
       </c>
@@ -6942,7 +6965,7 @@
       </c>
       <c r="I77" s="30"/>
     </row>
-    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="45">
       <c r="A78" s="28" t="s">
         <v>92</v>
       </c>
@@ -6969,7 +6992,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30">
       <c r="A79" s="28" t="s">
         <v>93</v>
       </c>
@@ -6996,7 +7019,7 @@
       </c>
       <c r="I79" s="30"/>
     </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="45">
       <c r="A80" s="28" t="s">
         <v>94</v>
       </c>
@@ -7021,7 +7044,7 @@
       </c>
       <c r="I80" s="30"/>
     </row>
-    <row r="81" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="240">
       <c r="A81" s="28" t="s">
         <v>95</v>
       </c>
@@ -7046,7 +7069,7 @@
       </c>
       <c r="I81" s="30"/>
     </row>
-    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="45">
       <c r="A82" s="28" t="s">
         <v>96</v>
       </c>
@@ -7071,7 +7094,7 @@
       </c>
       <c r="I82" s="30"/>
     </row>
-    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30">
       <c r="A83" s="28" t="s">
         <v>97</v>
       </c>
@@ -7096,7 +7119,7 @@
       </c>
       <c r="I83" s="30"/>
     </row>
-    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30">
       <c r="A84" s="28" t="s">
         <v>98</v>
       </c>
@@ -7121,7 +7144,7 @@
       </c>
       <c r="I84" s="30"/>
     </row>
-    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="45">
       <c r="A85" s="28" t="s">
         <v>99</v>
       </c>
@@ -7148,7 +7171,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30">
       <c r="A86" s="28" t="s">
         <v>100</v>
       </c>
@@ -7175,7 +7198,7 @@
       </c>
       <c r="I86" s="30"/>
     </row>
-    <row r="87" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="409.5">
       <c r="A87" s="28" t="s">
         <v>101</v>
       </c>
@@ -7200,7 +7223,7 @@
       </c>
       <c r="I87" s="30"/>
     </row>
-    <row r="88" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="45">
       <c r="A88" s="28" t="s">
         <v>102</v>
       </c>
@@ -7225,7 +7248,7 @@
       </c>
       <c r="I88" s="30"/>
     </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="30">
       <c r="A89" s="28" t="s">
         <v>103</v>
       </c>
@@ -7250,7 +7273,7 @@
       </c>
       <c r="I89" s="30"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="30">
       <c r="A90" s="28" t="s">
         <v>104</v>
       </c>
@@ -7275,7 +7298,7 @@
       </c>
       <c r="I90" s="30"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30">
       <c r="A91" s="28" t="s">
         <v>105</v>
       </c>
@@ -7300,7 +7323,7 @@
       </c>
       <c r="I91" s="30"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="30">
       <c r="A92" s="28" t="s">
         <v>106</v>
       </c>
@@ -7325,7 +7348,7 @@
       </c>
       <c r="I92" s="30"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9">
       <c r="A93" s="28" t="s">
         <v>107</v>
       </c>
@@ -7350,7 +7373,7 @@
       </c>
       <c r="I93" s="30"/>
     </row>
-    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="30">
       <c r="A94" s="28" t="s">
         <v>108</v>
       </c>
@@ -7375,7 +7398,7 @@
       </c>
       <c r="I94" s="30"/>
     </row>
-    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="45">
       <c r="A95" s="28" t="s">
         <v>109</v>
       </c>
@@ -7400,7 +7423,7 @@
       </c>
       <c r="I95" s="30"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9">
       <c r="A96" s="28" t="s">
         <v>110</v>
       </c>
@@ -7425,7 +7448,7 @@
       </c>
       <c r="I96" s="30"/>
     </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="45">
       <c r="A97" s="28" t="s">
         <v>111</v>
       </c>
@@ -7452,7 +7475,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="30">
       <c r="A98" s="28" t="s">
         <v>112</v>
       </c>
@@ -7479,7 +7502,7 @@
       </c>
       <c r="I98" s="30"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9">
       <c r="A99" s="28" t="s">
         <v>113</v>
       </c>
@@ -7504,7 +7527,7 @@
       </c>
       <c r="I99" s="30"/>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="30">
       <c r="A100" s="28" t="s">
         <v>114</v>
       </c>
@@ -7529,7 +7552,7 @@
       </c>
       <c r="I100" s="30"/>
     </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="30">
       <c r="A101" s="28" t="s">
         <v>115</v>
       </c>
@@ -7554,7 +7577,7 @@
       </c>
       <c r="I101" s="30"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9">
       <c r="A102" s="28" t="s">
         <v>116</v>
       </c>
@@ -7579,7 +7602,7 @@
       </c>
       <c r="I102" s="30"/>
     </row>
-    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="30">
       <c r="A103" s="28" t="s">
         <v>117</v>
       </c>
@@ -7604,7 +7627,7 @@
       </c>
       <c r="I103" s="30"/>
     </row>
-    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="30">
       <c r="A104" s="28" t="s">
         <v>118</v>
       </c>
@@ -7629,7 +7652,7 @@
       </c>
       <c r="I104" s="30"/>
     </row>
-    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="30">
       <c r="A105" s="28" t="s">
         <v>119</v>
       </c>
@@ -7654,7 +7677,7 @@
       </c>
       <c r="I105" s="30"/>
     </row>
-    <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="45">
       <c r="A106" s="28" t="s">
         <v>120</v>
       </c>
@@ -7681,7 +7704,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="30">
       <c r="A107" s="28" t="s">
         <v>121</v>
       </c>
@@ -7706,7 +7729,7 @@
       </c>
       <c r="I107" s="30"/>
     </row>
-    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30">
       <c r="A108" s="28" t="s">
         <v>122</v>
       </c>
@@ -7731,7 +7754,7 @@
       </c>
       <c r="I108" s="30"/>
     </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="30">
       <c r="A109" s="28" t="s">
         <v>123</v>
       </c>
@@ -7756,7 +7779,7 @@
       </c>
       <c r="I109" s="30"/>
     </row>
-    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30">
       <c r="A110" s="28" t="s">
         <v>124</v>
       </c>
@@ -7781,7 +7804,7 @@
       </c>
       <c r="I110" s="30"/>
     </row>
-    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="30">
       <c r="A111" s="28" t="s">
         <v>125</v>
       </c>
@@ -7806,7 +7829,7 @@
       </c>
       <c r="I111" s="30"/>
     </row>
-    <row r="112" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="330">
       <c r="A112" s="28" t="s">
         <v>126</v>
       </c>
@@ -7831,7 +7854,7 @@
       </c>
       <c r="I112" s="30"/>
     </row>
-    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="30">
       <c r="A113" s="28" t="s">
         <v>127</v>
       </c>
@@ -7856,7 +7879,7 @@
       </c>
       <c r="I113" s="30"/>
     </row>
-    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="45">
       <c r="A114" s="28" t="s">
         <v>128</v>
       </c>
@@ -7883,7 +7906,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="30">
       <c r="A115" s="28" t="s">
         <v>129</v>
       </c>
@@ -7908,7 +7931,7 @@
       </c>
       <c r="I115" s="30"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="30">
       <c r="A116" s="28" t="s">
         <v>130</v>
       </c>
@@ -7933,7 +7956,7 @@
       </c>
       <c r="I116" s="30"/>
     </row>
-    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="30">
       <c r="A117" s="28" t="s">
         <v>131</v>
       </c>
@@ -7958,7 +7981,7 @@
       </c>
       <c r="I117" s="30"/>
     </row>
-    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="30">
       <c r="A118" s="28" t="s">
         <v>132</v>
       </c>
@@ -7983,7 +8006,7 @@
       </c>
       <c r="I118" s="30"/>
     </row>
-    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="30">
       <c r="A119" s="28" t="s">
         <v>133</v>
       </c>
@@ -8008,7 +8031,7 @@
       </c>
       <c r="I119" s="30"/>
     </row>
-    <row r="120" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="60">
       <c r="A120" s="28" t="s">
         <v>775</v>
       </c>
@@ -8035,7 +8058,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="45">
       <c r="A121" s="28" t="s">
         <v>776</v>
       </c>
@@ -8060,7 +8083,7 @@
       </c>
       <c r="I121" s="30"/>
     </row>
-    <row r="122" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="409.5">
       <c r="A122" s="28" t="s">
         <v>134</v>
       </c>
@@ -8085,7 +8108,7 @@
       </c>
       <c r="I122" s="30"/>
     </row>
-    <row r="123" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="60">
       <c r="A123" s="28" t="s">
         <v>135</v>
       </c>
@@ -8110,7 +8133,7 @@
       </c>
       <c r="I123" s="30"/>
     </row>
-    <row r="124" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="45">
       <c r="A124" s="28" t="s">
         <v>136</v>
       </c>
@@ -8118,7 +8141,7 @@
         <v>397</v>
       </c>
       <c r="C124" s="30" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D124" s="28"/>
       <c r="E124" s="28" t="s">
@@ -8133,11 +8156,11 @@
       <c r="H124" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I124" s="30" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I124" s="19" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="28" t="s">
         <v>137</v>
       </c>
@@ -8145,7 +8168,7 @@
         <v>397</v>
       </c>
       <c r="C125" s="30" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D125" s="28"/>
       <c r="E125" s="28" t="s">
@@ -8158,11 +8181,11 @@
         <v>15</v>
       </c>
       <c r="H125" s="28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I125" s="30"/>
     </row>
-    <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="30">
       <c r="A126" s="28" t="s">
         <v>138</v>
       </c>
@@ -8187,7 +8210,7 @@
       </c>
       <c r="I126" s="30"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="30">
       <c r="A127" s="28" t="s">
         <v>139</v>
       </c>
@@ -8212,7 +8235,7 @@
       </c>
       <c r="I127" s="30"/>
     </row>
-    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="30">
       <c r="A128" s="28" t="s">
         <v>140</v>
       </c>
@@ -8237,7 +8260,7 @@
       </c>
       <c r="I128" s="30"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="30">
       <c r="A129" s="28" t="s">
         <v>141</v>
       </c>
@@ -8262,7 +8285,7 @@
       </c>
       <c r="I129" s="30"/>
     </row>
-    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="30">
       <c r="A130" s="28" t="s">
         <v>142</v>
       </c>
@@ -8287,7 +8310,7 @@
       </c>
       <c r="I130" s="30"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9">
       <c r="A131" s="28" t="s">
         <v>143</v>
       </c>
@@ -8312,7 +8335,7 @@
       </c>
       <c r="I131" s="30"/>
     </row>
-    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="30">
       <c r="A132" s="28" t="s">
         <v>144</v>
       </c>
@@ -8337,7 +8360,7 @@
       </c>
       <c r="I132" s="30"/>
     </row>
-    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="30">
       <c r="A133" s="28" t="s">
         <v>145</v>
       </c>
@@ -8362,7 +8385,7 @@
       </c>
       <c r="I133" s="30"/>
     </row>
-    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="30">
       <c r="A134" s="28" t="s">
         <v>146</v>
       </c>
@@ -8387,7 +8410,7 @@
       </c>
       <c r="I134" s="30"/>
     </row>
-    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="30">
       <c r="A135" s="28" t="s">
         <v>147</v>
       </c>
@@ -8412,7 +8435,7 @@
       </c>
       <c r="I135" s="30"/>
     </row>
-    <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="30">
       <c r="A136" s="28" t="s">
         <v>148</v>
       </c>
@@ -8437,7 +8460,7 @@
       </c>
       <c r="I136" s="30"/>
     </row>
-    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="30">
       <c r="A137" s="28" t="s">
         <v>149</v>
       </c>
@@ -8462,7 +8485,7 @@
       </c>
       <c r="I137" s="30"/>
     </row>
-    <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="30">
       <c r="A138" s="28" t="s">
         <v>150</v>
       </c>
@@ -8487,7 +8510,7 @@
       </c>
       <c r="I138" s="30"/>
     </row>
-    <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="30">
       <c r="A139" s="28" t="s">
         <v>151</v>
       </c>
@@ -8512,7 +8535,7 @@
       </c>
       <c r="I139" s="30"/>
     </row>
-    <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="30">
       <c r="A140" s="28" t="s">
         <v>152</v>
       </c>
@@ -8537,7 +8560,7 @@
       </c>
       <c r="I140" s="30"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="30">
       <c r="A141" s="28" t="s">
         <v>153</v>
       </c>
@@ -8562,7 +8585,7 @@
       </c>
       <c r="I141" s="30"/>
     </row>
-    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="30">
       <c r="A142" s="28" t="s">
         <v>154</v>
       </c>
@@ -8587,7 +8610,7 @@
       </c>
       <c r="I142" s="30"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="30">
       <c r="A143" s="28" t="s">
         <v>155</v>
       </c>
@@ -8612,7 +8635,7 @@
       </c>
       <c r="I143" s="30"/>
     </row>
-    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="30">
       <c r="A144" s="28" t="s">
         <v>795</v>
       </c>
@@ -8637,7 +8660,7 @@
       </c>
       <c r="I144" s="30"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="30">
       <c r="A145" s="28" t="s">
         <v>796</v>
       </c>
@@ -8662,7 +8685,7 @@
       </c>
       <c r="I145" s="30"/>
     </row>
-    <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" ht="30">
       <c r="A146" s="28" t="s">
         <v>797</v>
       </c>
@@ -8687,7 +8710,7 @@
       </c>
       <c r="I146" s="30"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9">
       <c r="A147" s="28" t="s">
         <v>798</v>
       </c>
@@ -8712,7 +8735,7 @@
       </c>
       <c r="I147" s="30"/>
     </row>
-    <row r="148" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="30">
       <c r="A148" s="28" t="s">
         <v>799</v>
       </c>
@@ -8737,7 +8760,7 @@
       </c>
       <c r="I148" s="30"/>
     </row>
-    <row r="149" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="45">
       <c r="A149" s="28" t="s">
         <v>800</v>
       </c>
@@ -8764,7 +8787,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" ht="30">
       <c r="A150" s="28" t="s">
         <v>801</v>
       </c>
@@ -8789,7 +8812,7 @@
       </c>
       <c r="I150" s="30"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9">
       <c r="A151" s="28" t="s">
         <v>802</v>
       </c>
@@ -8814,7 +8837,7 @@
       </c>
       <c r="I151" s="30"/>
     </row>
-    <row r="152" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" ht="45">
       <c r="A152" s="28" t="s">
         <v>156</v>
       </c>
@@ -8839,7 +8862,7 @@
       </c>
       <c r="I152" s="30"/>
     </row>
-    <row r="153" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" ht="180">
       <c r="A153" s="28" t="s">
         <v>157</v>
       </c>
@@ -8864,7 +8887,7 @@
       </c>
       <c r="I153" s="30"/>
     </row>
-    <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="45">
       <c r="A154" s="28" t="s">
         <v>158</v>
       </c>
@@ -8889,7 +8912,7 @@
       </c>
       <c r="I154" s="30"/>
     </row>
-    <row r="155" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="30">
       <c r="A155" s="28" t="s">
         <v>159</v>
       </c>
@@ -8914,7 +8937,7 @@
       </c>
       <c r="I155" s="30"/>
     </row>
-    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="30">
       <c r="A156" s="28" t="s">
         <v>160</v>
       </c>
@@ -8939,7 +8962,7 @@
       </c>
       <c r="I156" s="30"/>
     </row>
-    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="30">
       <c r="A157" s="28" t="s">
         <v>822</v>
       </c>
@@ -8964,7 +8987,7 @@
       </c>
       <c r="I157" s="30"/>
     </row>
-    <row r="158" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="45">
       <c r="A158" s="28" t="s">
         <v>823</v>
       </c>
@@ -8972,7 +8995,7 @@
         <v>399</v>
       </c>
       <c r="C158" s="30" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D158" s="28"/>
       <c r="E158" s="28" t="s">
@@ -8991,15 +9014,15 @@
         <v>918</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="330">
       <c r="A159" s="28" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B159" s="29" t="s">
         <v>399</v>
       </c>
       <c r="C159" s="30" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="D159" s="28"/>
       <c r="E159" s="28" t="s">
@@ -9016,7 +9039,7 @@
       </c>
       <c r="I159" s="30"/>
     </row>
-    <row r="160" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" ht="30">
       <c r="A160" s="28" t="s">
         <v>824</v>
       </c>
@@ -9041,7 +9064,7 @@
       </c>
       <c r="I160" s="30"/>
     </row>
-    <row r="161" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="30">
       <c r="A161" s="28" t="s">
         <v>825</v>
       </c>
@@ -9066,7 +9089,7 @@
       </c>
       <c r="I161" s="30"/>
     </row>
-    <row r="162" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="30">
       <c r="A162" s="28" t="s">
         <v>826</v>
       </c>
@@ -9091,7 +9114,7 @@
       </c>
       <c r="I162" s="30"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="30">
       <c r="A163" s="28" t="s">
         <v>827</v>
       </c>
@@ -9116,7 +9139,7 @@
       </c>
       <c r="I163" s="30"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" ht="30">
       <c r="A164" s="28" t="s">
         <v>828</v>
       </c>
@@ -9141,7 +9164,7 @@
       </c>
       <c r="I164" s="30"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="30">
       <c r="A165" s="28" t="s">
         <v>829</v>
       </c>
@@ -9166,7 +9189,7 @@
       </c>
       <c r="I165" s="30"/>
     </row>
-    <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" ht="30">
       <c r="A166" s="28" t="s">
         <v>830</v>
       </c>
@@ -9191,7 +9214,7 @@
       </c>
       <c r="I166" s="30"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" ht="30">
       <c r="A167" s="28" t="s">
         <v>831</v>
       </c>
@@ -9216,7 +9239,7 @@
       </c>
       <c r="I167" s="30"/>
     </row>
-    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" ht="30">
       <c r="A168" s="28" t="s">
         <v>832</v>
       </c>
@@ -9241,7 +9264,7 @@
       </c>
       <c r="I168" s="30"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" ht="30">
       <c r="A169" s="28" t="s">
         <v>833</v>
       </c>
@@ -9266,7 +9289,7 @@
       </c>
       <c r="I169" s="30"/>
     </row>
-    <row r="170" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="30">
       <c r="A170" s="28" t="s">
         <v>834</v>
       </c>
@@ -9291,7 +9314,7 @@
       </c>
       <c r="I170" s="30"/>
     </row>
-    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" ht="30">
       <c r="A171" s="28" t="s">
         <v>835</v>
       </c>
@@ -9316,7 +9339,7 @@
       </c>
       <c r="I171" s="30"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" ht="30">
       <c r="A172" s="28" t="s">
         <v>836</v>
       </c>
@@ -9341,7 +9364,7 @@
       </c>
       <c r="I172" s="30"/>
     </row>
-    <row r="173" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="30">
       <c r="A173" s="28" t="s">
         <v>837</v>
       </c>
@@ -9366,7 +9389,7 @@
       </c>
       <c r="I173" s="30"/>
     </row>
-    <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" ht="30">
       <c r="A174" s="28" t="s">
         <v>838</v>
       </c>
@@ -9391,7 +9414,7 @@
       </c>
       <c r="I174" s="30"/>
     </row>
-    <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" ht="30">
       <c r="A175" s="28" t="s">
         <v>161</v>
       </c>
@@ -9416,7 +9439,7 @@
       </c>
       <c r="I175" s="30"/>
     </row>
-    <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" ht="30">
       <c r="A176" s="28" t="s">
         <v>162</v>
       </c>
@@ -9441,7 +9464,7 @@
       </c>
       <c r="I176" s="30"/>
     </row>
-    <row r="177" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" ht="210">
       <c r="A177" s="28" t="s">
         <v>163</v>
       </c>
@@ -9466,7 +9489,7 @@
       </c>
       <c r="I177" s="30"/>
     </row>
-    <row r="178" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" ht="45">
       <c r="A178" s="28" t="s">
         <v>164</v>
       </c>
@@ -9491,7 +9514,7 @@
       </c>
       <c r="I178" s="30"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" ht="30">
       <c r="A179" s="28" t="s">
         <v>165</v>
       </c>
@@ -9516,7 +9539,7 @@
       </c>
       <c r="I179" s="30"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="30">
       <c r="A180" s="28" t="s">
         <v>166</v>
       </c>
@@ -9541,7 +9564,7 @@
       </c>
       <c r="I180" s="30"/>
     </row>
-    <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" ht="30">
       <c r="A181" s="28" t="s">
         <v>167</v>
       </c>
@@ -9566,7 +9589,7 @@
       </c>
       <c r="I181" s="30"/>
     </row>
-    <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" ht="30">
       <c r="A182" s="28" t="s">
         <v>180</v>
       </c>
@@ -9591,7 +9614,7 @@
       </c>
       <c r="I182" s="30"/>
     </row>
-    <row r="183" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" ht="30">
       <c r="A183" s="28" t="s">
         <v>181</v>
       </c>
@@ -9616,7 +9639,7 @@
       </c>
       <c r="I183" s="30"/>
     </row>
-    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" ht="30">
       <c r="A184" s="28" t="s">
         <v>182</v>
       </c>
@@ -9641,7 +9664,7 @@
       </c>
       <c r="I184" s="30"/>
     </row>
-    <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" ht="30">
       <c r="A185" s="28" t="s">
         <v>183</v>
       </c>
@@ -9666,7 +9689,7 @@
       </c>
       <c r="I185" s="30"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9">
       <c r="A186" s="28" t="s">
         <v>184</v>
       </c>
@@ -9691,7 +9714,7 @@
       </c>
       <c r="I186" s="30"/>
     </row>
-    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" ht="30">
       <c r="A187" s="28" t="s">
         <v>185</v>
       </c>
@@ -9716,7 +9739,7 @@
       </c>
       <c r="I187" s="30"/>
     </row>
-    <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="30">
       <c r="A188" s="28" t="s">
         <v>186</v>
       </c>
@@ -9741,7 +9764,7 @@
       </c>
       <c r="I188" s="30"/>
     </row>
-    <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" ht="45">
       <c r="A189" s="28" t="s">
         <v>187</v>
       </c>
@@ -9766,7 +9789,7 @@
       </c>
       <c r="I189" s="30"/>
     </row>
-    <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" ht="45">
       <c r="A190" s="28" t="s">
         <v>188</v>
       </c>
@@ -9791,7 +9814,7 @@
       </c>
       <c r="I190" s="30"/>
     </row>
-    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" ht="45">
       <c r="A191" s="28" t="s">
         <v>189</v>
       </c>
@@ -9816,7 +9839,7 @@
       </c>
       <c r="I191" s="30"/>
     </row>
-    <row r="192" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" ht="45">
       <c r="A192" s="28" t="s">
         <v>190</v>
       </c>
@@ -9841,7 +9864,7 @@
       </c>
       <c r="I192" s="30"/>
     </row>
-    <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" ht="45">
       <c r="A193" s="28" t="s">
         <v>191</v>
       </c>
@@ -9866,7 +9889,7 @@
       </c>
       <c r="I193" s="30"/>
     </row>
-    <row r="194" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" ht="60">
       <c r="A194" s="28" t="s">
         <v>192</v>
       </c>
@@ -9891,7 +9914,7 @@
       </c>
       <c r="I194" s="30"/>
     </row>
-    <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="30">
       <c r="A195" s="28" t="s">
         <v>193</v>
       </c>
@@ -9916,7 +9939,7 @@
       </c>
       <c r="I195" s="30"/>
     </row>
-    <row r="196" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" ht="60">
       <c r="A196" s="28" t="s">
         <v>194</v>
       </c>
@@ -9941,7 +9964,7 @@
       </c>
       <c r="I196" s="30"/>
     </row>
-    <row r="197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" ht="30">
       <c r="A197" s="28" t="s">
         <v>195</v>
       </c>
@@ -9966,7 +9989,7 @@
       </c>
       <c r="I197" s="30"/>
     </row>
-    <row r="198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" ht="30">
       <c r="A198" s="28" t="s">
         <v>196</v>
       </c>
@@ -9991,7 +10014,7 @@
       </c>
       <c r="I198" s="30"/>
     </row>
-    <row r="199" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" ht="30">
       <c r="A199" s="28" t="s">
         <v>197</v>
       </c>
@@ -10016,7 +10039,7 @@
       </c>
       <c r="I199" s="30"/>
     </row>
-    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" ht="30">
       <c r="A200" s="28" t="s">
         <v>198</v>
       </c>
@@ -10041,7 +10064,7 @@
       </c>
       <c r="I200" s="30"/>
     </row>
-    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="30">
       <c r="A201" s="28" t="s">
         <v>199</v>
       </c>
@@ -10066,7 +10089,7 @@
       </c>
       <c r="I201" s="30"/>
     </row>
-    <row r="202" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" ht="90">
       <c r="A202" s="28" t="s">
         <v>200</v>
       </c>
@@ -10091,7 +10114,7 @@
       </c>
       <c r="I202" s="30"/>
     </row>
-    <row r="203" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" ht="345">
       <c r="A203" s="28" t="s">
         <v>201</v>
       </c>
@@ -10116,7 +10139,7 @@
       </c>
       <c r="I203" s="30"/>
     </row>
-    <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" ht="30">
       <c r="A204" s="28" t="s">
         <v>202</v>
       </c>
@@ -10141,7 +10164,7 @@
       </c>
       <c r="I204" s="30"/>
     </row>
-    <row r="205" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" ht="30">
       <c r="A205" s="28" t="s">
         <v>203</v>
       </c>
@@ -10166,7 +10189,7 @@
       </c>
       <c r="I205" s="30"/>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9">
       <c r="A206" s="28" t="s">
         <v>204</v>
       </c>
@@ -10191,7 +10214,7 @@
       </c>
       <c r="I206" s="30"/>
     </row>
-    <row r="207" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" ht="45">
       <c r="A207" s="28" t="s">
         <v>205</v>
       </c>
@@ -10218,7 +10241,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" ht="30">
       <c r="A208" s="28" t="s">
         <v>206</v>
       </c>
@@ -10245,7 +10268,7 @@
       </c>
       <c r="I208" s="30"/>
     </row>
-    <row r="209" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="30">
       <c r="A209" s="28" t="s">
         <v>207</v>
       </c>
@@ -10270,7 +10293,7 @@
       </c>
       <c r="I209" s="30"/>
     </row>
-    <row r="210" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="45">
       <c r="A210" s="28" t="s">
         <v>210</v>
       </c>
@@ -10295,7 +10318,7 @@
       </c>
       <c r="I210" s="30"/>
     </row>
-    <row r="211" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="30">
       <c r="A211" s="28" t="s">
         <v>211</v>
       </c>
@@ -10320,7 +10343,7 @@
       </c>
       <c r="I211" s="30"/>
     </row>
-    <row r="212" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" ht="30">
       <c r="A212" s="28" t="s">
         <v>212</v>
       </c>
@@ -10345,7 +10368,7 @@
       </c>
       <c r="I212" s="30"/>
     </row>
-    <row r="213" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" ht="135">
       <c r="A213" s="28" t="s">
         <v>213</v>
       </c>
@@ -10370,7 +10393,7 @@
       </c>
       <c r="I213" s="30"/>
     </row>
-    <row r="214" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" ht="45">
       <c r="A214" s="28" t="s">
         <v>214</v>
       </c>
@@ -10395,7 +10418,7 @@
       </c>
       <c r="I214" s="30"/>
     </row>
-    <row r="215" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" ht="45">
       <c r="A215" s="28" t="s">
         <v>215</v>
       </c>
@@ -10420,7 +10443,7 @@
       </c>
       <c r="I215" s="30"/>
     </row>
-    <row r="216" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="30">
       <c r="A216" s="28" t="s">
         <v>216</v>
       </c>
@@ -10445,7 +10468,7 @@
       </c>
       <c r="I216" s="30"/>
     </row>
-    <row r="217" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="30">
       <c r="A217" s="28" t="s">
         <v>217</v>
       </c>
@@ -10470,7 +10493,7 @@
       </c>
       <c r="I217" s="30"/>
     </row>
-    <row r="218" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" ht="30">
       <c r="A218" s="28" t="s">
         <v>218</v>
       </c>
@@ -10495,7 +10518,7 @@
       </c>
       <c r="I218" s="30"/>
     </row>
-    <row r="219" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="30">
       <c r="A219" s="28" t="s">
         <v>219</v>
       </c>
@@ -10520,7 +10543,7 @@
       </c>
       <c r="I219" s="30"/>
     </row>
-    <row r="220" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="30">
       <c r="A220" s="28" t="s">
         <v>220</v>
       </c>
@@ -10545,7 +10568,7 @@
       </c>
       <c r="I220" s="30"/>
     </row>
-    <row r="221" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" ht="30">
       <c r="A221" s="28" t="s">
         <v>221</v>
       </c>
@@ -10570,7 +10593,7 @@
       </c>
       <c r="I221" s="30"/>
     </row>
-    <row r="222" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="30">
       <c r="A222" s="28" t="s">
         <v>222</v>
       </c>
@@ -10595,7 +10618,7 @@
       </c>
       <c r="I222" s="30"/>
     </row>
-    <row r="223" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="30">
       <c r="A223" s="28" t="s">
         <v>223</v>
       </c>
@@ -10620,7 +10643,7 @@
       </c>
       <c r="I223" s="30"/>
     </row>
-    <row r="224" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" ht="30">
       <c r="A224" s="28" t="s">
         <v>224</v>
       </c>
@@ -10645,7 +10668,7 @@
       </c>
       <c r="I224" s="30"/>
     </row>
-    <row r="225" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="30">
       <c r="A225" s="28" t="s">
         <v>225</v>
       </c>
@@ -10670,7 +10693,7 @@
       </c>
       <c r="I225" s="30"/>
     </row>
-    <row r="226" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" ht="30">
       <c r="A226" s="28" t="s">
         <v>226</v>
       </c>
@@ -10695,7 +10718,7 @@
       </c>
       <c r="I226" s="30"/>
     </row>
-    <row r="227" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="120">
       <c r="A227" s="28" t="s">
         <v>227</v>
       </c>
@@ -10720,7 +10743,7 @@
       </c>
       <c r="I227" s="30"/>
     </row>
-    <row r="228" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="45">
       <c r="A228" s="28" t="s">
         <v>228</v>
       </c>
@@ -10745,7 +10768,7 @@
       </c>
       <c r="I228" s="30"/>
     </row>
-    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="45">
       <c r="A229" s="28" t="s">
         <v>229</v>
       </c>
@@ -10770,7 +10793,7 @@
       </c>
       <c r="I229" s="30"/>
     </row>
-    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="30">
       <c r="A230" s="28" t="s">
         <v>230</v>
       </c>
@@ -10795,7 +10818,7 @@
       </c>
       <c r="I230" s="30"/>
     </row>
-    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="30">
       <c r="A231" s="28" t="s">
         <v>231</v>
       </c>
@@ -10820,7 +10843,7 @@
       </c>
       <c r="I231" s="30"/>
     </row>
-    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="30">
       <c r="A232" s="28" t="s">
         <v>232</v>
       </c>
@@ -10845,7 +10868,7 @@
       </c>
       <c r="I232" s="30"/>
     </row>
-    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="30">
       <c r="A233" s="28" t="s">
         <v>233</v>
       </c>
@@ -10870,7 +10893,7 @@
       </c>
       <c r="I233" s="30"/>
     </row>
-    <row r="234" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" ht="45">
       <c r="A234" s="28" t="s">
         <v>208</v>
       </c>
@@ -10895,7 +10918,7 @@
       </c>
       <c r="I234" s="30"/>
     </row>
-    <row r="235" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="45">
       <c r="A235" s="28" t="s">
         <v>209</v>
       </c>
@@ -10920,7 +10943,7 @@
       </c>
       <c r="I235" s="30"/>
     </row>
-    <row r="236" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="45">
       <c r="A236" s="28" t="s">
         <v>880</v>
       </c>
@@ -10945,7 +10968,7 @@
       </c>
       <c r="I236" s="30"/>
     </row>
-    <row r="237" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="60">
       <c r="A237" s="28" t="s">
         <v>881</v>
       </c>
@@ -10970,7 +10993,7 @@
       </c>
       <c r="I237" s="30"/>
     </row>
-    <row r="238" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" ht="30">
       <c r="A238" s="28" t="s">
         <v>234</v>
       </c>
@@ -10995,7 +11018,7 @@
       </c>
       <c r="I238" s="30"/>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" ht="30">
       <c r="A239" s="28" t="s">
         <v>235</v>
       </c>
@@ -11020,7 +11043,7 @@
       </c>
       <c r="I239" s="30"/>
     </row>
-    <row r="240" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" ht="30">
       <c r="A240" s="28" t="s">
         <v>236</v>
       </c>
@@ -11045,7 +11068,7 @@
       </c>
       <c r="I240" s="30"/>
     </row>
-    <row r="241" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" ht="75">
       <c r="A241" s="28" t="s">
         <v>237</v>
       </c>
@@ -11070,7 +11093,7 @@
       </c>
       <c r="I241" s="30"/>
     </row>
-    <row r="242" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" ht="75">
       <c r="A242" s="28" t="s">
         <v>238</v>
       </c>
@@ -11095,7 +11118,7 @@
       </c>
       <c r="I242" s="30"/>
     </row>
-    <row r="243" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" ht="45">
       <c r="A243" s="28" t="s">
         <v>239</v>
       </c>
@@ -11120,7 +11143,7 @@
       </c>
       <c r="I243" s="30"/>
     </row>
-    <row r="244" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="30">
       <c r="A244" s="28" t="s">
         <v>240</v>
       </c>
@@ -11145,7 +11168,7 @@
       </c>
       <c r="I244" s="30"/>
     </row>
-    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="30">
       <c r="A245" s="28" t="s">
         <v>241</v>
       </c>
@@ -11170,7 +11193,7 @@
       </c>
       <c r="I245" s="30"/>
     </row>
-    <row r="246" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" ht="45">
       <c r="A246" s="28" t="s">
         <v>242</v>
       </c>
@@ -11195,7 +11218,7 @@
       </c>
       <c r="I246" s="30"/>
     </row>
-    <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" ht="45">
       <c r="A247" s="28" t="s">
         <v>243</v>
       </c>
@@ -11220,7 +11243,7 @@
       </c>
       <c r="I247" s="30"/>
     </row>
-    <row r="248" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" ht="135">
       <c r="A248" s="28" t="s">
         <v>244</v>
       </c>
@@ -11245,7 +11268,7 @@
       </c>
       <c r="I248" s="30"/>
     </row>
-    <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" ht="45">
       <c r="A249" s="28" t="s">
         <v>245</v>
       </c>
@@ -11270,7 +11293,7 @@
       </c>
       <c r="I249" s="30"/>
     </row>
-    <row r="250" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" ht="30">
       <c r="A250" s="28" t="s">
         <v>246</v>
       </c>
@@ -11295,7 +11318,7 @@
       </c>
       <c r="I250" s="30"/>
     </row>
-    <row r="251" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" ht="270">
       <c r="A251" s="28" t="s">
         <v>247</v>
       </c>
@@ -11320,7 +11343,7 @@
       </c>
       <c r="I251" s="30"/>
     </row>
-    <row r="252" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" ht="45">
       <c r="A252" s="28" t="s">
         <v>248</v>
       </c>
@@ -11345,7 +11368,7 @@
       </c>
       <c r="I252" s="30"/>
     </row>
-    <row r="253" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" ht="30">
       <c r="A253" s="28" t="s">
         <v>249</v>
       </c>
@@ -11370,7 +11393,7 @@
       </c>
       <c r="I253" s="30"/>
     </row>
-    <row r="254" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" ht="30">
       <c r="A254" s="28" t="s">
         <v>250</v>
       </c>
@@ -11395,7 +11418,7 @@
       </c>
       <c r="I254" s="30"/>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" ht="30">
       <c r="A255" s="28" t="s">
         <v>251</v>
       </c>
@@ -11420,7 +11443,7 @@
       </c>
       <c r="I255" s="30"/>
     </row>
-    <row r="256" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" ht="30">
       <c r="A256" s="28" t="s">
         <v>252</v>
       </c>
@@ -11445,7 +11468,7 @@
       </c>
       <c r="I256" s="30"/>
     </row>
-    <row r="257" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="30">
       <c r="A257" s="28" t="s">
         <v>253</v>
       </c>
@@ -11470,7 +11493,7 @@
       </c>
       <c r="I257" s="30"/>
     </row>
-    <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" ht="30">
       <c r="A258" s="28" t="s">
         <v>254</v>
       </c>
@@ -11495,7 +11518,7 @@
       </c>
       <c r="I258" s="30"/>
     </row>
-    <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" ht="30">
       <c r="A259" s="28" t="s">
         <v>255</v>
       </c>
@@ -11520,7 +11543,7 @@
       </c>
       <c r="I259" s="30"/>
     </row>
-    <row r="260" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="90">
       <c r="A260" s="28" t="s">
         <v>256</v>
       </c>
@@ -11545,7 +11568,7 @@
       </c>
       <c r="I260" s="30"/>
     </row>
-    <row r="261" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" ht="315">
       <c r="A261" s="28" t="s">
         <v>257</v>
       </c>
@@ -11570,7 +11593,7 @@
       </c>
       <c r="I261" s="30"/>
     </row>
-    <row r="262" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" ht="30">
       <c r="A262" s="28" t="s">
         <v>258</v>
       </c>
@@ -11595,7 +11618,7 @@
       </c>
       <c r="I262" s="30"/>
     </row>
-    <row r="263" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" ht="30">
       <c r="A263" s="28" t="s">
         <v>259</v>
       </c>
@@ -11620,7 +11643,7 @@
       </c>
       <c r="I263" s="30"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9">
       <c r="A264" s="28" t="s">
         <v>260</v>
       </c>
@@ -11645,7 +11668,7 @@
       </c>
       <c r="I264" s="30"/>
     </row>
-    <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" ht="45">
       <c r="A265" s="28" t="s">
         <v>261</v>
       </c>
@@ -11672,7 +11695,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" ht="30">
       <c r="A266" s="28" t="s">
         <v>262</v>
       </c>
@@ -11699,7 +11722,7 @@
       </c>
       <c r="I266" s="30"/>
     </row>
-    <row r="267" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" ht="30">
       <c r="A267" s="28" t="s">
         <v>263</v>
       </c>
@@ -11724,7 +11747,7 @@
       </c>
       <c r="I267" s="30"/>
     </row>
-    <row r="268" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" ht="30">
       <c r="A268" s="28" t="s">
         <v>264</v>
       </c>
@@ -11749,7 +11772,7 @@
       </c>
       <c r="I268" s="30"/>
     </row>
-    <row r="269" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" ht="45">
       <c r="A269" s="28" t="s">
         <v>267</v>
       </c>
@@ -11774,7 +11797,7 @@
       </c>
       <c r="I269" s="30"/>
     </row>
-    <row r="270" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" ht="30">
       <c r="A270" s="28" t="s">
         <v>268</v>
       </c>
@@ -11799,7 +11822,7 @@
       </c>
       <c r="I270" s="30"/>
     </row>
-    <row r="271" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" ht="30">
       <c r="A271" s="28" t="s">
         <v>269</v>
       </c>
@@ -11824,7 +11847,7 @@
       </c>
       <c r="I271" s="30"/>
     </row>
-    <row r="272" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" ht="120">
       <c r="A272" s="28" t="s">
         <v>270</v>
       </c>
@@ -11849,7 +11872,7 @@
       </c>
       <c r="I272" s="30"/>
     </row>
-    <row r="273" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" ht="45">
       <c r="A273" s="28" t="s">
         <v>271</v>
       </c>
@@ -11874,7 +11897,7 @@
       </c>
       <c r="I273" s="30"/>
     </row>
-    <row r="274" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" ht="45">
       <c r="A274" s="28" t="s">
         <v>272</v>
       </c>
@@ -11899,7 +11922,7 @@
       </c>
       <c r="I274" s="30"/>
     </row>
-    <row r="275" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" ht="30">
       <c r="A275" s="28" t="s">
         <v>273</v>
       </c>
@@ -11924,7 +11947,7 @@
       </c>
       <c r="I275" s="30"/>
     </row>
-    <row r="276" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" ht="30">
       <c r="A276" s="28" t="s">
         <v>274</v>
       </c>
@@ -11949,7 +11972,7 @@
       </c>
       <c r="I276" s="30"/>
     </row>
-    <row r="277" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" ht="30">
       <c r="A277" s="28" t="s">
         <v>275</v>
       </c>
@@ -11974,7 +11997,7 @@
       </c>
       <c r="I277" s="30"/>
     </row>
-    <row r="278" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" ht="30">
       <c r="A278" s="28" t="s">
         <v>276</v>
       </c>
@@ -11999,7 +12022,7 @@
       </c>
       <c r="I278" s="30"/>
     </row>
-    <row r="279" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" ht="30">
       <c r="A279" s="28" t="s">
         <v>277</v>
       </c>
@@ -12024,7 +12047,7 @@
       </c>
       <c r="I279" s="30"/>
     </row>
-    <row r="280" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" ht="30">
       <c r="A280" s="28" t="s">
         <v>278</v>
       </c>
@@ -12049,7 +12072,7 @@
       </c>
       <c r="I280" s="30"/>
     </row>
-    <row r="281" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" ht="30">
       <c r="A281" s="28" t="s">
         <v>279</v>
       </c>
@@ -12074,7 +12097,7 @@
       </c>
       <c r="I281" s="30"/>
     </row>
-    <row r="282" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" ht="30">
       <c r="A282" s="28" t="s">
         <v>280</v>
       </c>
@@ -12099,7 +12122,7 @@
       </c>
       <c r="I282" s="30"/>
     </row>
-    <row r="283" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" ht="30">
       <c r="A283" s="28" t="s">
         <v>281</v>
       </c>
@@ -12124,7 +12147,7 @@
       </c>
       <c r="I283" s="30"/>
     </row>
-    <row r="284" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" ht="120">
       <c r="A284" s="28" t="s">
         <v>282</v>
       </c>
@@ -12149,7 +12172,7 @@
       </c>
       <c r="I284" s="30"/>
     </row>
-    <row r="285" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" ht="45">
       <c r="A285" s="28" t="s">
         <v>283</v>
       </c>
@@ -12174,7 +12197,7 @@
       </c>
       <c r="I285" s="30"/>
     </row>
-    <row r="286" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" ht="45">
       <c r="A286" s="28" t="s">
         <v>284</v>
       </c>
@@ -12199,7 +12222,7 @@
       </c>
       <c r="I286" s="30"/>
     </row>
-    <row r="287" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" ht="30">
       <c r="A287" s="28" t="s">
         <v>285</v>
       </c>
@@ -12224,7 +12247,7 @@
       </c>
       <c r="I287" s="30"/>
     </row>
-    <row r="288" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" ht="30">
       <c r="A288" s="28" t="s">
         <v>286</v>
       </c>
@@ -12249,7 +12272,7 @@
       </c>
       <c r="I288" s="30"/>
     </row>
-    <row r="289" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" ht="30">
       <c r="A289" s="28" t="s">
         <v>287</v>
       </c>
@@ -12274,7 +12297,7 @@
       </c>
       <c r="I289" s="30"/>
     </row>
-    <row r="290" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" ht="30">
       <c r="A290" s="28" t="s">
         <v>288</v>
       </c>
@@ -12299,7 +12322,7 @@
       </c>
       <c r="I290" s="30"/>
     </row>
-    <row r="291" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" ht="45">
       <c r="A291" s="28" t="s">
         <v>265</v>
       </c>
@@ -12324,7 +12347,7 @@
       </c>
       <c r="I291" s="30"/>
     </row>
-    <row r="292" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" ht="45">
       <c r="A292" s="28" t="s">
         <v>266</v>
       </c>
@@ -12349,7 +12372,7 @@
       </c>
       <c r="I292" s="30"/>
     </row>
-    <row r="293" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" ht="45">
       <c r="A293" s="28" t="s">
         <v>856</v>
       </c>
@@ -12374,7 +12397,7 @@
       </c>
       <c r="I293" s="30"/>
     </row>
-    <row r="294" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" ht="60">
       <c r="A294" s="28" t="s">
         <v>857</v>
       </c>
@@ -12399,7 +12422,7 @@
       </c>
       <c r="I294" s="30"/>
     </row>
-    <row r="295" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" ht="45">
       <c r="A295" s="28" t="s">
         <v>289</v>
       </c>
@@ -12424,7 +12447,7 @@
       </c>
       <c r="I295" s="30"/>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" ht="30">
       <c r="A296" s="28" t="s">
         <v>290</v>
       </c>
@@ -12449,7 +12472,7 @@
       </c>
       <c r="I296" s="30"/>
     </row>
-    <row r="297" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" ht="30">
       <c r="A297" s="28" t="s">
         <v>291</v>
       </c>
@@ -12474,7 +12497,7 @@
       </c>
       <c r="I297" s="30"/>
     </row>
-    <row r="298" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" ht="30">
       <c r="A298" s="28" t="s">
         <v>292</v>
       </c>
@@ -12499,7 +12522,7 @@
       </c>
       <c r="I298" s="30"/>
     </row>
-    <row r="299" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" ht="60">
       <c r="A299" s="28" t="s">
         <v>293</v>
       </c>
@@ -12524,7 +12547,7 @@
       </c>
       <c r="I299" s="30"/>
     </row>
-    <row r="300" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" ht="75">
       <c r="A300" s="28" t="s">
         <v>294</v>
       </c>
@@ -12549,7 +12572,7 @@
       </c>
       <c r="I300" s="30"/>
     </row>
-    <row r="301" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" ht="45">
       <c r="A301" s="28" t="s">
         <v>295</v>
       </c>
@@ -12574,7 +12597,7 @@
       </c>
       <c r="I301" s="30"/>
     </row>
-    <row r="302" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" ht="30">
       <c r="A302" s="28" t="s">
         <v>296</v>
       </c>
@@ -12599,7 +12622,7 @@
       </c>
       <c r="I302" s="30"/>
     </row>
-    <row r="303" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" ht="30">
       <c r="A303" s="28" t="s">
         <v>297</v>
       </c>
@@ -12624,7 +12647,7 @@
       </c>
       <c r="I303" s="30"/>
     </row>
-    <row r="304" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" ht="30">
       <c r="A304" s="28" t="s">
         <v>298</v>
       </c>
@@ -12649,7 +12672,7 @@
       </c>
       <c r="I304" s="30"/>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" ht="30">
       <c r="A305" s="28" t="s">
         <v>859</v>
       </c>
@@ -12674,7 +12697,7 @@
       </c>
       <c r="I305" s="30"/>
     </row>
-    <row r="306" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" ht="30">
       <c r="A306" s="28" t="s">
         <v>860</v>
       </c>
@@ -12699,7 +12722,7 @@
       </c>
       <c r="I306" s="30"/>
     </row>
-    <row r="307" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" ht="45">
       <c r="A307" s="28" t="s">
         <v>299</v>
       </c>
@@ -12724,7 +12747,7 @@
       </c>
       <c r="I307" s="30"/>
     </row>
-    <row r="308" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" ht="45">
       <c r="A308" s="28" t="s">
         <v>300</v>
       </c>
@@ -12749,7 +12772,7 @@
       </c>
       <c r="I308" s="30"/>
     </row>
-    <row r="309" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" ht="240">
       <c r="A309" s="28" t="s">
         <v>301</v>
       </c>
@@ -12774,7 +12797,7 @@
       </c>
       <c r="I309" s="30"/>
     </row>
-    <row r="310" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" ht="45">
       <c r="A310" s="28" t="s">
         <v>302</v>
       </c>
@@ -12799,7 +12822,7 @@
       </c>
       <c r="I310" s="30"/>
     </row>
-    <row r="311" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" ht="30">
       <c r="A311" s="28" t="s">
         <v>303</v>
       </c>
@@ -12824,7 +12847,7 @@
       </c>
       <c r="I311" s="30"/>
     </row>
-    <row r="312" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" ht="30">
       <c r="A312" s="28" t="s">
         <v>304</v>
       </c>
@@ -12849,7 +12872,7 @@
       </c>
       <c r="I312" s="30"/>
     </row>
-    <row r="313" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" ht="45">
       <c r="A313" s="28" t="s">
         <v>305</v>
       </c>
@@ -12874,7 +12897,7 @@
       </c>
       <c r="I313" s="30"/>
     </row>
-    <row r="314" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" ht="45">
       <c r="A314" s="28" t="s">
         <v>306</v>
       </c>
@@ -12899,7 +12922,7 @@
       </c>
       <c r="I314" s="30"/>
     </row>
-    <row r="315" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" ht="135">
       <c r="A315" s="28" t="s">
         <v>307</v>
       </c>
@@ -12924,7 +12947,7 @@
       </c>
       <c r="I315" s="30"/>
     </row>
-    <row r="316" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" ht="30">
       <c r="A316" s="28" t="s">
         <v>308</v>
       </c>
@@ -12949,7 +12972,7 @@
       </c>
       <c r="I316" s="30"/>
     </row>
-    <row r="317" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" ht="30">
       <c r="A317" s="28" t="s">
         <v>309</v>
       </c>
@@ -12974,7 +12997,7 @@
       </c>
       <c r="I317" s="30"/>
     </row>
-    <row r="318" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" ht="225">
       <c r="A318" s="28" t="s">
         <v>310</v>
       </c>
@@ -12999,7 +13022,7 @@
       </c>
       <c r="I318" s="30"/>
     </row>
-    <row r="319" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" ht="30">
       <c r="A319" s="28" t="s">
         <v>311</v>
       </c>
@@ -13024,7 +13047,7 @@
       </c>
       <c r="I319" s="30"/>
     </row>
-    <row r="320" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" ht="30">
       <c r="A320" s="28" t="s">
         <v>312</v>
       </c>
@@ -13049,7 +13072,7 @@
       </c>
       <c r="I320" s="30"/>
     </row>
-    <row r="321" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" ht="30">
       <c r="A321" s="28" t="s">
         <v>313</v>
       </c>
@@ -13074,7 +13097,7 @@
       </c>
       <c r="I321" s="30"/>
     </row>
-    <row r="322" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" ht="30">
       <c r="A322" s="28" t="s">
         <v>168</v>
       </c>
@@ -13099,7 +13122,7 @@
       </c>
       <c r="I322" s="30"/>
     </row>
-    <row r="323" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" ht="30">
       <c r="A323" s="28" t="s">
         <v>169</v>
       </c>
@@ -13124,7 +13147,7 @@
       </c>
       <c r="I323" s="30"/>
     </row>
-    <row r="324" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" ht="255">
       <c r="A324" s="28" t="s">
         <v>170</v>
       </c>
@@ -13149,7 +13172,7 @@
       </c>
       <c r="I324" s="30"/>
     </row>
-    <row r="325" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" ht="45">
       <c r="A325" s="28" t="s">
         <v>171</v>
       </c>
@@ -13174,7 +13197,7 @@
       </c>
       <c r="I325" s="30"/>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" ht="30">
       <c r="A326" s="28" t="s">
         <v>172</v>
       </c>
@@ -13199,7 +13222,7 @@
       </c>
       <c r="I326" s="30"/>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" ht="30">
       <c r="A327" s="28" t="s">
         <v>173</v>
       </c>
@@ -13224,7 +13247,7 @@
       </c>
       <c r="I327" s="30"/>
     </row>
-    <row r="328" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" ht="45">
       <c r="A328" s="28" t="s">
         <v>174</v>
       </c>
@@ -13251,7 +13274,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="329" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" ht="30">
       <c r="A329" s="28" t="s">
         <v>175</v>
       </c>
@@ -13278,7 +13301,7 @@
       </c>
       <c r="I329" s="30"/>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9">
       <c r="A330" s="28" t="s">
         <v>176</v>
       </c>
@@ -13303,7 +13326,7 @@
       </c>
       <c r="I330" s="30"/>
     </row>
-    <row r="331" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" ht="30">
       <c r="A331" s="28" t="s">
         <v>177</v>
       </c>
@@ -13328,7 +13351,7 @@
       </c>
       <c r="I331" s="30"/>
     </row>
-    <row r="332" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" ht="45">
       <c r="A332" s="28" t="s">
         <v>178</v>
       </c>
@@ -13355,7 +13378,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="333" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" ht="30">
       <c r="A333" s="28" t="s">
         <v>179</v>
       </c>
@@ -13382,7 +13405,7 @@
       </c>
       <c r="I333" s="30"/>
     </row>
-    <row r="334" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" ht="30">
       <c r="A334" s="28" t="s">
         <v>314</v>
       </c>
@@ -13407,7 +13430,7 @@
       </c>
       <c r="I334" s="30"/>
     </row>
-    <row r="335" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" ht="90">
       <c r="A335" s="28" t="s">
         <v>315</v>
       </c>
@@ -13432,7 +13455,7 @@
       </c>
       <c r="I335" s="30"/>
     </row>
-    <row r="336" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" ht="345">
       <c r="A336" s="28" t="s">
         <v>316</v>
       </c>
@@ -13457,7 +13480,7 @@
       </c>
       <c r="I336" s="30"/>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" ht="30">
       <c r="A337" s="28" t="s">
         <v>317</v>
       </c>
@@ -13482,7 +13505,7 @@
       </c>
       <c r="I337" s="30"/>
     </row>
-    <row r="338" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" ht="30">
       <c r="A338" s="28" t="s">
         <v>318</v>
       </c>
@@ -13507,7 +13530,7 @@
       </c>
       <c r="I338" s="30"/>
     </row>
-    <row r="339" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" ht="45">
       <c r="A339" s="28" t="s">
         <v>321</v>
       </c>
@@ -13532,7 +13555,7 @@
       </c>
       <c r="I339" s="30"/>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" ht="30">
       <c r="A340" s="28" t="s">
         <v>322</v>
       </c>
@@ -13557,7 +13580,7 @@
       </c>
       <c r="I340" s="30"/>
     </row>
-    <row r="341" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" ht="30">
       <c r="A341" s="28" t="s">
         <v>323</v>
       </c>
@@ -13582,7 +13605,7 @@
       </c>
       <c r="I341" s="30"/>
     </row>
-    <row r="342" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" ht="135">
       <c r="A342" s="28" t="s">
         <v>324</v>
       </c>
@@ -13607,7 +13630,7 @@
       </c>
       <c r="I342" s="30"/>
     </row>
-    <row r="343" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" ht="45">
       <c r="A343" s="28" t="s">
         <v>325</v>
       </c>
@@ -13632,7 +13655,7 @@
       </c>
       <c r="I343" s="30"/>
     </row>
-    <row r="344" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" ht="45">
       <c r="A344" s="28" t="s">
         <v>326</v>
       </c>
@@ -13657,7 +13680,7 @@
       </c>
       <c r="I344" s="30"/>
     </row>
-    <row r="345" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" ht="30">
       <c r="A345" s="28" t="s">
         <v>327</v>
       </c>
@@ -13682,7 +13705,7 @@
       </c>
       <c r="I345" s="30"/>
     </row>
-    <row r="346" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" ht="30">
       <c r="A346" s="28" t="s">
         <v>328</v>
       </c>
@@ -13707,7 +13730,7 @@
       </c>
       <c r="I346" s="30"/>
     </row>
-    <row r="347" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" ht="30">
       <c r="A347" s="28" t="s">
         <v>329</v>
       </c>
@@ -13732,7 +13755,7 @@
       </c>
       <c r="I347" s="30"/>
     </row>
-    <row r="348" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" ht="30">
       <c r="A348" s="28" t="s">
         <v>330</v>
       </c>
@@ -13757,7 +13780,7 @@
       </c>
       <c r="I348" s="30"/>
     </row>
-    <row r="349" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" ht="30">
       <c r="A349" s="28" t="s">
         <v>331</v>
       </c>
@@ -13782,7 +13805,7 @@
       </c>
       <c r="I349" s="30"/>
     </row>
-    <row r="350" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" ht="30">
       <c r="A350" s="28" t="s">
         <v>332</v>
       </c>
@@ -13807,7 +13830,7 @@
       </c>
       <c r="I350" s="30"/>
     </row>
-    <row r="351" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" ht="30">
       <c r="A351" s="28" t="s">
         <v>333</v>
       </c>
@@ -13832,7 +13855,7 @@
       </c>
       <c r="I351" s="30"/>
     </row>
-    <row r="352" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" ht="30">
       <c r="A352" s="28" t="s">
         <v>334</v>
       </c>
@@ -13857,7 +13880,7 @@
       </c>
       <c r="I352" s="30"/>
     </row>
-    <row r="353" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:9" ht="30">
       <c r="A353" s="28" t="s">
         <v>335</v>
       </c>
@@ -13882,7 +13905,7 @@
       </c>
       <c r="I353" s="30"/>
     </row>
-    <row r="354" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:9" ht="30">
       <c r="A354" s="28" t="s">
         <v>336</v>
       </c>
@@ -13907,7 +13930,7 @@
       </c>
       <c r="I354" s="30"/>
     </row>
-    <row r="355" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:9" ht="30">
       <c r="A355" s="28" t="s">
         <v>337</v>
       </c>
@@ -13932,7 +13955,7 @@
       </c>
       <c r="I355" s="30"/>
     </row>
-    <row r="356" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:9" ht="90">
       <c r="A356" s="28" t="s">
         <v>338</v>
       </c>
@@ -13957,7 +13980,7 @@
       </c>
       <c r="I356" s="30"/>
     </row>
-    <row r="357" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:9" ht="45">
       <c r="A357" s="28" t="s">
         <v>339</v>
       </c>
@@ -13982,7 +14005,7 @@
       </c>
       <c r="I357" s="30"/>
     </row>
-    <row r="358" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:9" ht="45">
       <c r="A358" s="28" t="s">
         <v>340</v>
       </c>
@@ -14007,7 +14030,7 @@
       </c>
       <c r="I358" s="30"/>
     </row>
-    <row r="359" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:9" ht="30">
       <c r="A359" s="28" t="s">
         <v>341</v>
       </c>
@@ -14032,7 +14055,7 @@
       </c>
       <c r="I359" s="30"/>
     </row>
-    <row r="360" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:9" ht="30">
       <c r="A360" s="28" t="s">
         <v>342</v>
       </c>
@@ -14057,7 +14080,7 @@
       </c>
       <c r="I360" s="30"/>
     </row>
-    <row r="361" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:9" ht="30">
       <c r="A361" s="28" t="s">
         <v>343</v>
       </c>
@@ -14082,7 +14105,7 @@
       </c>
       <c r="I361" s="30"/>
     </row>
-    <row r="362" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:9" ht="30">
       <c r="A362" s="28" t="s">
         <v>344</v>
       </c>
@@ -14107,7 +14130,7 @@
       </c>
       <c r="I362" s="30"/>
     </row>
-    <row r="363" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:9" ht="45">
       <c r="A363" s="28" t="s">
         <v>319</v>
       </c>
@@ -14132,7 +14155,7 @@
       </c>
       <c r="I363" s="30"/>
     </row>
-    <row r="364" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:9" ht="45">
       <c r="A364" s="28" t="s">
         <v>320</v>
       </c>
@@ -14157,7 +14180,7 @@
       </c>
       <c r="I364" s="30"/>
     </row>
-    <row r="365" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:9" ht="45">
       <c r="A365" s="28" t="s">
         <v>875</v>
       </c>
@@ -14182,7 +14205,7 @@
       </c>
       <c r="I365" s="30"/>
     </row>
-    <row r="366" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:9" ht="60">
       <c r="A366" s="28" t="s">
         <v>876</v>
       </c>
@@ -14207,7 +14230,7 @@
       </c>
       <c r="I366" s="30"/>
     </row>
-    <row r="367" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:9" ht="45">
       <c r="A367" s="28" t="s">
         <v>345</v>
       </c>
@@ -14232,7 +14255,7 @@
       </c>
       <c r="I367" s="30"/>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:9">
       <c r="A368" s="28" t="s">
         <v>346</v>
       </c>
@@ -14257,7 +14280,7 @@
       </c>
       <c r="I368" s="30"/>
     </row>
-    <row r="369" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:9" ht="30">
       <c r="A369" s="28" t="s">
         <v>347</v>
       </c>
@@ -14282,7 +14305,7 @@
       </c>
       <c r="I369" s="30"/>
     </row>
-    <row r="370" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" ht="75">
       <c r="A370" s="28" t="s">
         <v>348</v>
       </c>
@@ -14307,7 +14330,7 @@
       </c>
       <c r="I370" s="30"/>
     </row>
-    <row r="371" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" ht="75">
       <c r="A371" s="28" t="s">
         <v>349</v>
       </c>
@@ -14332,7 +14355,7 @@
       </c>
       <c r="I371" s="30"/>
     </row>
-    <row r="372" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" ht="60">
       <c r="A372" s="28" t="s">
         <v>350</v>
       </c>
@@ -14357,7 +14380,7 @@
       </c>
       <c r="I372" s="30"/>
     </row>
-    <row r="373" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" ht="30">
       <c r="A373" s="28" t="s">
         <v>351</v>
       </c>
@@ -14382,7 +14405,7 @@
       </c>
       <c r="I373" s="30"/>
     </row>
-    <row r="374" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" ht="30">
       <c r="A374" s="28" t="s">
         <v>352</v>
       </c>
@@ -14407,7 +14430,7 @@
       </c>
       <c r="I374" s="30"/>
     </row>
-    <row r="375" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:9" ht="30">
       <c r="A375" s="28" t="s">
         <v>353</v>
       </c>
@@ -14432,7 +14455,7 @@
       </c>
       <c r="I375" s="30"/>
     </row>
-    <row r="376" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" ht="45">
       <c r="A376" s="28" t="s">
         <v>354</v>
       </c>
@@ -14457,7 +14480,7 @@
       </c>
       <c r="I376" s="30"/>
     </row>
-    <row r="377" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" ht="150">
       <c r="A377" s="28" t="s">
         <v>355</v>
       </c>
@@ -14482,7 +14505,7 @@
       </c>
       <c r="I377" s="30"/>
     </row>
-    <row r="378" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" ht="30">
       <c r="A378" s="28" t="s">
         <v>356</v>
       </c>
@@ -14507,7 +14530,7 @@
       </c>
       <c r="I378" s="30"/>
     </row>
-    <row r="379" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" ht="285">
       <c r="A379" s="28" t="s">
         <v>357</v>
       </c>
@@ -14532,7 +14555,7 @@
       </c>
       <c r="I379" s="30"/>
     </row>
-    <row r="380" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:9" ht="45">
       <c r="A380" s="28" t="s">
         <v>358</v>
       </c>
@@ -14557,7 +14580,7 @@
       </c>
       <c r="I380" s="30"/>
     </row>
-    <row r="381" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" ht="30">
       <c r="A381" s="28" t="s">
         <v>359</v>
       </c>
@@ -14582,7 +14605,7 @@
       </c>
       <c r="I381" s="30"/>
     </row>
-    <row r="382" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:9" ht="30">
       <c r="A382" s="28" t="s">
         <v>360</v>
       </c>
@@ -14607,7 +14630,7 @@
       </c>
       <c r="I382" s="30"/>
     </row>
-    <row r="383" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:9" ht="30">
       <c r="A383" s="28" t="s">
         <v>361</v>
       </c>
@@ -14632,7 +14655,7 @@
       </c>
       <c r="I383" s="30"/>
     </row>
-    <row r="384" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:9" ht="30">
       <c r="A384" s="28" t="s">
         <v>362</v>
       </c>
@@ -14657,7 +14680,7 @@
       </c>
       <c r="I384" s="30"/>
     </row>
-    <row r="385" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:9" ht="345">
       <c r="A385" s="28" t="s">
         <v>363</v>
       </c>
@@ -14682,7 +14705,7 @@
       </c>
       <c r="I385" s="30"/>
     </row>
-    <row r="386" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:9" ht="45">
       <c r="A386" s="28" t="s">
         <v>364</v>
       </c>
@@ -14707,7 +14730,7 @@
       </c>
       <c r="I386" s="30"/>
     </row>
-    <row r="387" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:9" ht="30">
       <c r="A387" s="28" t="s">
         <v>365</v>
       </c>
@@ -14732,7 +14755,7 @@
       </c>
       <c r="I387" s="30"/>
     </row>
-    <row r="388" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:9" ht="30">
       <c r="A388" s="28" t="s">
         <v>366</v>
       </c>
@@ -14753,13 +14776,11 @@
         <v>15</v>
       </c>
       <c r="H388" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I388" s="30" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="389" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I388" s="30"/>
+    </row>
+    <row r="389" spans="1:9" ht="90">
       <c r="A389" s="28" t="s">
         <v>367</v>
       </c>
@@ -14783,10 +14804,10 @@
         <v>17</v>
       </c>
       <c r="I389" s="30" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="390" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" ht="30">
       <c r="A390" s="28" t="s">
         <v>368</v>
       </c>
@@ -14813,7 +14834,7 @@
       </c>
       <c r="I390" s="30"/>
     </row>
-    <row r="391" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:9" ht="30">
       <c r="A391" s="28" t="s">
         <v>373</v>
       </c>
@@ -14838,7 +14859,7 @@
       </c>
       <c r="I391" s="30"/>
     </row>
-    <row r="392" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:9" ht="30">
       <c r="A392" s="28" t="s">
         <v>374</v>
       </c>
@@ -14863,7 +14884,7 @@
       </c>
       <c r="I392" s="30"/>
     </row>
-    <row r="393" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:9" ht="45">
       <c r="A393" s="28" t="s">
         <v>375</v>
       </c>
@@ -14887,10 +14908,10 @@
         <v>17</v>
       </c>
       <c r="I393" s="30" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="394" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9" ht="30">
       <c r="A394" s="28" t="s">
         <v>376</v>
       </c>
@@ -14911,13 +14932,11 @@
         <v>15</v>
       </c>
       <c r="H394" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="I394" s="30" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="395" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I394" s="30"/>
+    </row>
+    <row r="395" spans="1:9" ht="45">
       <c r="A395" s="28" t="s">
         <v>899</v>
       </c>
@@ -14942,7 +14961,7 @@
       </c>
       <c r="I395" s="30"/>
     </row>
-    <row r="396" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:9" ht="45">
       <c r="A396" s="28" t="s">
         <v>902</v>
       </c>
@@ -14969,7 +14988,7 @@
       </c>
       <c r="I396" s="30"/>
     </row>
-    <row r="397" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:9" ht="30">
       <c r="A397" s="28" t="s">
         <v>377</v>
       </c>
@@ -14994,7 +15013,7 @@
       </c>
       <c r="I397" s="30"/>
     </row>
-    <row r="398" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:9" ht="30">
       <c r="A398" s="28" t="s">
         <v>378</v>
       </c>
@@ -15019,7 +15038,7 @@
       </c>
       <c r="I398" s="30"/>
     </row>
-    <row r="399" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:9" ht="45">
       <c r="A399" s="28" t="s">
         <v>379</v>
       </c>
@@ -15044,7 +15063,7 @@
       </c>
       <c r="I399" s="30"/>
     </row>
-    <row r="400" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:9" ht="30">
       <c r="A400" s="28" t="s">
         <v>380</v>
       </c>
@@ -15069,7 +15088,7 @@
       </c>
       <c r="I400" s="30"/>
     </row>
-    <row r="401" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:9" ht="45">
       <c r="A401" s="28" t="s">
         <v>381</v>
       </c>
@@ -15098,7 +15117,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="402" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:9" ht="75">
       <c r="A402" s="28" t="s">
         <v>777</v>
       </c>
@@ -15109,7 +15128,7 @@
         <v>778</v>
       </c>
       <c r="D402" s="28" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E402" s="28" t="s">
         <v>22</v>
@@ -15127,7 +15146,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="403" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:9" ht="30">
       <c r="A403" s="28" t="s">
         <v>903</v>
       </c>
@@ -15154,7 +15173,7 @@
       </c>
       <c r="I403" s="30"/>
     </row>
-    <row r="404" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:9" ht="45">
       <c r="A404" s="28" t="s">
         <v>904</v>
       </c>
@@ -15183,7 +15202,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="405" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:9" ht="30">
       <c r="A405" s="28" t="s">
         <v>905</v>
       </c>
@@ -15210,7 +15229,7 @@
       </c>
       <c r="I405" s="19"/>
     </row>
-    <row r="406" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:9" ht="45">
       <c r="A406" s="28" t="s">
         <v>906</v>
       </c>
@@ -15239,7 +15258,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="407" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:9" ht="45">
       <c r="A407" s="28" t="s">
         <v>914</v>
       </c>
@@ -15250,7 +15269,7 @@
         <v>915</v>
       </c>
       <c r="D407" s="28" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="E407" s="28" t="s">
         <v>22</v>
@@ -15268,18 +15287,18 @@
         <v>745</v>
       </c>
     </row>
-    <row r="408" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:9" ht="30">
       <c r="A408" s="28" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B408" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C408" s="30" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D408" s="28" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="E408" s="28" t="s">
         <v>22</v>
@@ -15295,7 +15314,7 @@
       </c>
       <c r="I408" s="30"/>
     </row>
-    <row r="409" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:9" ht="45">
       <c r="A409" s="28" t="s">
         <v>907</v>
       </c>
@@ -15322,7 +15341,7 @@
       </c>
       <c r="I409" s="19"/>
     </row>
-    <row r="410" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:9" ht="45">
       <c r="A410" s="28" t="s">
         <v>908</v>
       </c>
@@ -15351,7 +15370,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="411" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:9" ht="60">
       <c r="A411" s="28" t="s">
         <v>909</v>
       </c>
@@ -15359,7 +15378,7 @@
         <v>439</v>
       </c>
       <c r="C411" s="30" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D411" s="28" t="s">
         <v>932</v>
@@ -15378,7 +15397,7 @@
       </c>
       <c r="I411" s="30"/>
     </row>
-    <row r="412" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:9" ht="45">
       <c r="A412" s="28" t="s">
         <v>910</v>
       </c>
@@ -15386,7 +15405,7 @@
         <v>439</v>
       </c>
       <c r="C412" s="30" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D412" s="28" t="s">
         <v>932</v>
@@ -15407,7 +15426,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="413" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:9" ht="45">
       <c r="A413" s="28" t="s">
         <v>911</v>
       </c>
@@ -15418,7 +15437,7 @@
         <v>898</v>
       </c>
       <c r="D413" s="28" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E413" s="28" t="s">
         <v>22</v>
@@ -15434,7 +15453,7 @@
       </c>
       <c r="I413" s="30"/>
     </row>
-    <row r="414" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:9" ht="45">
       <c r="A414" s="28" t="s">
         <v>912</v>
       </c>
@@ -15445,7 +15464,7 @@
         <v>897</v>
       </c>
       <c r="D414" s="28" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E414" s="28" t="s">
         <v>22</v>
@@ -15457,13 +15476,13 @@
         <v>15</v>
       </c>
       <c r="H414" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I414" s="30" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="415" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:9" ht="75">
       <c r="A415" s="28" t="s">
         <v>369</v>
       </c>
@@ -15492,7 +15511,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="416" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:9" ht="75">
       <c r="A416" s="28" t="s">
         <v>370</v>
       </c>
@@ -15521,7 +15540,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="417" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:9" ht="75">
       <c r="A417" s="28" t="s">
         <v>371</v>
       </c>
@@ -15550,7 +15569,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="418" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:9" ht="105">
       <c r="A418" s="28" t="s">
         <v>372</v>
       </c>
@@ -15579,7 +15598,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="419" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:9" ht="30">
       <c r="A419" s="28" t="s">
         <v>919</v>
       </c>
@@ -15606,7 +15625,7 @@
       </c>
       <c r="I419" s="30"/>
     </row>
-    <row r="420" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:9" ht="45">
       <c r="A420" s="28" t="s">
         <v>382</v>
       </c>
@@ -15631,7 +15650,7 @@
       </c>
       <c r="I420" s="30"/>
     </row>
-    <row r="421" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:9" ht="30">
       <c r="A421" s="28" t="s">
         <v>383</v>
       </c>
@@ -15656,7 +15675,7 @@
       </c>
       <c r="I421" s="30"/>
     </row>
-    <row r="422" spans="1:9" ht="360" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:9" ht="360">
       <c r="A422" s="28" t="s">
         <v>384</v>
       </c>
@@ -15681,27 +15700,27 @@
       </c>
       <c r="I422" s="30"/>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:9">
       <c r="A423" s="3"/>
       <c r="B423" s="10"/>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:9">
       <c r="A424" s="3"/>
       <c r="B424" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A126:I233 A125:H125 A20:I124 A396:I422">
@@ -16009,105 +16028,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all/>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/office/internal/2005/internalDocumentation" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type" ma:readOnly="true"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="lastPrinted" minOccurs="0" maxOccurs="1" type="xsd:dateTime"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1. Update setup script 2. Add new SHOLDMAY config for Exchange 2019 and update test suites for MS-OXWSATT
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFED12EB-1F41-4C47-B3B9-EC9D0D74B758}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6615C0CA-22FE-433A-964D-0541E30AAAAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -3498,9 +3498,6 @@
     <t>[In tns:CreateAttachmentSoapIn Message][The type of RequestVersion part is] t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.9).</t>
   </si>
   <si>
-    <t>[In tns:CreateAttachmentSoapOut Message][The element of ServerVersion part is] t:ServerVersionInfo ([MS-OXWSCDATA] section 2.2.3.10                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                    ).</t>
-  </si>
-  <si>
     <t>[In tns:DeleteAttachmentSoapIn Message][The type of Impersonation part is] t:ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.3.3).</t>
   </si>
   <si>
@@ -3525,12 +3522,6 @@
     <t>[In tns:GetAttachmentSoapIn Message][The RequestVersion part is] t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.9)</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms "SHOULD" or "SHOULD NOT" implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Unless otherwise specified, the term "MAY" implies that the product does not follow the prescription.</t>
-  </si>
-  <si>
     <t>[In Appendix C: Product Behavior] Implementation does support the Person element. (Exchange 2016  and above follow this behavior).</t>
   </si>
   <si>
@@ -3543,13 +3534,26 @@
     <t>2.2.3.10</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Exchange2007 and Exchange2019.)</t>
-  </si>
-  <si>
     <t>2.2.4.50</t>
   </si>
   <si>
     <t>[In m:ResponseCodeType Simple Type] The value "ErrorUnsupportedMimeConversion" occurs when an attempt is made to retrieve  MIME content for an item other than a PostItemType, MessageType, or CalendarItemType object.</t>
+  </si>
+  <si>
+    <t>[In tns:CreateAttachmentSoapOut Message][The element of ServerVersion part is] t:ServerVersionInfo ([MS-OXWSCDATA] section 2.2.3.10).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Exchange2007 and Exchange2019 follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3557,14 +3561,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3604,6 +3608,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3769,7 +3774,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3807,7 +3812,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3848,8 +3853,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3861,27 +3866,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3906,6 +3890,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5136,26 +5141,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A413" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C420" sqref="C420"/>
+    <sheetView tabSelected="1" topLeftCell="A394" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C401" sqref="C401"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="21.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>735</v>
       </c>
@@ -5167,7 +5172,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>736</v>
       </c>
@@ -5181,7 +5186,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="37" t="s">
         <v>25</v>
@@ -5202,141 +5207,141 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="52" t="s">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="78.75" customHeight="1">
+    <row r="9" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="33.75" customHeight="1">
+    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="56" t="s">
         <v>738</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>737</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>8</v>
       </c>
@@ -5355,7 +5360,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>6</v>
       </c>
@@ -5374,7 +5379,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>7</v>
       </c>
@@ -5393,7 +5398,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>3</v>
       </c>
@@ -5412,59 +5417,59 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1">
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="64.5" customHeight="1">
+    <row r="17" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1">
+    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>739</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="30">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -5493,7 +5498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="22" customFormat="1" ht="60">
+    <row r="20" spans="1:13" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A20" s="21" t="s">
         <v>41</v>
       </c>
@@ -5519,7 +5524,7 @@
       <c r="I20" s="23"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:13" s="22" customFormat="1" ht="45">
+    <row r="21" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="21" t="s">
         <v>42</v>
       </c>
@@ -5545,7 +5550,7 @@
       <c r="I21" s="23"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="22" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="21" t="s">
         <v>43</v>
       </c>
@@ -5571,7 +5576,7 @@
       <c r="I22" s="23"/>
       <c r="J22" s="35"/>
     </row>
-    <row r="23" spans="1:13" s="22" customFormat="1">
+    <row r="23" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="21" t="s">
         <v>44</v>
       </c>
@@ -5597,7 +5602,7 @@
       <c r="I23" s="23"/>
       <c r="J23" s="35"/>
     </row>
-    <row r="24" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="24" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="21" t="s">
         <v>45</v>
       </c>
@@ -5623,7 +5628,7 @@
       <c r="I24" s="23"/>
       <c r="J24" s="35"/>
     </row>
-    <row r="25" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="25" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A25" s="21" t="s">
         <v>46</v>
       </c>
@@ -5649,7 +5654,7 @@
       <c r="I25" s="23"/>
       <c r="J25" s="35"/>
     </row>
-    <row r="26" spans="1:13" s="22" customFormat="1" ht="45">
+    <row r="26" spans="1:13" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A26" s="21" t="s">
         <v>47</v>
       </c>
@@ -5675,7 +5680,7 @@
       <c r="I26" s="23"/>
       <c r="J26" s="35"/>
     </row>
-    <row r="27" spans="1:13" s="22" customFormat="1">
+    <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="21" t="s">
         <v>48</v>
       </c>
@@ -5701,7 +5706,7 @@
       <c r="I27" s="23"/>
       <c r="J27" s="35"/>
     </row>
-    <row r="28" spans="1:13" s="22" customFormat="1">
+    <row r="28" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
@@ -5727,7 +5732,7 @@
       <c r="I28" s="23"/>
       <c r="J28" s="35"/>
     </row>
-    <row r="29" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="29" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>50</v>
       </c>
@@ -5753,7 +5758,7 @@
       <c r="I29" s="23"/>
       <c r="J29" s="35"/>
     </row>
-    <row r="30" spans="1:13" s="22" customFormat="1">
+    <row r="30" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>743</v>
       </c>
@@ -5779,7 +5784,7 @@
       <c r="I30" s="30"/>
       <c r="J30" s="35"/>
     </row>
-    <row r="31" spans="1:13" s="22" customFormat="1" ht="45">
+    <row r="31" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>51</v>
       </c>
@@ -5807,7 +5812,7 @@
       </c>
       <c r="J31" s="35"/>
     </row>
-    <row r="32" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="32" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>52</v>
       </c>
@@ -5833,7 +5838,7 @@
       <c r="I32" s="23"/>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="1:10" s="22" customFormat="1" ht="45">
+    <row r="33" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="21" t="s">
         <v>53</v>
       </c>
@@ -5859,7 +5864,7 @@
       <c r="I33" s="23"/>
       <c r="J33" s="35"/>
     </row>
-    <row r="34" spans="1:10" s="22" customFormat="1" ht="45">
+    <row r="34" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>54</v>
       </c>
@@ -5885,7 +5890,7 @@
       <c r="I34" s="23"/>
       <c r="J34" s="35"/>
     </row>
-    <row r="35" spans="1:10" ht="60">
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>55</v>
       </c>
@@ -5910,7 +5915,7 @@
       </c>
       <c r="I35" s="30"/>
     </row>
-    <row r="36" spans="1:10" ht="30">
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>56</v>
       </c>
@@ -5935,7 +5940,7 @@
       </c>
       <c r="I36" s="30"/>
     </row>
-    <row r="37" spans="1:10" ht="30">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>57</v>
       </c>
@@ -5960,7 +5965,7 @@
       </c>
       <c r="I37" s="30"/>
     </row>
-    <row r="38" spans="1:10" ht="30">
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>58</v>
       </c>
@@ -5985,7 +5990,7 @@
       </c>
       <c r="I38" s="30"/>
     </row>
-    <row r="39" spans="1:10" ht="30">
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>59</v>
       </c>
@@ -6010,7 +6015,7 @@
       </c>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:10" ht="30">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>745</v>
       </c>
@@ -6035,7 +6040,7 @@
       </c>
       <c r="I40" s="30"/>
     </row>
-    <row r="41" spans="1:10" ht="30">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>60</v>
       </c>
@@ -6060,7 +6065,7 @@
       </c>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" spans="1:10" ht="30">
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>748</v>
       </c>
@@ -6085,7 +6090,7 @@
       </c>
       <c r="I42" s="30"/>
     </row>
-    <row r="43" spans="1:10" ht="30">
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>61</v>
       </c>
@@ -6110,7 +6115,7 @@
       </c>
       <c r="I43" s="30"/>
     </row>
-    <row r="44" spans="1:10" ht="30">
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>62</v>
       </c>
@@ -6135,7 +6140,7 @@
       </c>
       <c r="I44" s="30"/>
     </row>
-    <row r="45" spans="1:10" ht="45">
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>63</v>
       </c>
@@ -6160,7 +6165,7 @@
       </c>
       <c r="I45" s="30"/>
     </row>
-    <row r="46" spans="1:10" ht="75">
+    <row r="46" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>64</v>
       </c>
@@ -6185,7 +6190,7 @@
       </c>
       <c r="I46" s="30"/>
     </row>
-    <row r="47" spans="1:10" ht="30">
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>65</v>
       </c>
@@ -6210,7 +6215,7 @@
       </c>
       <c r="I47" s="30"/>
     </row>
-    <row r="48" spans="1:10" ht="45">
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>66</v>
       </c>
@@ -6235,7 +6240,7 @@
       </c>
       <c r="I48" s="30"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>67</v>
       </c>
@@ -6260,7 +6265,7 @@
       </c>
       <c r="I49" s="30"/>
     </row>
-    <row r="50" spans="1:9" ht="30">
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>68</v>
       </c>
@@ -6285,7 +6290,7 @@
       </c>
       <c r="I50" s="30"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>69</v>
       </c>
@@ -6310,7 +6315,7 @@
       </c>
       <c r="I51" s="30"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>70</v>
       </c>
@@ -6335,7 +6340,7 @@
       </c>
       <c r="I52" s="30"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>71</v>
       </c>
@@ -6360,7 +6365,7 @@
       </c>
       <c r="I53" s="30"/>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>752</v>
       </c>
@@ -6385,7 +6390,7 @@
       </c>
       <c r="I54" s="30"/>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>72</v>
       </c>
@@ -6410,7 +6415,7 @@
       </c>
       <c r="I55" s="30"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>73</v>
       </c>
@@ -6435,7 +6440,7 @@
       </c>
       <c r="I56" s="30"/>
     </row>
-    <row r="57" spans="1:9" ht="45">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>74</v>
       </c>
@@ -6462,7 +6467,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>75</v>
       </c>
@@ -6489,7 +6494,7 @@
       </c>
       <c r="I58" s="30"/>
     </row>
-    <row r="59" spans="1:9" ht="270">
+    <row r="59" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
         <v>76</v>
       </c>
@@ -6514,7 +6519,7 @@
       </c>
       <c r="I59" s="30"/>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
         <v>77</v>
       </c>
@@ -6539,7 +6544,7 @@
       </c>
       <c r="I60" s="30"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
         <v>78</v>
       </c>
@@ -6564,7 +6569,7 @@
       </c>
       <c r="I61" s="30"/>
     </row>
-    <row r="62" spans="1:9" ht="30">
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="28" t="s">
         <v>79</v>
       </c>
@@ -6589,7 +6594,7 @@
       </c>
       <c r="I62" s="30"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>80</v>
       </c>
@@ -6614,7 +6619,7 @@
       </c>
       <c r="I63" s="30"/>
     </row>
-    <row r="64" spans="1:9" ht="30">
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="28" t="s">
         <v>81</v>
       </c>
@@ -6639,7 +6644,7 @@
       </c>
       <c r="I64" s="30"/>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
         <v>757</v>
       </c>
@@ -6664,7 +6669,7 @@
       </c>
       <c r="I65" s="30"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="28" t="s">
         <v>758</v>
       </c>
@@ -6689,7 +6694,7 @@
       </c>
       <c r="I66" s="30"/>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
         <v>82</v>
       </c>
@@ -6714,7 +6719,7 @@
       </c>
       <c r="I67" s="30"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>83</v>
       </c>
@@ -6739,7 +6744,7 @@
       </c>
       <c r="I68" s="30"/>
     </row>
-    <row r="69" spans="1:9" ht="255">
+    <row r="69" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
         <v>84</v>
       </c>
@@ -6764,7 +6769,7 @@
       </c>
       <c r="I69" s="30"/>
     </row>
-    <row r="70" spans="1:9" ht="45">
+    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
         <v>85</v>
       </c>
@@ -6789,7 +6794,7 @@
       </c>
       <c r="I70" s="30"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
         <v>86</v>
       </c>
@@ -6814,7 +6819,7 @@
       </c>
       <c r="I71" s="30"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="28" t="s">
         <v>87</v>
       </c>
@@ -6839,7 +6844,7 @@
       </c>
       <c r="I72" s="30"/>
     </row>
-    <row r="73" spans="1:9" ht="30">
+    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="28" t="s">
         <v>902</v>
       </c>
@@ -6864,7 +6869,7 @@
       </c>
       <c r="I73" s="30"/>
     </row>
-    <row r="74" spans="1:9" ht="45">
+    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
         <v>88</v>
       </c>
@@ -6891,7 +6896,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30">
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="28" t="s">
         <v>89</v>
       </c>
@@ -6918,7 +6923,7 @@
       </c>
       <c r="I75" s="30"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
         <v>90</v>
       </c>
@@ -6943,7 +6948,7 @@
       </c>
       <c r="I76" s="30"/>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>91</v>
       </c>
@@ -6968,7 +6973,7 @@
       </c>
       <c r="I77" s="30"/>
     </row>
-    <row r="78" spans="1:9" ht="45">
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>92</v>
       </c>
@@ -6995,7 +7000,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30">
+    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
         <v>93</v>
       </c>
@@ -7022,7 +7027,7 @@
       </c>
       <c r="I79" s="30"/>
     </row>
-    <row r="80" spans="1:9" ht="45">
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
         <v>94</v>
       </c>
@@ -7047,7 +7052,7 @@
       </c>
       <c r="I80" s="30"/>
     </row>
-    <row r="81" spans="1:9" ht="240">
+    <row r="81" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
         <v>95</v>
       </c>
@@ -7072,7 +7077,7 @@
       </c>
       <c r="I81" s="30"/>
     </row>
-    <row r="82" spans="1:9" ht="45">
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
         <v>96</v>
       </c>
@@ -7097,7 +7102,7 @@
       </c>
       <c r="I82" s="30"/>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
         <v>97</v>
       </c>
@@ -7122,7 +7127,7 @@
       </c>
       <c r="I83" s="30"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
         <v>98</v>
       </c>
@@ -7147,7 +7152,7 @@
       </c>
       <c r="I84" s="30"/>
     </row>
-    <row r="85" spans="1:9" ht="45">
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
         <v>99</v>
       </c>
@@ -7174,7 +7179,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
         <v>100</v>
       </c>
@@ -7201,7 +7206,7 @@
       </c>
       <c r="I86" s="30"/>
     </row>
-    <row r="87" spans="1:9" ht="409.5">
+    <row r="87" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
         <v>101</v>
       </c>
@@ -7226,7 +7231,7 @@
       </c>
       <c r="I87" s="30"/>
     </row>
-    <row r="88" spans="1:9" ht="45">
+    <row r="88" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
         <v>102</v>
       </c>
@@ -7251,7 +7256,7 @@
       </c>
       <c r="I88" s="30"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
         <v>103</v>
       </c>
@@ -7276,7 +7281,7 @@
       </c>
       <c r="I89" s="30"/>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
         <v>104</v>
       </c>
@@ -7301,7 +7306,7 @@
       </c>
       <c r="I90" s="30"/>
     </row>
-    <row r="91" spans="1:9" ht="30">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
         <v>105</v>
       </c>
@@ -7326,7 +7331,7 @@
       </c>
       <c r="I91" s="30"/>
     </row>
-    <row r="92" spans="1:9" ht="30">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
         <v>106</v>
       </c>
@@ -7351,7 +7356,7 @@
       </c>
       <c r="I92" s="30"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
         <v>107</v>
       </c>
@@ -7376,7 +7381,7 @@
       </c>
       <c r="I93" s="30"/>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
         <v>108</v>
       </c>
@@ -7401,7 +7406,7 @@
       </c>
       <c r="I94" s="30"/>
     </row>
-    <row r="95" spans="1:9" ht="45">
+    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="28" t="s">
         <v>109</v>
       </c>
@@ -7426,7 +7431,7 @@
       </c>
       <c r="I95" s="30"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="28" t="s">
         <v>110</v>
       </c>
@@ -7451,7 +7456,7 @@
       </c>
       <c r="I96" s="30"/>
     </row>
-    <row r="97" spans="1:9" ht="45">
+    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="28" t="s">
         <v>111</v>
       </c>
@@ -7478,7 +7483,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="28" t="s">
         <v>112</v>
       </c>
@@ -7505,7 +7510,7 @@
       </c>
       <c r="I98" s="30"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="28" t="s">
         <v>113</v>
       </c>
@@ -7530,7 +7535,7 @@
       </c>
       <c r="I99" s="30"/>
     </row>
-    <row r="100" spans="1:9" ht="30">
+    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="28" t="s">
         <v>114</v>
       </c>
@@ -7555,7 +7560,7 @@
       </c>
       <c r="I100" s="30"/>
     </row>
-    <row r="101" spans="1:9" ht="30">
+    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="28" t="s">
         <v>115</v>
       </c>
@@ -7580,7 +7585,7 @@
       </c>
       <c r="I101" s="30"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="28" t="s">
         <v>116</v>
       </c>
@@ -7605,7 +7610,7 @@
       </c>
       <c r="I102" s="30"/>
     </row>
-    <row r="103" spans="1:9" ht="30">
+    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="28" t="s">
         <v>117</v>
       </c>
@@ -7630,7 +7635,7 @@
       </c>
       <c r="I103" s="30"/>
     </row>
-    <row r="104" spans="1:9" ht="30">
+    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="28" t="s">
         <v>118</v>
       </c>
@@ -7655,7 +7660,7 @@
       </c>
       <c r="I104" s="30"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="28" t="s">
         <v>119</v>
       </c>
@@ -7680,7 +7685,7 @@
       </c>
       <c r="I105" s="30"/>
     </row>
-    <row r="106" spans="1:9" ht="45">
+    <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="28" t="s">
         <v>120</v>
       </c>
@@ -7707,7 +7712,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="28" t="s">
         <v>121</v>
       </c>
@@ -7732,7 +7737,7 @@
       </c>
       <c r="I107" s="30"/>
     </row>
-    <row r="108" spans="1:9" ht="30">
+    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="28" t="s">
         <v>122</v>
       </c>
@@ -7757,7 +7762,7 @@
       </c>
       <c r="I108" s="30"/>
     </row>
-    <row r="109" spans="1:9" ht="30">
+    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="28" t="s">
         <v>123</v>
       </c>
@@ -7782,7 +7787,7 @@
       </c>
       <c r="I109" s="30"/>
     </row>
-    <row r="110" spans="1:9" ht="30">
+    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="28" t="s">
         <v>124</v>
       </c>
@@ -7807,7 +7812,7 @@
       </c>
       <c r="I110" s="30"/>
     </row>
-    <row r="111" spans="1:9" ht="30">
+    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="28" t="s">
         <v>125</v>
       </c>
@@ -7832,7 +7837,7 @@
       </c>
       <c r="I111" s="30"/>
     </row>
-    <row r="112" spans="1:9" ht="330">
+    <row r="112" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A112" s="28" t="s">
         <v>126</v>
       </c>
@@ -7857,7 +7862,7 @@
       </c>
       <c r="I112" s="30"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="28" t="s">
         <v>127</v>
       </c>
@@ -7882,7 +7887,7 @@
       </c>
       <c r="I113" s="30"/>
     </row>
-    <row r="114" spans="1:9" ht="45">
+    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="28" t="s">
         <v>128</v>
       </c>
@@ -7909,7 +7914,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="30">
+    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="28" t="s">
         <v>129</v>
       </c>
@@ -7934,7 +7939,7 @@
       </c>
       <c r="I115" s="30"/>
     </row>
-    <row r="116" spans="1:9" ht="30">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="28" t="s">
         <v>130</v>
       </c>
@@ -7959,7 +7964,7 @@
       </c>
       <c r="I116" s="30"/>
     </row>
-    <row r="117" spans="1:9" ht="30">
+    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="28" t="s">
         <v>131</v>
       </c>
@@ -7984,7 +7989,7 @@
       </c>
       <c r="I117" s="30"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="28" t="s">
         <v>132</v>
       </c>
@@ -8009,7 +8014,7 @@
       </c>
       <c r="I118" s="30"/>
     </row>
-    <row r="119" spans="1:9" ht="30">
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="28" t="s">
         <v>133</v>
       </c>
@@ -8034,7 +8039,7 @@
       </c>
       <c r="I119" s="30"/>
     </row>
-    <row r="120" spans="1:9" ht="60">
+    <row r="120" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="28" t="s">
         <v>764</v>
       </c>
@@ -8061,7 +8066,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="45">
+    <row r="121" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="28" t="s">
         <v>765</v>
       </c>
@@ -8086,7 +8091,7 @@
       </c>
       <c r="I121" s="30"/>
     </row>
-    <row r="122" spans="1:9" ht="409.5">
+    <row r="122" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A122" s="28" t="s">
         <v>134</v>
       </c>
@@ -8111,7 +8116,7 @@
       </c>
       <c r="I122" s="30"/>
     </row>
-    <row r="123" spans="1:9" ht="60">
+    <row r="123" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="28" t="s">
         <v>135</v>
       </c>
@@ -8136,7 +8141,7 @@
       </c>
       <c r="I123" s="30"/>
     </row>
-    <row r="124" spans="1:9" ht="45">
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="28" t="s">
         <v>136</v>
       </c>
@@ -8163,7 +8168,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="30">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="28" t="s">
         <v>137</v>
       </c>
@@ -8188,7 +8193,7 @@
       </c>
       <c r="I125" s="30"/>
     </row>
-    <row r="126" spans="1:9" ht="30">
+    <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="28" t="s">
         <v>138</v>
       </c>
@@ -8213,7 +8218,7 @@
       </c>
       <c r="I126" s="30"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="28" t="s">
         <v>139</v>
       </c>
@@ -8238,7 +8243,7 @@
       </c>
       <c r="I127" s="30"/>
     </row>
-    <row r="128" spans="1:9" ht="30">
+    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="28" t="s">
         <v>140</v>
       </c>
@@ -8263,7 +8268,7 @@
       </c>
       <c r="I128" s="30"/>
     </row>
-    <row r="129" spans="1:9" ht="30">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="28" t="s">
         <v>141</v>
       </c>
@@ -8288,7 +8293,7 @@
       </c>
       <c r="I129" s="30"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="28" t="s">
         <v>142</v>
       </c>
@@ -8313,7 +8318,7 @@
       </c>
       <c r="I130" s="30"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="28" t="s">
         <v>143</v>
       </c>
@@ -8338,7 +8343,7 @@
       </c>
       <c r="I131" s="30"/>
     </row>
-    <row r="132" spans="1:9" ht="30">
+    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="28" t="s">
         <v>144</v>
       </c>
@@ -8363,7 +8368,7 @@
       </c>
       <c r="I132" s="30"/>
     </row>
-    <row r="133" spans="1:9" ht="30">
+    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="28" t="s">
         <v>145</v>
       </c>
@@ -8388,7 +8393,7 @@
       </c>
       <c r="I133" s="30"/>
     </row>
-    <row r="134" spans="1:9" ht="30">
+    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="28" t="s">
         <v>146</v>
       </c>
@@ -8413,7 +8418,7 @@
       </c>
       <c r="I134" s="30"/>
     </row>
-    <row r="135" spans="1:9" ht="30">
+    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="28" t="s">
         <v>147</v>
       </c>
@@ -8438,7 +8443,7 @@
       </c>
       <c r="I135" s="30"/>
     </row>
-    <row r="136" spans="1:9" ht="30">
+    <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="28" t="s">
         <v>148</v>
       </c>
@@ -8463,7 +8468,7 @@
       </c>
       <c r="I136" s="30"/>
     </row>
-    <row r="137" spans="1:9" ht="30">
+    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="28" t="s">
         <v>149</v>
       </c>
@@ -8488,7 +8493,7 @@
       </c>
       <c r="I137" s="30"/>
     </row>
-    <row r="138" spans="1:9" ht="30">
+    <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="28" t="s">
         <v>150</v>
       </c>
@@ -8513,7 +8518,7 @@
       </c>
       <c r="I138" s="30"/>
     </row>
-    <row r="139" spans="1:9" ht="30">
+    <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="28" t="s">
         <v>151</v>
       </c>
@@ -8538,7 +8543,7 @@
       </c>
       <c r="I139" s="30"/>
     </row>
-    <row r="140" spans="1:9" ht="30">
+    <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="28" t="s">
         <v>152</v>
       </c>
@@ -8563,7 +8568,7 @@
       </c>
       <c r="I140" s="30"/>
     </row>
-    <row r="141" spans="1:9" ht="30">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="28" t="s">
         <v>153</v>
       </c>
@@ -8588,7 +8593,7 @@
       </c>
       <c r="I141" s="30"/>
     </row>
-    <row r="142" spans="1:9" ht="30">
+    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="28" t="s">
         <v>154</v>
       </c>
@@ -8613,7 +8618,7 @@
       </c>
       <c r="I142" s="30"/>
     </row>
-    <row r="143" spans="1:9" ht="30">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="28" t="s">
         <v>155</v>
       </c>
@@ -8638,7 +8643,7 @@
       </c>
       <c r="I143" s="30"/>
     </row>
-    <row r="144" spans="1:9" ht="30">
+    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="28" t="s">
         <v>779</v>
       </c>
@@ -8663,7 +8668,7 @@
       </c>
       <c r="I144" s="30"/>
     </row>
-    <row r="145" spans="1:9" ht="30">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="28" t="s">
         <v>780</v>
       </c>
@@ -8688,7 +8693,7 @@
       </c>
       <c r="I145" s="30"/>
     </row>
-    <row r="146" spans="1:9" ht="30">
+    <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="28" t="s">
         <v>781</v>
       </c>
@@ -8713,7 +8718,7 @@
       </c>
       <c r="I146" s="30"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="28" t="s">
         <v>782</v>
       </c>
@@ -8738,7 +8743,7 @@
       </c>
       <c r="I147" s="30"/>
     </row>
-    <row r="148" spans="1:9" ht="30">
+    <row r="148" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="28" t="s">
         <v>783</v>
       </c>
@@ -8763,7 +8768,7 @@
       </c>
       <c r="I148" s="30"/>
     </row>
-    <row r="149" spans="1:9" ht="45">
+    <row r="149" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="28" t="s">
         <v>784</v>
       </c>
@@ -8790,7 +8795,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="30">
+    <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="28" t="s">
         <v>785</v>
       </c>
@@ -8815,7 +8820,7 @@
       </c>
       <c r="I150" s="30"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="28" t="s">
         <v>786</v>
       </c>
@@ -8840,7 +8845,7 @@
       </c>
       <c r="I151" s="30"/>
     </row>
-    <row r="152" spans="1:9" ht="45">
+    <row r="152" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="28" t="s">
         <v>156</v>
       </c>
@@ -8865,7 +8870,7 @@
       </c>
       <c r="I152" s="30"/>
     </row>
-    <row r="153" spans="1:9" ht="180">
+    <row r="153" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A153" s="28" t="s">
         <v>157</v>
       </c>
@@ -8890,7 +8895,7 @@
       </c>
       <c r="I153" s="30"/>
     </row>
-    <row r="154" spans="1:9" ht="45">
+    <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="28" t="s">
         <v>158</v>
       </c>
@@ -8915,7 +8920,7 @@
       </c>
       <c r="I154" s="30"/>
     </row>
-    <row r="155" spans="1:9" ht="30">
+    <row r="155" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="28" t="s">
         <v>159</v>
       </c>
@@ -8940,7 +8945,7 @@
       </c>
       <c r="I155" s="30"/>
     </row>
-    <row r="156" spans="1:9" ht="30">
+    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="28" t="s">
         <v>160</v>
       </c>
@@ -8965,7 +8970,7 @@
       </c>
       <c r="I156" s="30"/>
     </row>
-    <row r="157" spans="1:9" ht="30">
+    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="28" t="s">
         <v>806</v>
       </c>
@@ -8990,7 +8995,7 @@
       </c>
       <c r="I157" s="30"/>
     </row>
-    <row r="158" spans="1:9" ht="45">
+    <row r="158" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="28" t="s">
         <v>807</v>
       </c>
@@ -9017,7 +9022,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="330">
+    <row r="159" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A159" s="28" t="s">
         <v>915</v>
       </c>
@@ -9042,7 +9047,7 @@
       </c>
       <c r="I159" s="30"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="28" t="s">
         <v>808</v>
       </c>
@@ -9067,7 +9072,7 @@
       </c>
       <c r="I160" s="30"/>
     </row>
-    <row r="161" spans="1:9" ht="30">
+    <row r="161" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="28" t="s">
         <v>809</v>
       </c>
@@ -9092,7 +9097,7 @@
       </c>
       <c r="I161" s="30"/>
     </row>
-    <row r="162" spans="1:9" ht="30">
+    <row r="162" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="28" t="s">
         <v>810</v>
       </c>
@@ -9117,7 +9122,7 @@
       </c>
       <c r="I162" s="30"/>
     </row>
-    <row r="163" spans="1:9" ht="30">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="28" t="s">
         <v>811</v>
       </c>
@@ -9142,7 +9147,7 @@
       </c>
       <c r="I163" s="30"/>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="28" t="s">
         <v>812</v>
       </c>
@@ -9167,7 +9172,7 @@
       </c>
       <c r="I164" s="30"/>
     </row>
-    <row r="165" spans="1:9" ht="30">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="28" t="s">
         <v>813</v>
       </c>
@@ -9192,7 +9197,7 @@
       </c>
       <c r="I165" s="30"/>
     </row>
-    <row r="166" spans="1:9" ht="30">
+    <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="28" t="s">
         <v>814</v>
       </c>
@@ -9217,7 +9222,7 @@
       </c>
       <c r="I166" s="30"/>
     </row>
-    <row r="167" spans="1:9" ht="30">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="28" t="s">
         <v>815</v>
       </c>
@@ -9242,7 +9247,7 @@
       </c>
       <c r="I167" s="30"/>
     </row>
-    <row r="168" spans="1:9" ht="30">
+    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="28" t="s">
         <v>816</v>
       </c>
@@ -9267,7 +9272,7 @@
       </c>
       <c r="I168" s="30"/>
     </row>
-    <row r="169" spans="1:9" ht="30">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="28" t="s">
         <v>817</v>
       </c>
@@ -9292,7 +9297,7 @@
       </c>
       <c r="I169" s="30"/>
     </row>
-    <row r="170" spans="1:9" ht="30">
+    <row r="170" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="28" t="s">
         <v>818</v>
       </c>
@@ -9317,7 +9322,7 @@
       </c>
       <c r="I170" s="30"/>
     </row>
-    <row r="171" spans="1:9" ht="30">
+    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="28" t="s">
         <v>819</v>
       </c>
@@ -9342,7 +9347,7 @@
       </c>
       <c r="I171" s="30"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="28" t="s">
         <v>820</v>
       </c>
@@ -9367,7 +9372,7 @@
       </c>
       <c r="I172" s="30"/>
     </row>
-    <row r="173" spans="1:9" ht="30">
+    <row r="173" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="28" t="s">
         <v>821</v>
       </c>
@@ -9392,7 +9397,7 @@
       </c>
       <c r="I173" s="30"/>
     </row>
-    <row r="174" spans="1:9" ht="30">
+    <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="28" t="s">
         <v>822</v>
       </c>
@@ -9417,7 +9422,7 @@
       </c>
       <c r="I174" s="30"/>
     </row>
-    <row r="175" spans="1:9" ht="30">
+    <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="28" t="s">
         <v>161</v>
       </c>
@@ -9442,7 +9447,7 @@
       </c>
       <c r="I175" s="30"/>
     </row>
-    <row r="176" spans="1:9" ht="30">
+    <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="28" t="s">
         <v>162</v>
       </c>
@@ -9467,7 +9472,7 @@
       </c>
       <c r="I176" s="30"/>
     </row>
-    <row r="177" spans="1:9" ht="210">
+    <row r="177" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A177" s="28" t="s">
         <v>163</v>
       </c>
@@ -9492,7 +9497,7 @@
       </c>
       <c r="I177" s="30"/>
     </row>
-    <row r="178" spans="1:9" ht="45">
+    <row r="178" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="28" t="s">
         <v>164</v>
       </c>
@@ -9517,7 +9522,7 @@
       </c>
       <c r="I178" s="30"/>
     </row>
-    <row r="179" spans="1:9" ht="30">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="28" t="s">
         <v>165</v>
       </c>
@@ -9542,7 +9547,7 @@
       </c>
       <c r="I179" s="30"/>
     </row>
-    <row r="180" spans="1:9" ht="30">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="28" t="s">
         <v>166</v>
       </c>
@@ -9567,7 +9572,7 @@
       </c>
       <c r="I180" s="30"/>
     </row>
-    <row r="181" spans="1:9" ht="30">
+    <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="28" t="s">
         <v>167</v>
       </c>
@@ -9592,7 +9597,7 @@
       </c>
       <c r="I181" s="30"/>
     </row>
-    <row r="182" spans="1:9" ht="30">
+    <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="28" t="s">
         <v>180</v>
       </c>
@@ -9617,7 +9622,7 @@
       </c>
       <c r="I182" s="30"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="28" t="s">
         <v>181</v>
       </c>
@@ -9642,7 +9647,7 @@
       </c>
       <c r="I183" s="30"/>
     </row>
-    <row r="184" spans="1:9" ht="30">
+    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="28" t="s">
         <v>182</v>
       </c>
@@ -9667,7 +9672,7 @@
       </c>
       <c r="I184" s="30"/>
     </row>
-    <row r="185" spans="1:9" ht="30">
+    <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="28" t="s">
         <v>183</v>
       </c>
@@ -9692,7 +9697,7 @@
       </c>
       <c r="I185" s="30"/>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="28" t="s">
         <v>184</v>
       </c>
@@ -9717,7 +9722,7 @@
       </c>
       <c r="I186" s="30"/>
     </row>
-    <row r="187" spans="1:9" ht="30">
+    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="28" t="s">
         <v>185</v>
       </c>
@@ -9742,7 +9747,7 @@
       </c>
       <c r="I187" s="30"/>
     </row>
-    <row r="188" spans="1:9" ht="30">
+    <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="28" t="s">
         <v>186</v>
       </c>
@@ -9767,7 +9772,7 @@
       </c>
       <c r="I188" s="30"/>
     </row>
-    <row r="189" spans="1:9" ht="45">
+    <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="28" t="s">
         <v>187</v>
       </c>
@@ -9792,7 +9797,7 @@
       </c>
       <c r="I189" s="30"/>
     </row>
-    <row r="190" spans="1:9" ht="45">
+    <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="28" t="s">
         <v>188</v>
       </c>
@@ -9817,7 +9822,7 @@
       </c>
       <c r="I190" s="30"/>
     </row>
-    <row r="191" spans="1:9" ht="45">
+    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="28" t="s">
         <v>189</v>
       </c>
@@ -9842,7 +9847,7 @@
       </c>
       <c r="I191" s="30"/>
     </row>
-    <row r="192" spans="1:9" ht="45">
+    <row r="192" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="28" t="s">
         <v>190</v>
       </c>
@@ -9867,7 +9872,7 @@
       </c>
       <c r="I192" s="30"/>
     </row>
-    <row r="193" spans="1:9" ht="45">
+    <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="28" t="s">
         <v>191</v>
       </c>
@@ -9892,7 +9897,7 @@
       </c>
       <c r="I193" s="30"/>
     </row>
-    <row r="194" spans="1:9" ht="60">
+    <row r="194" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="28" t="s">
         <v>192</v>
       </c>
@@ -9917,7 +9922,7 @@
       </c>
       <c r="I194" s="30"/>
     </row>
-    <row r="195" spans="1:9" ht="30">
+    <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="28" t="s">
         <v>193</v>
       </c>
@@ -9942,7 +9947,7 @@
       </c>
       <c r="I195" s="30"/>
     </row>
-    <row r="196" spans="1:9" ht="60">
+    <row r="196" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="28" t="s">
         <v>194</v>
       </c>
@@ -9967,7 +9972,7 @@
       </c>
       <c r="I196" s="30"/>
     </row>
-    <row r="197" spans="1:9" ht="30">
+    <row r="197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="28" t="s">
         <v>195</v>
       </c>
@@ -9992,7 +9997,7 @@
       </c>
       <c r="I197" s="30"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
+    <row r="198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="28" t="s">
         <v>196</v>
       </c>
@@ -10017,7 +10022,7 @@
       </c>
       <c r="I198" s="30"/>
     </row>
-    <row r="199" spans="1:9" ht="30">
+    <row r="199" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="28" t="s">
         <v>197</v>
       </c>
@@ -10042,7 +10047,7 @@
       </c>
       <c r="I199" s="30"/>
     </row>
-    <row r="200" spans="1:9" ht="30">
+    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="28" t="s">
         <v>198</v>
       </c>
@@ -10067,7 +10072,7 @@
       </c>
       <c r="I200" s="30"/>
     </row>
-    <row r="201" spans="1:9" ht="30">
+    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="28" t="s">
         <v>199</v>
       </c>
@@ -10092,7 +10097,7 @@
       </c>
       <c r="I201" s="30"/>
     </row>
-    <row r="202" spans="1:9" ht="90">
+    <row r="202" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A202" s="28" t="s">
         <v>200</v>
       </c>
@@ -10117,7 +10122,7 @@
       </c>
       <c r="I202" s="30"/>
     </row>
-    <row r="203" spans="1:9" ht="345">
+    <row r="203" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A203" s="28" t="s">
         <v>201</v>
       </c>
@@ -10142,7 +10147,7 @@
       </c>
       <c r="I203" s="30"/>
     </row>
-    <row r="204" spans="1:9" ht="30">
+    <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="28" t="s">
         <v>202</v>
       </c>
@@ -10167,7 +10172,7 @@
       </c>
       <c r="I204" s="30"/>
     </row>
-    <row r="205" spans="1:9" ht="30">
+    <row r="205" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="28" t="s">
         <v>203</v>
       </c>
@@ -10192,7 +10197,7 @@
       </c>
       <c r="I205" s="30"/>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="28" t="s">
         <v>204</v>
       </c>
@@ -10217,7 +10222,7 @@
       </c>
       <c r="I206" s="30"/>
     </row>
-    <row r="207" spans="1:9" ht="45">
+    <row r="207" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="28" t="s">
         <v>205</v>
       </c>
@@ -10244,7 +10249,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="30">
+    <row r="208" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="28" t="s">
         <v>206</v>
       </c>
@@ -10271,7 +10276,7 @@
       </c>
       <c r="I208" s="30"/>
     </row>
-    <row r="209" spans="1:9" ht="30">
+    <row r="209" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="28" t="s">
         <v>207</v>
       </c>
@@ -10296,7 +10301,7 @@
       </c>
       <c r="I209" s="30"/>
     </row>
-    <row r="210" spans="1:9" ht="45">
+    <row r="210" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="28" t="s">
         <v>210</v>
       </c>
@@ -10321,7 +10326,7 @@
       </c>
       <c r="I210" s="30"/>
     </row>
-    <row r="211" spans="1:9" ht="30">
+    <row r="211" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="28" t="s">
         <v>211</v>
       </c>
@@ -10346,7 +10351,7 @@
       </c>
       <c r="I211" s="30"/>
     </row>
-    <row r="212" spans="1:9" ht="30">
+    <row r="212" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="28" t="s">
         <v>212</v>
       </c>
@@ -10371,7 +10376,7 @@
       </c>
       <c r="I212" s="30"/>
     </row>
-    <row r="213" spans="1:9" ht="135">
+    <row r="213" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A213" s="28" t="s">
         <v>213</v>
       </c>
@@ -10396,7 +10401,7 @@
       </c>
       <c r="I213" s="30"/>
     </row>
-    <row r="214" spans="1:9" ht="45">
+    <row r="214" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="28" t="s">
         <v>214</v>
       </c>
@@ -10421,7 +10426,7 @@
       </c>
       <c r="I214" s="30"/>
     </row>
-    <row r="215" spans="1:9" ht="45">
+    <row r="215" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="28" t="s">
         <v>215</v>
       </c>
@@ -10446,7 +10451,7 @@
       </c>
       <c r="I215" s="30"/>
     </row>
-    <row r="216" spans="1:9" ht="30">
+    <row r="216" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="28" t="s">
         <v>216</v>
       </c>
@@ -10471,7 +10476,7 @@
       </c>
       <c r="I216" s="30"/>
     </row>
-    <row r="217" spans="1:9" ht="30">
+    <row r="217" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="28" t="s">
         <v>217</v>
       </c>
@@ -10496,7 +10501,7 @@
       </c>
       <c r="I217" s="30"/>
     </row>
-    <row r="218" spans="1:9" ht="30">
+    <row r="218" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="28" t="s">
         <v>218</v>
       </c>
@@ -10521,7 +10526,7 @@
       </c>
       <c r="I218" s="30"/>
     </row>
-    <row r="219" spans="1:9" ht="30">
+    <row r="219" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="28" t="s">
         <v>219</v>
       </c>
@@ -10546,7 +10551,7 @@
       </c>
       <c r="I219" s="30"/>
     </row>
-    <row r="220" spans="1:9" ht="30">
+    <row r="220" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="28" t="s">
         <v>220</v>
       </c>
@@ -10571,7 +10576,7 @@
       </c>
       <c r="I220" s="30"/>
     </row>
-    <row r="221" spans="1:9" ht="30">
+    <row r="221" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="28" t="s">
         <v>221</v>
       </c>
@@ -10596,7 +10601,7 @@
       </c>
       <c r="I221" s="30"/>
     </row>
-    <row r="222" spans="1:9" ht="30">
+    <row r="222" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="28" t="s">
         <v>222</v>
       </c>
@@ -10621,7 +10626,7 @@
       </c>
       <c r="I222" s="30"/>
     </row>
-    <row r="223" spans="1:9" ht="30">
+    <row r="223" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="28" t="s">
         <v>223</v>
       </c>
@@ -10646,7 +10651,7 @@
       </c>
       <c r="I223" s="30"/>
     </row>
-    <row r="224" spans="1:9" ht="30">
+    <row r="224" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="28" t="s">
         <v>224</v>
       </c>
@@ -10671,7 +10676,7 @@
       </c>
       <c r="I224" s="30"/>
     </row>
-    <row r="225" spans="1:9" ht="30">
+    <row r="225" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="28" t="s">
         <v>225</v>
       </c>
@@ -10696,7 +10701,7 @@
       </c>
       <c r="I225" s="30"/>
     </row>
-    <row r="226" spans="1:9" ht="30">
+    <row r="226" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="28" t="s">
         <v>226</v>
       </c>
@@ -10721,7 +10726,7 @@
       </c>
       <c r="I226" s="30"/>
     </row>
-    <row r="227" spans="1:9" ht="120">
+    <row r="227" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A227" s="28" t="s">
         <v>227</v>
       </c>
@@ -10746,7 +10751,7 @@
       </c>
       <c r="I227" s="30"/>
     </row>
-    <row r="228" spans="1:9" ht="45">
+    <row r="228" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A228" s="28" t="s">
         <v>228</v>
       </c>
@@ -10771,7 +10776,7 @@
       </c>
       <c r="I228" s="30"/>
     </row>
-    <row r="229" spans="1:9" ht="45">
+    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="28" t="s">
         <v>229</v>
       </c>
@@ -10796,7 +10801,7 @@
       </c>
       <c r="I229" s="30"/>
     </row>
-    <row r="230" spans="1:9" ht="30">
+    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="28" t="s">
         <v>230</v>
       </c>
@@ -10821,7 +10826,7 @@
       </c>
       <c r="I230" s="30"/>
     </row>
-    <row r="231" spans="1:9" ht="30">
+    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="28" t="s">
         <v>231</v>
       </c>
@@ -10846,7 +10851,7 @@
       </c>
       <c r="I231" s="30"/>
     </row>
-    <row r="232" spans="1:9" ht="45">
+    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="28" t="s">
         <v>232</v>
       </c>
@@ -10854,7 +10859,7 @@
         <v>411</v>
       </c>
       <c r="C232" s="19" t="s">
-        <v>932</v>
+        <v>946</v>
       </c>
       <c r="D232" s="28"/>
       <c r="E232" s="28" t="s">
@@ -10871,7 +10876,7 @@
       </c>
       <c r="I232" s="30"/>
     </row>
-    <row r="233" spans="1:9" ht="30">
+    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="28" t="s">
         <v>233</v>
       </c>
@@ -10896,7 +10901,7 @@
       </c>
       <c r="I233" s="30"/>
     </row>
-    <row r="234" spans="1:9" ht="45">
+    <row r="234" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A234" s="28" t="s">
         <v>208</v>
       </c>
@@ -10921,7 +10926,7 @@
       </c>
       <c r="I234" s="30"/>
     </row>
-    <row r="235" spans="1:9" ht="45">
+    <row r="235" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A235" s="28" t="s">
         <v>209</v>
       </c>
@@ -10946,7 +10951,7 @@
       </c>
       <c r="I235" s="30"/>
     </row>
-    <row r="236" spans="1:9" ht="45">
+    <row r="236" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="28" t="s">
         <v>855</v>
       </c>
@@ -10971,7 +10976,7 @@
       </c>
       <c r="I236" s="30"/>
     </row>
-    <row r="237" spans="1:9" ht="60">
+    <row r="237" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A237" s="28" t="s">
         <v>856</v>
       </c>
@@ -10996,7 +11001,7 @@
       </c>
       <c r="I237" s="30"/>
     </row>
-    <row r="238" spans="1:9" ht="30">
+    <row r="238" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="28" t="s">
         <v>234</v>
       </c>
@@ -11021,7 +11026,7 @@
       </c>
       <c r="I238" s="30"/>
     </row>
-    <row r="239" spans="1:9" ht="30">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="28" t="s">
         <v>235</v>
       </c>
@@ -11046,7 +11051,7 @@
       </c>
       <c r="I239" s="30"/>
     </row>
-    <row r="240" spans="1:9" ht="30">
+    <row r="240" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="28" t="s">
         <v>236</v>
       </c>
@@ -11071,7 +11076,7 @@
       </c>
       <c r="I240" s="30"/>
     </row>
-    <row r="241" spans="1:9" ht="75">
+    <row r="241" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A241" s="28" t="s">
         <v>237</v>
       </c>
@@ -11096,7 +11101,7 @@
       </c>
       <c r="I241" s="30"/>
     </row>
-    <row r="242" spans="1:9" ht="75">
+    <row r="242" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A242" s="28" t="s">
         <v>238</v>
       </c>
@@ -11121,7 +11126,7 @@
       </c>
       <c r="I242" s="30"/>
     </row>
-    <row r="243" spans="1:9" ht="45">
+    <row r="243" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A243" s="28" t="s">
         <v>239</v>
       </c>
@@ -11146,7 +11151,7 @@
       </c>
       <c r="I243" s="30"/>
     </row>
-    <row r="244" spans="1:9" ht="30">
+    <row r="244" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="28" t="s">
         <v>240</v>
       </c>
@@ -11171,7 +11176,7 @@
       </c>
       <c r="I244" s="30"/>
     </row>
-    <row r="245" spans="1:9" ht="30">
+    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="28" t="s">
         <v>241</v>
       </c>
@@ -11196,7 +11201,7 @@
       </c>
       <c r="I245" s="30"/>
     </row>
-    <row r="246" spans="1:9" ht="45">
+    <row r="246" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="28" t="s">
         <v>242</v>
       </c>
@@ -11221,7 +11226,7 @@
       </c>
       <c r="I246" s="30"/>
     </row>
-    <row r="247" spans="1:9" ht="45">
+    <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="28" t="s">
         <v>243</v>
       </c>
@@ -11246,7 +11251,7 @@
       </c>
       <c r="I247" s="30"/>
     </row>
-    <row r="248" spans="1:9" ht="135">
+    <row r="248" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A248" s="28" t="s">
         <v>244</v>
       </c>
@@ -11271,7 +11276,7 @@
       </c>
       <c r="I248" s="30"/>
     </row>
-    <row r="249" spans="1:9" ht="45">
+    <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="28" t="s">
         <v>245</v>
       </c>
@@ -11296,7 +11301,7 @@
       </c>
       <c r="I249" s="30"/>
     </row>
-    <row r="250" spans="1:9" ht="30">
+    <row r="250" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="28" t="s">
         <v>246</v>
       </c>
@@ -11321,7 +11326,7 @@
       </c>
       <c r="I250" s="30"/>
     </row>
-    <row r="251" spans="1:9" ht="270">
+    <row r="251" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A251" s="28" t="s">
         <v>247</v>
       </c>
@@ -11346,7 +11351,7 @@
       </c>
       <c r="I251" s="30"/>
     </row>
-    <row r="252" spans="1:9" ht="45">
+    <row r="252" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="28" t="s">
         <v>248</v>
       </c>
@@ -11371,7 +11376,7 @@
       </c>
       <c r="I252" s="30"/>
     </row>
-    <row r="253" spans="1:9" ht="30">
+    <row r="253" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" s="28" t="s">
         <v>249</v>
       </c>
@@ -11396,7 +11401,7 @@
       </c>
       <c r="I253" s="30"/>
     </row>
-    <row r="254" spans="1:9" ht="30">
+    <row r="254" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="28" t="s">
         <v>250</v>
       </c>
@@ -11421,7 +11426,7 @@
       </c>
       <c r="I254" s="30"/>
     </row>
-    <row r="255" spans="1:9" ht="30">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="28" t="s">
         <v>251</v>
       </c>
@@ -11446,7 +11451,7 @@
       </c>
       <c r="I255" s="30"/>
     </row>
-    <row r="256" spans="1:9" ht="30">
+    <row r="256" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="28" t="s">
         <v>252</v>
       </c>
@@ -11471,7 +11476,7 @@
       </c>
       <c r="I256" s="30"/>
     </row>
-    <row r="257" spans="1:9" ht="30">
+    <row r="257" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" s="28" t="s">
         <v>253</v>
       </c>
@@ -11496,7 +11501,7 @@
       </c>
       <c r="I257" s="30"/>
     </row>
-    <row r="258" spans="1:9" ht="30">
+    <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="28" t="s">
         <v>254</v>
       </c>
@@ -11521,7 +11526,7 @@
       </c>
       <c r="I258" s="30"/>
     </row>
-    <row r="259" spans="1:9" ht="30">
+    <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="28" t="s">
         <v>255</v>
       </c>
@@ -11546,7 +11551,7 @@
       </c>
       <c r="I259" s="30"/>
     </row>
-    <row r="260" spans="1:9" ht="90">
+    <row r="260" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A260" s="28" t="s">
         <v>256</v>
       </c>
@@ -11571,7 +11576,7 @@
       </c>
       <c r="I260" s="30"/>
     </row>
-    <row r="261" spans="1:9" ht="315">
+    <row r="261" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A261" s="28" t="s">
         <v>257</v>
       </c>
@@ -11596,7 +11601,7 @@
       </c>
       <c r="I261" s="30"/>
     </row>
-    <row r="262" spans="1:9" ht="30">
+    <row r="262" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="28" t="s">
         <v>258</v>
       </c>
@@ -11621,7 +11626,7 @@
       </c>
       <c r="I262" s="30"/>
     </row>
-    <row r="263" spans="1:9" ht="30">
+    <row r="263" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="28" t="s">
         <v>259</v>
       </c>
@@ -11646,7 +11651,7 @@
       </c>
       <c r="I263" s="30"/>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="28" t="s">
         <v>260</v>
       </c>
@@ -11671,7 +11676,7 @@
       </c>
       <c r="I264" s="30"/>
     </row>
-    <row r="265" spans="1:9" ht="45">
+    <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="28" t="s">
         <v>261</v>
       </c>
@@ -11698,7 +11703,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="30">
+    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="28" t="s">
         <v>262</v>
       </c>
@@ -11725,7 +11730,7 @@
       </c>
       <c r="I266" s="30"/>
     </row>
-    <row r="267" spans="1:9" ht="30">
+    <row r="267" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="28" t="s">
         <v>263</v>
       </c>
@@ -11750,7 +11755,7 @@
       </c>
       <c r="I267" s="30"/>
     </row>
-    <row r="268" spans="1:9" ht="30">
+    <row r="268" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="28" t="s">
         <v>264</v>
       </c>
@@ -11775,7 +11780,7 @@
       </c>
       <c r="I268" s="30"/>
     </row>
-    <row r="269" spans="1:9" ht="45">
+    <row r="269" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="28" t="s">
         <v>267</v>
       </c>
@@ -11800,7 +11805,7 @@
       </c>
       <c r="I269" s="30"/>
     </row>
-    <row r="270" spans="1:9" ht="30">
+    <row r="270" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="28" t="s">
         <v>268</v>
       </c>
@@ -11825,7 +11830,7 @@
       </c>
       <c r="I270" s="30"/>
     </row>
-    <row r="271" spans="1:9" ht="30">
+    <row r="271" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="28" t="s">
         <v>269</v>
       </c>
@@ -11850,7 +11855,7 @@
       </c>
       <c r="I271" s="30"/>
     </row>
-    <row r="272" spans="1:9" ht="120">
+    <row r="272" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A272" s="28" t="s">
         <v>270</v>
       </c>
@@ -11875,7 +11880,7 @@
       </c>
       <c r="I272" s="30"/>
     </row>
-    <row r="273" spans="1:9" ht="45">
+    <row r="273" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="28" t="s">
         <v>271</v>
       </c>
@@ -11900,7 +11905,7 @@
       </c>
       <c r="I273" s="30"/>
     </row>
-    <row r="274" spans="1:9" ht="45">
+    <row r="274" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A274" s="28" t="s">
         <v>272</v>
       </c>
@@ -11925,7 +11930,7 @@
       </c>
       <c r="I274" s="30"/>
     </row>
-    <row r="275" spans="1:9" ht="30">
+    <row r="275" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="28" t="s">
         <v>273</v>
       </c>
@@ -11950,7 +11955,7 @@
       </c>
       <c r="I275" s="30"/>
     </row>
-    <row r="276" spans="1:9" ht="30">
+    <row r="276" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="28" t="s">
         <v>274</v>
       </c>
@@ -11975,7 +11980,7 @@
       </c>
       <c r="I276" s="30"/>
     </row>
-    <row r="277" spans="1:9" ht="30">
+    <row r="277" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="28" t="s">
         <v>275</v>
       </c>
@@ -11983,7 +11988,7 @@
         <v>419</v>
       </c>
       <c r="C277" s="19" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D277" s="28"/>
       <c r="E277" s="28" t="s">
@@ -12000,7 +12005,7 @@
       </c>
       <c r="I277" s="30"/>
     </row>
-    <row r="278" spans="1:9" ht="30">
+    <row r="278" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="28" t="s">
         <v>276</v>
       </c>
@@ -12025,7 +12030,7 @@
       </c>
       <c r="I278" s="30"/>
     </row>
-    <row r="279" spans="1:9" ht="30">
+    <row r="279" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="28" t="s">
         <v>277</v>
       </c>
@@ -12033,7 +12038,7 @@
         <v>419</v>
       </c>
       <c r="C279" s="19" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D279" s="28"/>
       <c r="E279" s="28" t="s">
@@ -12050,7 +12055,7 @@
       </c>
       <c r="I279" s="30"/>
     </row>
-    <row r="280" spans="1:9" ht="30">
+    <row r="280" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A280" s="28" t="s">
         <v>278</v>
       </c>
@@ -12075,7 +12080,7 @@
       </c>
       <c r="I280" s="30"/>
     </row>
-    <row r="281" spans="1:9" ht="30">
+    <row r="281" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" s="28" t="s">
         <v>279</v>
       </c>
@@ -12100,7 +12105,7 @@
       </c>
       <c r="I281" s="30"/>
     </row>
-    <row r="282" spans="1:9" ht="30">
+    <row r="282" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="28" t="s">
         <v>280</v>
       </c>
@@ -12108,7 +12113,7 @@
         <v>419</v>
       </c>
       <c r="C282" s="19" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D282" s="28"/>
       <c r="E282" s="28" t="s">
@@ -12125,7 +12130,7 @@
       </c>
       <c r="I282" s="30"/>
     </row>
-    <row r="283" spans="1:9" ht="30">
+    <row r="283" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="28" t="s">
         <v>281</v>
       </c>
@@ -12150,7 +12155,7 @@
       </c>
       <c r="I283" s="30"/>
     </row>
-    <row r="284" spans="1:9" ht="120">
+    <row r="284" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A284" s="28" t="s">
         <v>282</v>
       </c>
@@ -12175,7 +12180,7 @@
       </c>
       <c r="I284" s="30"/>
     </row>
-    <row r="285" spans="1:9" ht="45">
+    <row r="285" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A285" s="28" t="s">
         <v>283</v>
       </c>
@@ -12200,7 +12205,7 @@
       </c>
       <c r="I285" s="30"/>
     </row>
-    <row r="286" spans="1:9" ht="45">
+    <row r="286" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="28" t="s">
         <v>284</v>
       </c>
@@ -12225,7 +12230,7 @@
       </c>
       <c r="I286" s="30"/>
     </row>
-    <row r="287" spans="1:9" ht="30">
+    <row r="287" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="28" t="s">
         <v>285</v>
       </c>
@@ -12250,7 +12255,7 @@
       </c>
       <c r="I287" s="30"/>
     </row>
-    <row r="288" spans="1:9" ht="30">
+    <row r="288" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="28" t="s">
         <v>286</v>
       </c>
@@ -12275,7 +12280,7 @@
       </c>
       <c r="I288" s="30"/>
     </row>
-    <row r="289" spans="1:9" ht="30">
+    <row r="289" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="28" t="s">
         <v>287</v>
       </c>
@@ -12283,7 +12288,7 @@
         <v>420</v>
       </c>
       <c r="C289" s="19" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D289" s="28"/>
       <c r="E289" s="28" t="s">
@@ -12300,7 +12305,7 @@
       </c>
       <c r="I289" s="30"/>
     </row>
-    <row r="290" spans="1:9" ht="30">
+    <row r="290" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="28" t="s">
         <v>288</v>
       </c>
@@ -12325,7 +12330,7 @@
       </c>
       <c r="I290" s="30"/>
     </row>
-    <row r="291" spans="1:9" ht="45">
+    <row r="291" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A291" s="28" t="s">
         <v>265</v>
       </c>
@@ -12350,7 +12355,7 @@
       </c>
       <c r="I291" s="30"/>
     </row>
-    <row r="292" spans="1:9" ht="45">
+    <row r="292" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A292" s="28" t="s">
         <v>266</v>
       </c>
@@ -12375,7 +12380,7 @@
       </c>
       <c r="I292" s="30"/>
     </row>
-    <row r="293" spans="1:9" ht="45">
+    <row r="293" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A293" s="28" t="s">
         <v>835</v>
       </c>
@@ -12400,7 +12405,7 @@
       </c>
       <c r="I293" s="30"/>
     </row>
-    <row r="294" spans="1:9" ht="60">
+    <row r="294" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A294" s="28" t="s">
         <v>836</v>
       </c>
@@ -12425,7 +12430,7 @@
       </c>
       <c r="I294" s="30"/>
     </row>
-    <row r="295" spans="1:9" ht="45">
+    <row r="295" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="28" t="s">
         <v>289</v>
       </c>
@@ -12450,7 +12455,7 @@
       </c>
       <c r="I295" s="30"/>
     </row>
-    <row r="296" spans="1:9" ht="30">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="28" t="s">
         <v>290</v>
       </c>
@@ -12475,7 +12480,7 @@
       </c>
       <c r="I296" s="30"/>
     </row>
-    <row r="297" spans="1:9" ht="30">
+    <row r="297" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="28" t="s">
         <v>291</v>
       </c>
@@ -12500,7 +12505,7 @@
       </c>
       <c r="I297" s="30"/>
     </row>
-    <row r="298" spans="1:9" ht="30">
+    <row r="298" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="28" t="s">
         <v>292</v>
       </c>
@@ -12525,7 +12530,7 @@
       </c>
       <c r="I298" s="30"/>
     </row>
-    <row r="299" spans="1:9" ht="60">
+    <row r="299" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A299" s="28" t="s">
         <v>293</v>
       </c>
@@ -12550,7 +12555,7 @@
       </c>
       <c r="I299" s="30"/>
     </row>
-    <row r="300" spans="1:9" ht="75">
+    <row r="300" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A300" s="28" t="s">
         <v>294</v>
       </c>
@@ -12575,7 +12580,7 @@
       </c>
       <c r="I300" s="30"/>
     </row>
-    <row r="301" spans="1:9" ht="45">
+    <row r="301" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A301" s="28" t="s">
         <v>295</v>
       </c>
@@ -12600,7 +12605,7 @@
       </c>
       <c r="I301" s="30"/>
     </row>
-    <row r="302" spans="1:9" ht="30">
+    <row r="302" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A302" s="28" t="s">
         <v>296</v>
       </c>
@@ -12625,7 +12630,7 @@
       </c>
       <c r="I302" s="30"/>
     </row>
-    <row r="303" spans="1:9" ht="30">
+    <row r="303" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="28" t="s">
         <v>297</v>
       </c>
@@ -12650,7 +12655,7 @@
       </c>
       <c r="I303" s="30"/>
     </row>
-    <row r="304" spans="1:9" ht="30">
+    <row r="304" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A304" s="28" t="s">
         <v>298</v>
       </c>
@@ -12675,7 +12680,7 @@
       </c>
       <c r="I304" s="30"/>
     </row>
-    <row r="305" spans="1:9" ht="30">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" s="28" t="s">
         <v>838</v>
       </c>
@@ -12700,7 +12705,7 @@
       </c>
       <c r="I305" s="30"/>
     </row>
-    <row r="306" spans="1:9" ht="30">
+    <row r="306" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A306" s="28" t="s">
         <v>839</v>
       </c>
@@ -12725,7 +12730,7 @@
       </c>
       <c r="I306" s="30"/>
     </row>
-    <row r="307" spans="1:9" ht="45">
+    <row r="307" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A307" s="28" t="s">
         <v>299</v>
       </c>
@@ -12750,7 +12755,7 @@
       </c>
       <c r="I307" s="30"/>
     </row>
-    <row r="308" spans="1:9" ht="45">
+    <row r="308" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="28" t="s">
         <v>300</v>
       </c>
@@ -12775,7 +12780,7 @@
       </c>
       <c r="I308" s="30"/>
     </row>
-    <row r="309" spans="1:9" ht="240">
+    <row r="309" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A309" s="28" t="s">
         <v>301</v>
       </c>
@@ -12800,7 +12805,7 @@
       </c>
       <c r="I309" s="30"/>
     </row>
-    <row r="310" spans="1:9" ht="45">
+    <row r="310" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="28" t="s">
         <v>302</v>
       </c>
@@ -12825,7 +12830,7 @@
       </c>
       <c r="I310" s="30"/>
     </row>
-    <row r="311" spans="1:9" ht="30">
+    <row r="311" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A311" s="28" t="s">
         <v>303</v>
       </c>
@@ -12850,7 +12855,7 @@
       </c>
       <c r="I311" s="30"/>
     </row>
-    <row r="312" spans="1:9" ht="30">
+    <row r="312" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A312" s="28" t="s">
         <v>304</v>
       </c>
@@ -12875,7 +12880,7 @@
       </c>
       <c r="I312" s="30"/>
     </row>
-    <row r="313" spans="1:9" ht="45">
+    <row r="313" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A313" s="28" t="s">
         <v>305</v>
       </c>
@@ -12900,7 +12905,7 @@
       </c>
       <c r="I313" s="30"/>
     </row>
-    <row r="314" spans="1:9" ht="45">
+    <row r="314" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A314" s="28" t="s">
         <v>306</v>
       </c>
@@ -12925,7 +12930,7 @@
       </c>
       <c r="I314" s="30"/>
     </row>
-    <row r="315" spans="1:9" ht="135">
+    <row r="315" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A315" s="28" t="s">
         <v>307</v>
       </c>
@@ -12950,7 +12955,7 @@
       </c>
       <c r="I315" s="30"/>
     </row>
-    <row r="316" spans="1:9" ht="30">
+    <row r="316" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A316" s="28" t="s">
         <v>308</v>
       </c>
@@ -12975,7 +12980,7 @@
       </c>
       <c r="I316" s="30"/>
     </row>
-    <row r="317" spans="1:9" ht="30">
+    <row r="317" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A317" s="28" t="s">
         <v>309</v>
       </c>
@@ -13000,7 +13005,7 @@
       </c>
       <c r="I317" s="30"/>
     </row>
-    <row r="318" spans="1:9" ht="225">
+    <row r="318" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A318" s="28" t="s">
         <v>310</v>
       </c>
@@ -13025,7 +13030,7 @@
       </c>
       <c r="I318" s="30"/>
     </row>
-    <row r="319" spans="1:9" ht="30">
+    <row r="319" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A319" s="28" t="s">
         <v>311</v>
       </c>
@@ -13050,7 +13055,7 @@
       </c>
       <c r="I319" s="30"/>
     </row>
-    <row r="320" spans="1:9" ht="30">
+    <row r="320" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A320" s="28" t="s">
         <v>312</v>
       </c>
@@ -13075,7 +13080,7 @@
       </c>
       <c r="I320" s="30"/>
     </row>
-    <row r="321" spans="1:9" ht="30">
+    <row r="321" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A321" s="28" t="s">
         <v>313</v>
       </c>
@@ -13100,7 +13105,7 @@
       </c>
       <c r="I321" s="30"/>
     </row>
-    <row r="322" spans="1:9" ht="30">
+    <row r="322" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A322" s="28" t="s">
         <v>168</v>
       </c>
@@ -13125,7 +13130,7 @@
       </c>
       <c r="I322" s="30"/>
     </row>
-    <row r="323" spans="1:9" ht="30">
+    <row r="323" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A323" s="28" t="s">
         <v>169</v>
       </c>
@@ -13150,7 +13155,7 @@
       </c>
       <c r="I323" s="30"/>
     </row>
-    <row r="324" spans="1:9" ht="255">
+    <row r="324" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A324" s="28" t="s">
         <v>170</v>
       </c>
@@ -13175,7 +13180,7 @@
       </c>
       <c r="I324" s="30"/>
     </row>
-    <row r="325" spans="1:9" ht="45">
+    <row r="325" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A325" s="28" t="s">
         <v>171</v>
       </c>
@@ -13200,7 +13205,7 @@
       </c>
       <c r="I325" s="30"/>
     </row>
-    <row r="326" spans="1:9" ht="30">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" s="28" t="s">
         <v>172</v>
       </c>
@@ -13225,7 +13230,7 @@
       </c>
       <c r="I326" s="30"/>
     </row>
-    <row r="327" spans="1:9" ht="30">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" s="28" t="s">
         <v>173</v>
       </c>
@@ -13250,7 +13255,7 @@
       </c>
       <c r="I327" s="30"/>
     </row>
-    <row r="328" spans="1:9" ht="45">
+    <row r="328" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A328" s="28" t="s">
         <v>174</v>
       </c>
@@ -13277,7 +13282,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="329" spans="1:9" ht="30">
+    <row r="329" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A329" s="28" t="s">
         <v>175</v>
       </c>
@@ -13304,7 +13309,7 @@
       </c>
       <c r="I329" s="30"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" s="28" t="s">
         <v>176</v>
       </c>
@@ -13329,7 +13334,7 @@
       </c>
       <c r="I330" s="30"/>
     </row>
-    <row r="331" spans="1:9" ht="30">
+    <row r="331" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A331" s="28" t="s">
         <v>177</v>
       </c>
@@ -13354,7 +13359,7 @@
       </c>
       <c r="I331" s="30"/>
     </row>
-    <row r="332" spans="1:9" ht="45">
+    <row r="332" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A332" s="28" t="s">
         <v>178</v>
       </c>
@@ -13381,7 +13386,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="333" spans="1:9" ht="30">
+    <row r="333" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A333" s="28" t="s">
         <v>179</v>
       </c>
@@ -13408,7 +13413,7 @@
       </c>
       <c r="I333" s="30"/>
     </row>
-    <row r="334" spans="1:9" ht="30">
+    <row r="334" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A334" s="28" t="s">
         <v>314</v>
       </c>
@@ -13433,7 +13438,7 @@
       </c>
       <c r="I334" s="30"/>
     </row>
-    <row r="335" spans="1:9" ht="90">
+    <row r="335" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A335" s="28" t="s">
         <v>315</v>
       </c>
@@ -13458,7 +13463,7 @@
       </c>
       <c r="I335" s="30"/>
     </row>
-    <row r="336" spans="1:9" ht="345">
+    <row r="336" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A336" s="28" t="s">
         <v>316</v>
       </c>
@@ -13483,7 +13488,7 @@
       </c>
       <c r="I336" s="30"/>
     </row>
-    <row r="337" spans="1:9" ht="30">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" s="28" t="s">
         <v>317</v>
       </c>
@@ -13508,7 +13513,7 @@
       </c>
       <c r="I337" s="30"/>
     </row>
-    <row r="338" spans="1:9" ht="30">
+    <row r="338" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A338" s="28" t="s">
         <v>318</v>
       </c>
@@ -13533,7 +13538,7 @@
       </c>
       <c r="I338" s="30"/>
     </row>
-    <row r="339" spans="1:9" ht="45">
+    <row r="339" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A339" s="28" t="s">
         <v>321</v>
       </c>
@@ -13558,7 +13563,7 @@
       </c>
       <c r="I339" s="30"/>
     </row>
-    <row r="340" spans="1:9" ht="30">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="28" t="s">
         <v>322</v>
       </c>
@@ -13583,7 +13588,7 @@
       </c>
       <c r="I340" s="30"/>
     </row>
-    <row r="341" spans="1:9" ht="30">
+    <row r="341" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A341" s="28" t="s">
         <v>323</v>
       </c>
@@ -13608,7 +13613,7 @@
       </c>
       <c r="I341" s="30"/>
     </row>
-    <row r="342" spans="1:9" ht="135">
+    <row r="342" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A342" s="28" t="s">
         <v>324</v>
       </c>
@@ -13633,7 +13638,7 @@
       </c>
       <c r="I342" s="30"/>
     </row>
-    <row r="343" spans="1:9" ht="45">
+    <row r="343" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A343" s="28" t="s">
         <v>325</v>
       </c>
@@ -13658,7 +13663,7 @@
       </c>
       <c r="I343" s="30"/>
     </row>
-    <row r="344" spans="1:9" ht="45">
+    <row r="344" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A344" s="28" t="s">
         <v>326</v>
       </c>
@@ -13683,7 +13688,7 @@
       </c>
       <c r="I344" s="30"/>
     </row>
-    <row r="345" spans="1:9" ht="30">
+    <row r="345" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A345" s="28" t="s">
         <v>327</v>
       </c>
@@ -13708,7 +13713,7 @@
       </c>
       <c r="I345" s="30"/>
     </row>
-    <row r="346" spans="1:9" ht="30">
+    <row r="346" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A346" s="28" t="s">
         <v>328</v>
       </c>
@@ -13733,7 +13738,7 @@
       </c>
       <c r="I346" s="30"/>
     </row>
-    <row r="347" spans="1:9" ht="30">
+    <row r="347" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A347" s="28" t="s">
         <v>329</v>
       </c>
@@ -13741,7 +13746,7 @@
         <v>430</v>
       </c>
       <c r="C347" s="19" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D347" s="28"/>
       <c r="E347" s="28" t="s">
@@ -13758,7 +13763,7 @@
       </c>
       <c r="I347" s="30"/>
     </row>
-    <row r="348" spans="1:9" ht="30">
+    <row r="348" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A348" s="28" t="s">
         <v>330</v>
       </c>
@@ -13783,7 +13788,7 @@
       </c>
       <c r="I348" s="30"/>
     </row>
-    <row r="349" spans="1:9" ht="30">
+    <row r="349" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A349" s="28" t="s">
         <v>331</v>
       </c>
@@ -13791,7 +13796,7 @@
         <v>430</v>
       </c>
       <c r="C349" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D349" s="28"/>
       <c r="E349" s="28" t="s">
@@ -13808,7 +13813,7 @@
       </c>
       <c r="I349" s="30"/>
     </row>
-    <row r="350" spans="1:9" ht="30">
+    <row r="350" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A350" s="28" t="s">
         <v>332</v>
       </c>
@@ -13833,7 +13838,7 @@
       </c>
       <c r="I350" s="30"/>
     </row>
-    <row r="351" spans="1:9" ht="30">
+    <row r="351" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A351" s="28" t="s">
         <v>333</v>
       </c>
@@ -13858,7 +13863,7 @@
       </c>
       <c r="I351" s="30"/>
     </row>
-    <row r="352" spans="1:9" ht="30">
+    <row r="352" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A352" s="28" t="s">
         <v>334</v>
       </c>
@@ -13866,7 +13871,7 @@
         <v>430</v>
       </c>
       <c r="C352" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D352" s="28"/>
       <c r="E352" s="28" t="s">
@@ -13883,7 +13888,7 @@
       </c>
       <c r="I352" s="30"/>
     </row>
-    <row r="353" spans="1:9" ht="30">
+    <row r="353" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A353" s="28" t="s">
         <v>335</v>
       </c>
@@ -13908,7 +13913,7 @@
       </c>
       <c r="I353" s="30"/>
     </row>
-    <row r="354" spans="1:9" ht="30">
+    <row r="354" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A354" s="28" t="s">
         <v>336</v>
       </c>
@@ -13933,7 +13938,7 @@
       </c>
       <c r="I354" s="30"/>
     </row>
-    <row r="355" spans="1:9" ht="30">
+    <row r="355" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A355" s="28" t="s">
         <v>337</v>
       </c>
@@ -13958,7 +13963,7 @@
       </c>
       <c r="I355" s="30"/>
     </row>
-    <row r="356" spans="1:9" ht="90">
+    <row r="356" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A356" s="28" t="s">
         <v>338</v>
       </c>
@@ -13983,7 +13988,7 @@
       </c>
       <c r="I356" s="30"/>
     </row>
-    <row r="357" spans="1:9" ht="45">
+    <row r="357" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A357" s="28" t="s">
         <v>339</v>
       </c>
@@ -14008,7 +14013,7 @@
       </c>
       <c r="I357" s="30"/>
     </row>
-    <row r="358" spans="1:9" ht="45">
+    <row r="358" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A358" s="28" t="s">
         <v>340</v>
       </c>
@@ -14033,7 +14038,7 @@
       </c>
       <c r="I358" s="30"/>
     </row>
-    <row r="359" spans="1:9" ht="30">
+    <row r="359" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A359" s="28" t="s">
         <v>341</v>
       </c>
@@ -14058,7 +14063,7 @@
       </c>
       <c r="I359" s="30"/>
     </row>
-    <row r="360" spans="1:9" ht="30">
+    <row r="360" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A360" s="28" t="s">
         <v>342</v>
       </c>
@@ -14083,7 +14088,7 @@
       </c>
       <c r="I360" s="30"/>
     </row>
-    <row r="361" spans="1:9" ht="30">
+    <row r="361" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A361" s="28" t="s">
         <v>343</v>
       </c>
@@ -14091,7 +14096,7 @@
         <v>431</v>
       </c>
       <c r="C361" s="19" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D361" s="28"/>
       <c r="E361" s="28" t="s">
@@ -14108,7 +14113,7 @@
       </c>
       <c r="I361" s="30"/>
     </row>
-    <row r="362" spans="1:9" ht="30">
+    <row r="362" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A362" s="28" t="s">
         <v>344</v>
       </c>
@@ -14133,7 +14138,7 @@
       </c>
       <c r="I362" s="30"/>
     </row>
-    <row r="363" spans="1:9" ht="45">
+    <row r="363" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A363" s="28" t="s">
         <v>319</v>
       </c>
@@ -14158,7 +14163,7 @@
       </c>
       <c r="I363" s="30"/>
     </row>
-    <row r="364" spans="1:9" ht="45">
+    <row r="364" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A364" s="28" t="s">
         <v>320</v>
       </c>
@@ -14183,7 +14188,7 @@
       </c>
       <c r="I364" s="30"/>
     </row>
-    <row r="365" spans="1:9" ht="45">
+    <row r="365" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A365" s="28" t="s">
         <v>850</v>
       </c>
@@ -14208,7 +14213,7 @@
       </c>
       <c r="I365" s="30"/>
     </row>
-    <row r="366" spans="1:9" ht="60">
+    <row r="366" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="28" t="s">
         <v>851</v>
       </c>
@@ -14233,7 +14238,7 @@
       </c>
       <c r="I366" s="30"/>
     </row>
-    <row r="367" spans="1:9" ht="45">
+    <row r="367" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A367" s="28" t="s">
         <v>345</v>
       </c>
@@ -14258,7 +14263,7 @@
       </c>
       <c r="I367" s="30"/>
     </row>
-    <row r="368" spans="1:9">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" s="28" t="s">
         <v>346</v>
       </c>
@@ -14283,7 +14288,7 @@
       </c>
       <c r="I368" s="30"/>
     </row>
-    <row r="369" spans="1:9" ht="30">
+    <row r="369" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A369" s="28" t="s">
         <v>347</v>
       </c>
@@ -14308,7 +14313,7 @@
       </c>
       <c r="I369" s="30"/>
     </row>
-    <row r="370" spans="1:9" ht="75">
+    <row r="370" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A370" s="28" t="s">
         <v>348</v>
       </c>
@@ -14333,7 +14338,7 @@
       </c>
       <c r="I370" s="30"/>
     </row>
-    <row r="371" spans="1:9" ht="75">
+    <row r="371" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A371" s="28" t="s">
         <v>349</v>
       </c>
@@ -14358,7 +14363,7 @@
       </c>
       <c r="I371" s="30"/>
     </row>
-    <row r="372" spans="1:9" ht="60">
+    <row r="372" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A372" s="28" t="s">
         <v>350</v>
       </c>
@@ -14383,7 +14388,7 @@
       </c>
       <c r="I372" s="30"/>
     </row>
-    <row r="373" spans="1:9" ht="30">
+    <row r="373" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A373" s="28" t="s">
         <v>351</v>
       </c>
@@ -14408,7 +14413,7 @@
       </c>
       <c r="I373" s="30"/>
     </row>
-    <row r="374" spans="1:9" ht="30">
+    <row r="374" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A374" s="28" t="s">
         <v>352</v>
       </c>
@@ -14433,7 +14438,7 @@
       </c>
       <c r="I374" s="30"/>
     </row>
-    <row r="375" spans="1:9" ht="30">
+    <row r="375" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A375" s="28" t="s">
         <v>353</v>
       </c>
@@ -14458,7 +14463,7 @@
       </c>
       <c r="I375" s="30"/>
     </row>
-    <row r="376" spans="1:9" ht="45">
+    <row r="376" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A376" s="28" t="s">
         <v>354</v>
       </c>
@@ -14483,7 +14488,7 @@
       </c>
       <c r="I376" s="30"/>
     </row>
-    <row r="377" spans="1:9" ht="150">
+    <row r="377" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A377" s="28" t="s">
         <v>355</v>
       </c>
@@ -14508,7 +14513,7 @@
       </c>
       <c r="I377" s="30"/>
     </row>
-    <row r="378" spans="1:9" ht="30">
+    <row r="378" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A378" s="28" t="s">
         <v>356</v>
       </c>
@@ -14533,7 +14538,7 @@
       </c>
       <c r="I378" s="30"/>
     </row>
-    <row r="379" spans="1:9" ht="285">
+    <row r="379" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A379" s="28" t="s">
         <v>357</v>
       </c>
@@ -14558,7 +14563,7 @@
       </c>
       <c r="I379" s="30"/>
     </row>
-    <row r="380" spans="1:9" ht="45">
+    <row r="380" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A380" s="28" t="s">
         <v>358</v>
       </c>
@@ -14583,7 +14588,7 @@
       </c>
       <c r="I380" s="30"/>
     </row>
-    <row r="381" spans="1:9" ht="30">
+    <row r="381" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A381" s="28" t="s">
         <v>359</v>
       </c>
@@ -14608,7 +14613,7 @@
       </c>
       <c r="I381" s="30"/>
     </row>
-    <row r="382" spans="1:9" ht="30">
+    <row r="382" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A382" s="28" t="s">
         <v>360</v>
       </c>
@@ -14633,7 +14638,7 @@
       </c>
       <c r="I382" s="30"/>
     </row>
-    <row r="383" spans="1:9" ht="30">
+    <row r="383" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A383" s="28" t="s">
         <v>361</v>
       </c>
@@ -14658,7 +14663,7 @@
       </c>
       <c r="I383" s="30"/>
     </row>
-    <row r="384" spans="1:9" ht="30">
+    <row r="384" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A384" s="28" t="s">
         <v>362</v>
       </c>
@@ -14683,7 +14688,7 @@
       </c>
       <c r="I384" s="30"/>
     </row>
-    <row r="385" spans="1:9" ht="345">
+    <row r="385" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A385" s="28" t="s">
         <v>363</v>
       </c>
@@ -14708,7 +14713,7 @@
       </c>
       <c r="I385" s="30"/>
     </row>
-    <row r="386" spans="1:9" ht="45">
+    <row r="386" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="28" t="s">
         <v>364</v>
       </c>
@@ -14733,7 +14738,7 @@
       </c>
       <c r="I386" s="30"/>
     </row>
-    <row r="387" spans="1:9" ht="30">
+    <row r="387" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A387" s="28" t="s">
         <v>365</v>
       </c>
@@ -14758,7 +14763,7 @@
       </c>
       <c r="I387" s="30"/>
     </row>
-    <row r="388" spans="1:9" ht="30">
+    <row r="388" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A388" s="28" t="s">
         <v>366</v>
       </c>
@@ -14783,7 +14788,7 @@
       </c>
       <c r="I388" s="30"/>
     </row>
-    <row r="389" spans="1:9" ht="90">
+    <row r="389" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" s="28" t="s">
         <v>367</v>
       </c>
@@ -14810,7 +14815,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="390" spans="1:9" ht="30">
+    <row r="390" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A390" s="28" t="s">
         <v>368</v>
       </c>
@@ -14837,7 +14842,7 @@
       </c>
       <c r="I390" s="30"/>
     </row>
-    <row r="391" spans="1:9" ht="30">
+    <row r="391" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A391" s="28" t="s">
         <v>373</v>
       </c>
@@ -14862,7 +14867,7 @@
       </c>
       <c r="I391" s="30"/>
     </row>
-    <row r="392" spans="1:9" ht="30">
+    <row r="392" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A392" s="28" t="s">
         <v>374</v>
       </c>
@@ -14887,7 +14892,7 @@
       </c>
       <c r="I392" s="30"/>
     </row>
-    <row r="393" spans="1:9" ht="45">
+    <row r="393" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A393" s="28" t="s">
         <v>375</v>
       </c>
@@ -14914,7 +14919,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="394" spans="1:9" ht="30">
+    <row r="394" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A394" s="28" t="s">
         <v>376</v>
       </c>
@@ -14939,7 +14944,7 @@
       </c>
       <c r="I394" s="30"/>
     </row>
-    <row r="395" spans="1:9" ht="45">
+    <row r="395" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A395" s="28" t="s">
         <v>873</v>
       </c>
@@ -14964,7 +14969,7 @@
       </c>
       <c r="I395" s="30"/>
     </row>
-    <row r="396" spans="1:9" ht="45">
+    <row r="396" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A396" s="28" t="s">
         <v>876</v>
       </c>
@@ -14991,7 +14996,7 @@
       </c>
       <c r="I396" s="30"/>
     </row>
-    <row r="397" spans="1:9" ht="30">
+    <row r="397" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A397" s="28" t="s">
         <v>377</v>
       </c>
@@ -15016,7 +15021,7 @@
       </c>
       <c r="I397" s="30"/>
     </row>
-    <row r="398" spans="1:9" ht="30">
+    <row r="398" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A398" s="28" t="s">
         <v>378</v>
       </c>
@@ -15041,7 +15046,7 @@
       </c>
       <c r="I398" s="30"/>
     </row>
-    <row r="399" spans="1:9" ht="45">
+    <row r="399" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A399" s="28" t="s">
         <v>379</v>
       </c>
@@ -15049,7 +15054,7 @@
         <v>439</v>
       </c>
       <c r="C399" s="19" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
       <c r="D399" s="28"/>
       <c r="E399" s="28" t="s">
@@ -15066,7 +15071,7 @@
       </c>
       <c r="I399" s="30"/>
     </row>
-    <row r="400" spans="1:9" ht="30">
+    <row r="400" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A400" s="28" t="s">
         <v>380</v>
       </c>
@@ -15074,7 +15079,7 @@
         <v>439</v>
       </c>
       <c r="C400" s="19" t="s">
-        <v>942</v>
+        <v>949</v>
       </c>
       <c r="D400" s="28"/>
       <c r="E400" s="28" t="s">
@@ -15091,7 +15096,7 @@
       </c>
       <c r="I400" s="30"/>
     </row>
-    <row r="401" spans="1:9" ht="45">
+    <row r="401" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A401" s="28" t="s">
         <v>381</v>
       </c>
@@ -15120,7 +15125,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="402" spans="1:9" ht="75">
+    <row r="402" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A402" s="28" t="s">
         <v>766</v>
       </c>
@@ -15149,7 +15154,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="403" spans="1:9" ht="30">
+    <row r="403" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A403" s="28" t="s">
         <v>877</v>
       </c>
@@ -15176,7 +15181,7 @@
       </c>
       <c r="I403" s="30"/>
     </row>
-    <row r="404" spans="1:9" ht="45">
+    <row r="404" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A404" s="28" t="s">
         <v>878</v>
       </c>
@@ -15205,7 +15210,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="405" spans="1:9" ht="30">
+    <row r="405" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A405" s="28" t="s">
         <v>879</v>
       </c>
@@ -15232,7 +15237,7 @@
       </c>
       <c r="I405" s="19"/>
     </row>
-    <row r="406" spans="1:9" ht="45">
+    <row r="406" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A406" s="28" t="s">
         <v>880</v>
       </c>
@@ -15261,7 +15266,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="407" spans="1:9" ht="45">
+    <row r="407" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A407" s="28" t="s">
         <v>888</v>
       </c>
@@ -15290,7 +15295,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="408" spans="1:9" ht="30">
+    <row r="408" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A408" s="28" t="s">
         <v>920</v>
       </c>
@@ -15317,7 +15322,7 @@
       </c>
       <c r="I408" s="30"/>
     </row>
-    <row r="409" spans="1:9" ht="45">
+    <row r="409" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A409" s="28" t="s">
         <v>881</v>
       </c>
@@ -15344,7 +15349,7 @@
       </c>
       <c r="I409" s="19"/>
     </row>
-    <row r="410" spans="1:9" ht="45">
+    <row r="410" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A410" s="28" t="s">
         <v>882</v>
       </c>
@@ -15352,7 +15357,7 @@
         <v>439</v>
       </c>
       <c r="C410" s="19" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="D410" s="21" t="s">
         <v>905</v>
@@ -15373,7 +15378,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="411" spans="1:9" ht="60">
+    <row r="411" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A411" s="28" t="s">
         <v>883</v>
       </c>
@@ -15400,7 +15405,7 @@
       </c>
       <c r="I411" s="30"/>
     </row>
-    <row r="412" spans="1:9" ht="45">
+    <row r="412" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A412" s="28" t="s">
         <v>884</v>
       </c>
@@ -15429,7 +15434,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="413" spans="1:9" ht="45">
+    <row r="413" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A413" s="28" t="s">
         <v>885</v>
       </c>
@@ -15456,7 +15461,7 @@
       </c>
       <c r="I413" s="30"/>
     </row>
-    <row r="414" spans="1:9" ht="45">
+    <row r="414" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A414" s="28" t="s">
         <v>886</v>
       </c>
@@ -15485,7 +15490,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="415" spans="1:9" ht="75">
+    <row r="415" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A415" s="28" t="s">
         <v>369</v>
       </c>
@@ -15514,7 +15519,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="416" spans="1:9" ht="75">
+    <row r="416" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A416" s="28" t="s">
         <v>370</v>
       </c>
@@ -15543,7 +15548,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="417" spans="1:9" ht="75">
+    <row r="417" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A417" s="28" t="s">
         <v>371</v>
       </c>
@@ -15572,7 +15577,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="418" spans="1:9" ht="105">
+    <row r="418" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A418" s="28" t="s">
         <v>372</v>
       </c>
@@ -15601,7 +15606,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="419" spans="1:9" ht="30">
+    <row r="419" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A419" s="21" t="s">
         <v>893</v>
       </c>
@@ -15628,15 +15633,15 @@
       </c>
       <c r="I419" s="30"/>
     </row>
-    <row r="420" spans="1:9" ht="45">
+    <row r="420" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A420" s="21" t="s">
         <v>382</v>
       </c>
       <c r="B420" s="23" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="C420" s="19" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="D420" s="28"/>
       <c r="E420" s="28" t="s">
@@ -15653,15 +15658,15 @@
       </c>
       <c r="I420" s="30"/>
     </row>
-    <row r="421" spans="1:9" ht="30">
+    <row r="421" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A421" s="28" t="s">
         <v>383</v>
       </c>
       <c r="B421" s="23" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="C421" s="19" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="D421" s="28"/>
       <c r="E421" s="28" t="s">
@@ -15678,12 +15683,12 @@
       </c>
       <c r="I421" s="30"/>
     </row>
-    <row r="422" spans="1:9" ht="360">
+    <row r="422" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A422" s="28" t="s">
         <v>384</v>
       </c>
       <c r="B422" s="23" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="C422" s="19" t="s">
         <v>712</v>
@@ -15703,27 +15708,27 @@
       </c>
       <c r="I422" s="30"/>
     </row>
-    <row r="423" spans="1:9">
+    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A423" s="3"/>
       <c r="B423" s="10"/>
     </row>
-    <row r="424" spans="1:9">
+    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A424" s="3"/>
       <c r="B424" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A126:I233 A125:H125 A20:I124 A396:I422">

</xml_diff>

<commit_message>
Update setup script Add new SHOLDMAY config for Exchange 2019 and update test suites for MS-OXWSATT
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFED12EB-1F41-4C47-B3B9-EC9D0D74B758}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E15836-AA0C-4E9A-90CD-D3E20730B277}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -3498,9 +3498,6 @@
     <t>[In tns:CreateAttachmentSoapIn Message][The type of RequestVersion part is] t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.9).</t>
   </si>
   <si>
-    <t>[In tns:CreateAttachmentSoapOut Message][The element of ServerVersion part is] t:ServerVersionInfo ([MS-OXWSCDATA] section 2.2.3.10                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                    ).</t>
-  </si>
-  <si>
     <t>[In tns:DeleteAttachmentSoapIn Message][The type of Impersonation part is] t:ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.3.3).</t>
   </si>
   <si>
@@ -3525,12 +3522,6 @@
     <t>[In tns:GetAttachmentSoapIn Message][The RequestVersion part is] t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.9)</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms "SHOULD" or "SHOULD NOT" implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Unless otherwise specified, the term "MAY" implies that the product does not follow the prescription.</t>
-  </si>
-  <si>
     <t>[In Appendix C: Product Behavior] Implementation does support the Person element. (Exchange 2016  and above follow this behavior).</t>
   </si>
   <si>
@@ -3543,13 +3534,26 @@
     <t>2.2.3.10</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Exchange2007 and Exchange2019.)</t>
-  </si>
-  <si>
     <t>2.2.4.50</t>
   </si>
   <si>
     <t>[In m:ResponseCodeType Simple Type] The value "ErrorUnsupportedMimeConversion" occurs when an attempt is made to retrieve  MIME content for an item other than a PostItemType, MessageType, or CalendarItemType object.</t>
+  </si>
+  <si>
+    <t>[In tns:CreateAttachmentSoapOut Message][The element of ServerVersion part is] t:ServerVersionInfo ([MS-OXWSCDATA] section 2.2.3.10).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Exchange2007 and Exchange2019 follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3557,14 +3561,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3769,7 +3773,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3807,7 +3811,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3848,8 +3852,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3861,27 +3865,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3906,6 +3889,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5136,26 +5140,26 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A413" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C420" sqref="C420"/>
+    <sheetView tabSelected="1" topLeftCell="A402" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C408" sqref="C408"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="21.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>735</v>
       </c>
@@ -5167,7 +5171,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>736</v>
       </c>
@@ -5181,7 +5185,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="37" t="s">
         <v>25</v>
@@ -5202,141 +5206,141 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="52" t="s">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="78.75" customHeight="1">
+    <row r="9" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="33.75" customHeight="1">
+    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="56" t="s">
         <v>738</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>737</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>8</v>
       </c>
@@ -5355,7 +5359,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>6</v>
       </c>
@@ -5374,7 +5378,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>7</v>
       </c>
@@ -5393,7 +5397,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>3</v>
       </c>
@@ -5412,59 +5416,59 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1">
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="64.5" customHeight="1">
+    <row r="17" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1">
+    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>739</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="30">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -5493,7 +5497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="22" customFormat="1" ht="60">
+    <row r="20" spans="1:13" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A20" s="21" t="s">
         <v>41</v>
       </c>
@@ -5519,7 +5523,7 @@
       <c r="I20" s="23"/>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:13" s="22" customFormat="1" ht="45">
+    <row r="21" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="21" t="s">
         <v>42</v>
       </c>
@@ -5545,7 +5549,7 @@
       <c r="I21" s="23"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="22" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="21" t="s">
         <v>43</v>
       </c>
@@ -5571,7 +5575,7 @@
       <c r="I22" s="23"/>
       <c r="J22" s="35"/>
     </row>
-    <row r="23" spans="1:13" s="22" customFormat="1">
+    <row r="23" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="21" t="s">
         <v>44</v>
       </c>
@@ -5597,7 +5601,7 @@
       <c r="I23" s="23"/>
       <c r="J23" s="35"/>
     </row>
-    <row r="24" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="24" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="21" t="s">
         <v>45</v>
       </c>
@@ -5623,7 +5627,7 @@
       <c r="I24" s="23"/>
       <c r="J24" s="35"/>
     </row>
-    <row r="25" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="25" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A25" s="21" t="s">
         <v>46</v>
       </c>
@@ -5649,7 +5653,7 @@
       <c r="I25" s="23"/>
       <c r="J25" s="35"/>
     </row>
-    <row r="26" spans="1:13" s="22" customFormat="1" ht="45">
+    <row r="26" spans="1:13" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A26" s="21" t="s">
         <v>47</v>
       </c>
@@ -5675,7 +5679,7 @@
       <c r="I26" s="23"/>
       <c r="J26" s="35"/>
     </row>
-    <row r="27" spans="1:13" s="22" customFormat="1">
+    <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="21" t="s">
         <v>48</v>
       </c>
@@ -5701,7 +5705,7 @@
       <c r="I27" s="23"/>
       <c r="J27" s="35"/>
     </row>
-    <row r="28" spans="1:13" s="22" customFormat="1">
+    <row r="28" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="21" t="s">
         <v>49</v>
       </c>
@@ -5727,7 +5731,7 @@
       <c r="I28" s="23"/>
       <c r="J28" s="35"/>
     </row>
-    <row r="29" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="29" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A29" s="21" t="s">
         <v>50</v>
       </c>
@@ -5753,7 +5757,7 @@
       <c r="I29" s="23"/>
       <c r="J29" s="35"/>
     </row>
-    <row r="30" spans="1:13" s="22" customFormat="1">
+    <row r="30" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A30" s="21" t="s">
         <v>743</v>
       </c>
@@ -5779,7 +5783,7 @@
       <c r="I30" s="30"/>
       <c r="J30" s="35"/>
     </row>
-    <row r="31" spans="1:13" s="22" customFormat="1" ht="45">
+    <row r="31" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A31" s="21" t="s">
         <v>51</v>
       </c>
@@ -5807,7 +5811,7 @@
       </c>
       <c r="J31" s="35"/>
     </row>
-    <row r="32" spans="1:13" s="22" customFormat="1" ht="30">
+    <row r="32" spans="1:13" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>52</v>
       </c>
@@ -5833,7 +5837,7 @@
       <c r="I32" s="23"/>
       <c r="J32" s="35"/>
     </row>
-    <row r="33" spans="1:10" s="22" customFormat="1" ht="45">
+    <row r="33" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="21" t="s">
         <v>53</v>
       </c>
@@ -5859,7 +5863,7 @@
       <c r="I33" s="23"/>
       <c r="J33" s="35"/>
     </row>
-    <row r="34" spans="1:10" s="22" customFormat="1" ht="45">
+    <row r="34" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A34" s="21" t="s">
         <v>54</v>
       </c>
@@ -5885,7 +5889,7 @@
       <c r="I34" s="23"/>
       <c r="J34" s="35"/>
     </row>
-    <row r="35" spans="1:10" ht="60">
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>55</v>
       </c>
@@ -5910,7 +5914,7 @@
       </c>
       <c r="I35" s="30"/>
     </row>
-    <row r="36" spans="1:10" ht="30">
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>56</v>
       </c>
@@ -5935,7 +5939,7 @@
       </c>
       <c r="I36" s="30"/>
     </row>
-    <row r="37" spans="1:10" ht="30">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>57</v>
       </c>
@@ -5960,7 +5964,7 @@
       </c>
       <c r="I37" s="30"/>
     </row>
-    <row r="38" spans="1:10" ht="30">
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>58</v>
       </c>
@@ -5985,7 +5989,7 @@
       </c>
       <c r="I38" s="30"/>
     </row>
-    <row r="39" spans="1:10" ht="30">
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>59</v>
       </c>
@@ -6010,7 +6014,7 @@
       </c>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:10" ht="30">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>745</v>
       </c>
@@ -6035,7 +6039,7 @@
       </c>
       <c r="I40" s="30"/>
     </row>
-    <row r="41" spans="1:10" ht="30">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>60</v>
       </c>
@@ -6060,7 +6064,7 @@
       </c>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" spans="1:10" ht="30">
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>748</v>
       </c>
@@ -6085,7 +6089,7 @@
       </c>
       <c r="I42" s="30"/>
     </row>
-    <row r="43" spans="1:10" ht="30">
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>61</v>
       </c>
@@ -6110,7 +6114,7 @@
       </c>
       <c r="I43" s="30"/>
     </row>
-    <row r="44" spans="1:10" ht="30">
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>62</v>
       </c>
@@ -6135,7 +6139,7 @@
       </c>
       <c r="I44" s="30"/>
     </row>
-    <row r="45" spans="1:10" ht="45">
+    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>63</v>
       </c>
@@ -6160,7 +6164,7 @@
       </c>
       <c r="I45" s="30"/>
     </row>
-    <row r="46" spans="1:10" ht="75">
+    <row r="46" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>64</v>
       </c>
@@ -6185,7 +6189,7 @@
       </c>
       <c r="I46" s="30"/>
     </row>
-    <row r="47" spans="1:10" ht="30">
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>65</v>
       </c>
@@ -6210,7 +6214,7 @@
       </c>
       <c r="I47" s="30"/>
     </row>
-    <row r="48" spans="1:10" ht="45">
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>66</v>
       </c>
@@ -6235,7 +6239,7 @@
       </c>
       <c r="I48" s="30"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>67</v>
       </c>
@@ -6260,7 +6264,7 @@
       </c>
       <c r="I49" s="30"/>
     </row>
-    <row r="50" spans="1:9" ht="30">
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>68</v>
       </c>
@@ -6285,7 +6289,7 @@
       </c>
       <c r="I50" s="30"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>69</v>
       </c>
@@ -6310,7 +6314,7 @@
       </c>
       <c r="I51" s="30"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>70</v>
       </c>
@@ -6335,7 +6339,7 @@
       </c>
       <c r="I52" s="30"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>71</v>
       </c>
@@ -6360,7 +6364,7 @@
       </c>
       <c r="I53" s="30"/>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>752</v>
       </c>
@@ -6385,7 +6389,7 @@
       </c>
       <c r="I54" s="30"/>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>72</v>
       </c>
@@ -6410,7 +6414,7 @@
       </c>
       <c r="I55" s="30"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>73</v>
       </c>
@@ -6435,7 +6439,7 @@
       </c>
       <c r="I56" s="30"/>
     </row>
-    <row r="57" spans="1:9" ht="45">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>74</v>
       </c>
@@ -6462,7 +6466,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>75</v>
       </c>
@@ -6489,7 +6493,7 @@
       </c>
       <c r="I58" s="30"/>
     </row>
-    <row r="59" spans="1:9" ht="270">
+    <row r="59" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
         <v>76</v>
       </c>
@@ -6514,7 +6518,7 @@
       </c>
       <c r="I59" s="30"/>
     </row>
-    <row r="60" spans="1:9" ht="45">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
         <v>77</v>
       </c>
@@ -6539,7 +6543,7 @@
       </c>
       <c r="I60" s="30"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
         <v>78</v>
       </c>
@@ -6564,7 +6568,7 @@
       </c>
       <c r="I61" s="30"/>
     </row>
-    <row r="62" spans="1:9" ht="30">
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="28" t="s">
         <v>79</v>
       </c>
@@ -6589,7 +6593,7 @@
       </c>
       <c r="I62" s="30"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>80</v>
       </c>
@@ -6614,7 +6618,7 @@
       </c>
       <c r="I63" s="30"/>
     </row>
-    <row r="64" spans="1:9" ht="30">
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="28" t="s">
         <v>81</v>
       </c>
@@ -6639,7 +6643,7 @@
       </c>
       <c r="I64" s="30"/>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
         <v>757</v>
       </c>
@@ -6664,7 +6668,7 @@
       </c>
       <c r="I65" s="30"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="28" t="s">
         <v>758</v>
       </c>
@@ -6689,7 +6693,7 @@
       </c>
       <c r="I66" s="30"/>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
         <v>82</v>
       </c>
@@ -6714,7 +6718,7 @@
       </c>
       <c r="I67" s="30"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>83</v>
       </c>
@@ -6739,7 +6743,7 @@
       </c>
       <c r="I68" s="30"/>
     </row>
-    <row r="69" spans="1:9" ht="255">
+    <row r="69" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
         <v>84</v>
       </c>
@@ -6764,7 +6768,7 @@
       </c>
       <c r="I69" s="30"/>
     </row>
-    <row r="70" spans="1:9" ht="45">
+    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
         <v>85</v>
       </c>
@@ -6789,7 +6793,7 @@
       </c>
       <c r="I70" s="30"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
         <v>86</v>
       </c>
@@ -6814,7 +6818,7 @@
       </c>
       <c r="I71" s="30"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="28" t="s">
         <v>87</v>
       </c>
@@ -6839,7 +6843,7 @@
       </c>
       <c r="I72" s="30"/>
     </row>
-    <row r="73" spans="1:9" ht="30">
+    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="28" t="s">
         <v>902</v>
       </c>
@@ -6864,7 +6868,7 @@
       </c>
       <c r="I73" s="30"/>
     </row>
-    <row r="74" spans="1:9" ht="45">
+    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
         <v>88</v>
       </c>
@@ -6891,7 +6895,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="30">
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="28" t="s">
         <v>89</v>
       </c>
@@ -6918,7 +6922,7 @@
       </c>
       <c r="I75" s="30"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
         <v>90</v>
       </c>
@@ -6943,7 +6947,7 @@
       </c>
       <c r="I76" s="30"/>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>91</v>
       </c>
@@ -6968,7 +6972,7 @@
       </c>
       <c r="I77" s="30"/>
     </row>
-    <row r="78" spans="1:9" ht="45">
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>92</v>
       </c>
@@ -6995,7 +6999,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30">
+    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
         <v>93</v>
       </c>
@@ -7022,7 +7026,7 @@
       </c>
       <c r="I79" s="30"/>
     </row>
-    <row r="80" spans="1:9" ht="45">
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
         <v>94</v>
       </c>
@@ -7047,7 +7051,7 @@
       </c>
       <c r="I80" s="30"/>
     </row>
-    <row r="81" spans="1:9" ht="240">
+    <row r="81" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
         <v>95</v>
       </c>
@@ -7072,7 +7076,7 @@
       </c>
       <c r="I81" s="30"/>
     </row>
-    <row r="82" spans="1:9" ht="45">
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="28" t="s">
         <v>96</v>
       </c>
@@ -7097,7 +7101,7 @@
       </c>
       <c r="I82" s="30"/>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="28" t="s">
         <v>97</v>
       </c>
@@ -7122,7 +7126,7 @@
       </c>
       <c r="I83" s="30"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
         <v>98</v>
       </c>
@@ -7147,7 +7151,7 @@
       </c>
       <c r="I84" s="30"/>
     </row>
-    <row r="85" spans="1:9" ht="45">
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
         <v>99</v>
       </c>
@@ -7174,7 +7178,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
         <v>100</v>
       </c>
@@ -7201,7 +7205,7 @@
       </c>
       <c r="I86" s="30"/>
     </row>
-    <row r="87" spans="1:9" ht="409.5">
+    <row r="87" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
         <v>101</v>
       </c>
@@ -7226,7 +7230,7 @@
       </c>
       <c r="I87" s="30"/>
     </row>
-    <row r="88" spans="1:9" ht="45">
+    <row r="88" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
         <v>102</v>
       </c>
@@ -7251,7 +7255,7 @@
       </c>
       <c r="I88" s="30"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
         <v>103</v>
       </c>
@@ -7276,7 +7280,7 @@
       </c>
       <c r="I89" s="30"/>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
         <v>104</v>
       </c>
@@ -7301,7 +7305,7 @@
       </c>
       <c r="I90" s="30"/>
     </row>
-    <row r="91" spans="1:9" ht="30">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
         <v>105</v>
       </c>
@@ -7326,7 +7330,7 @@
       </c>
       <c r="I91" s="30"/>
     </row>
-    <row r="92" spans="1:9" ht="30">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
         <v>106</v>
       </c>
@@ -7351,7 +7355,7 @@
       </c>
       <c r="I92" s="30"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="28" t="s">
         <v>107</v>
       </c>
@@ -7376,7 +7380,7 @@
       </c>
       <c r="I93" s="30"/>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="28" t="s">
         <v>108</v>
       </c>
@@ -7401,7 +7405,7 @@
       </c>
       <c r="I94" s="30"/>
     </row>
-    <row r="95" spans="1:9" ht="45">
+    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="28" t="s">
         <v>109</v>
       </c>
@@ -7426,7 +7430,7 @@
       </c>
       <c r="I95" s="30"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="28" t="s">
         <v>110</v>
       </c>
@@ -7451,7 +7455,7 @@
       </c>
       <c r="I96" s="30"/>
     </row>
-    <row r="97" spans="1:9" ht="45">
+    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="28" t="s">
         <v>111</v>
       </c>
@@ -7478,7 +7482,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="28" t="s">
         <v>112</v>
       </c>
@@ -7505,7 +7509,7 @@
       </c>
       <c r="I98" s="30"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="28" t="s">
         <v>113</v>
       </c>
@@ -7530,7 +7534,7 @@
       </c>
       <c r="I99" s="30"/>
     </row>
-    <row r="100" spans="1:9" ht="30">
+    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="28" t="s">
         <v>114</v>
       </c>
@@ -7555,7 +7559,7 @@
       </c>
       <c r="I100" s="30"/>
     </row>
-    <row r="101" spans="1:9" ht="30">
+    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="28" t="s">
         <v>115</v>
       </c>
@@ -7580,7 +7584,7 @@
       </c>
       <c r="I101" s="30"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="28" t="s">
         <v>116</v>
       </c>
@@ -7605,7 +7609,7 @@
       </c>
       <c r="I102" s="30"/>
     </row>
-    <row r="103" spans="1:9" ht="30">
+    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="28" t="s">
         <v>117</v>
       </c>
@@ -7630,7 +7634,7 @@
       </c>
       <c r="I103" s="30"/>
     </row>
-    <row r="104" spans="1:9" ht="30">
+    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="28" t="s">
         <v>118</v>
       </c>
@@ -7655,7 +7659,7 @@
       </c>
       <c r="I104" s="30"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="28" t="s">
         <v>119</v>
       </c>
@@ -7680,7 +7684,7 @@
       </c>
       <c r="I105" s="30"/>
     </row>
-    <row r="106" spans="1:9" ht="45">
+    <row r="106" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="28" t="s">
         <v>120</v>
       </c>
@@ -7707,7 +7711,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="28" t="s">
         <v>121</v>
       </c>
@@ -7732,7 +7736,7 @@
       </c>
       <c r="I107" s="30"/>
     </row>
-    <row r="108" spans="1:9" ht="30">
+    <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="28" t="s">
         <v>122</v>
       </c>
@@ -7757,7 +7761,7 @@
       </c>
       <c r="I108" s="30"/>
     </row>
-    <row r="109" spans="1:9" ht="30">
+    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="28" t="s">
         <v>123</v>
       </c>
@@ -7782,7 +7786,7 @@
       </c>
       <c r="I109" s="30"/>
     </row>
-    <row r="110" spans="1:9" ht="30">
+    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="28" t="s">
         <v>124</v>
       </c>
@@ -7807,7 +7811,7 @@
       </c>
       <c r="I110" s="30"/>
     </row>
-    <row r="111" spans="1:9" ht="30">
+    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="28" t="s">
         <v>125</v>
       </c>
@@ -7832,7 +7836,7 @@
       </c>
       <c r="I111" s="30"/>
     </row>
-    <row r="112" spans="1:9" ht="330">
+    <row r="112" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A112" s="28" t="s">
         <v>126</v>
       </c>
@@ -7857,7 +7861,7 @@
       </c>
       <c r="I112" s="30"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="28" t="s">
         <v>127</v>
       </c>
@@ -7882,7 +7886,7 @@
       </c>
       <c r="I113" s="30"/>
     </row>
-    <row r="114" spans="1:9" ht="45">
+    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="28" t="s">
         <v>128</v>
       </c>
@@ -7909,7 +7913,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="30">
+    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="28" t="s">
         <v>129</v>
       </c>
@@ -7934,7 +7938,7 @@
       </c>
       <c r="I115" s="30"/>
     </row>
-    <row r="116" spans="1:9" ht="30">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="28" t="s">
         <v>130</v>
       </c>
@@ -7959,7 +7963,7 @@
       </c>
       <c r="I116" s="30"/>
     </row>
-    <row r="117" spans="1:9" ht="30">
+    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="28" t="s">
         <v>131</v>
       </c>
@@ -7984,7 +7988,7 @@
       </c>
       <c r="I117" s="30"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="28" t="s">
         <v>132</v>
       </c>
@@ -8009,7 +8013,7 @@
       </c>
       <c r="I118" s="30"/>
     </row>
-    <row r="119" spans="1:9" ht="30">
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="28" t="s">
         <v>133</v>
       </c>
@@ -8034,7 +8038,7 @@
       </c>
       <c r="I119" s="30"/>
     </row>
-    <row r="120" spans="1:9" ht="60">
+    <row r="120" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="28" t="s">
         <v>764</v>
       </c>
@@ -8061,7 +8065,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="45">
+    <row r="121" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="28" t="s">
         <v>765</v>
       </c>
@@ -8086,7 +8090,7 @@
       </c>
       <c r="I121" s="30"/>
     </row>
-    <row r="122" spans="1:9" ht="409.5">
+    <row r="122" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A122" s="28" t="s">
         <v>134</v>
       </c>
@@ -8111,7 +8115,7 @@
       </c>
       <c r="I122" s="30"/>
     </row>
-    <row r="123" spans="1:9" ht="60">
+    <row r="123" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="28" t="s">
         <v>135</v>
       </c>
@@ -8136,7 +8140,7 @@
       </c>
       <c r="I123" s="30"/>
     </row>
-    <row r="124" spans="1:9" ht="45">
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="28" t="s">
         <v>136</v>
       </c>
@@ -8163,7 +8167,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="30">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="28" t="s">
         <v>137</v>
       </c>
@@ -8188,7 +8192,7 @@
       </c>
       <c r="I125" s="30"/>
     </row>
-    <row r="126" spans="1:9" ht="30">
+    <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="28" t="s">
         <v>138</v>
       </c>
@@ -8213,7 +8217,7 @@
       </c>
       <c r="I126" s="30"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="28" t="s">
         <v>139</v>
       </c>
@@ -8238,7 +8242,7 @@
       </c>
       <c r="I127" s="30"/>
     </row>
-    <row r="128" spans="1:9" ht="30">
+    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="28" t="s">
         <v>140</v>
       </c>
@@ -8263,7 +8267,7 @@
       </c>
       <c r="I128" s="30"/>
     </row>
-    <row r="129" spans="1:9" ht="30">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="28" t="s">
         <v>141</v>
       </c>
@@ -8288,7 +8292,7 @@
       </c>
       <c r="I129" s="30"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="28" t="s">
         <v>142</v>
       </c>
@@ -8313,7 +8317,7 @@
       </c>
       <c r="I130" s="30"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="28" t="s">
         <v>143</v>
       </c>
@@ -8338,7 +8342,7 @@
       </c>
       <c r="I131" s="30"/>
     </row>
-    <row r="132" spans="1:9" ht="30">
+    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="28" t="s">
         <v>144</v>
       </c>
@@ -8363,7 +8367,7 @@
       </c>
       <c r="I132" s="30"/>
     </row>
-    <row r="133" spans="1:9" ht="30">
+    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="28" t="s">
         <v>145</v>
       </c>
@@ -8388,7 +8392,7 @@
       </c>
       <c r="I133" s="30"/>
     </row>
-    <row r="134" spans="1:9" ht="30">
+    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="28" t="s">
         <v>146</v>
       </c>
@@ -8413,7 +8417,7 @@
       </c>
       <c r="I134" s="30"/>
     </row>
-    <row r="135" spans="1:9" ht="30">
+    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="28" t="s">
         <v>147</v>
       </c>
@@ -8438,7 +8442,7 @@
       </c>
       <c r="I135" s="30"/>
     </row>
-    <row r="136" spans="1:9" ht="30">
+    <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="28" t="s">
         <v>148</v>
       </c>
@@ -8463,7 +8467,7 @@
       </c>
       <c r="I136" s="30"/>
     </row>
-    <row r="137" spans="1:9" ht="30">
+    <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="28" t="s">
         <v>149</v>
       </c>
@@ -8488,7 +8492,7 @@
       </c>
       <c r="I137" s="30"/>
     </row>
-    <row r="138" spans="1:9" ht="30">
+    <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="28" t="s">
         <v>150</v>
       </c>
@@ -8513,7 +8517,7 @@
       </c>
       <c r="I138" s="30"/>
     </row>
-    <row r="139" spans="1:9" ht="30">
+    <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="28" t="s">
         <v>151</v>
       </c>
@@ -8538,7 +8542,7 @@
       </c>
       <c r="I139" s="30"/>
     </row>
-    <row r="140" spans="1:9" ht="30">
+    <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="28" t="s">
         <v>152</v>
       </c>
@@ -8563,7 +8567,7 @@
       </c>
       <c r="I140" s="30"/>
     </row>
-    <row r="141" spans="1:9" ht="30">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="28" t="s">
         <v>153</v>
       </c>
@@ -8588,7 +8592,7 @@
       </c>
       <c r="I141" s="30"/>
     </row>
-    <row r="142" spans="1:9" ht="30">
+    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="28" t="s">
         <v>154</v>
       </c>
@@ -8613,7 +8617,7 @@
       </c>
       <c r="I142" s="30"/>
     </row>
-    <row r="143" spans="1:9" ht="30">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="28" t="s">
         <v>155</v>
       </c>
@@ -8638,7 +8642,7 @@
       </c>
       <c r="I143" s="30"/>
     </row>
-    <row r="144" spans="1:9" ht="30">
+    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="28" t="s">
         <v>779</v>
       </c>
@@ -8663,7 +8667,7 @@
       </c>
       <c r="I144" s="30"/>
     </row>
-    <row r="145" spans="1:9" ht="30">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="28" t="s">
         <v>780</v>
       </c>
@@ -8688,7 +8692,7 @@
       </c>
       <c r="I145" s="30"/>
     </row>
-    <row r="146" spans="1:9" ht="30">
+    <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="28" t="s">
         <v>781</v>
       </c>
@@ -8713,7 +8717,7 @@
       </c>
       <c r="I146" s="30"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="28" t="s">
         <v>782</v>
       </c>
@@ -8738,7 +8742,7 @@
       </c>
       <c r="I147" s="30"/>
     </row>
-    <row r="148" spans="1:9" ht="30">
+    <row r="148" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="28" t="s">
         <v>783</v>
       </c>
@@ -8763,7 +8767,7 @@
       </c>
       <c r="I148" s="30"/>
     </row>
-    <row r="149" spans="1:9" ht="45">
+    <row r="149" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="28" t="s">
         <v>784</v>
       </c>
@@ -8790,7 +8794,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="30">
+    <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="28" t="s">
         <v>785</v>
       </c>
@@ -8815,7 +8819,7 @@
       </c>
       <c r="I150" s="30"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="28" t="s">
         <v>786</v>
       </c>
@@ -8840,7 +8844,7 @@
       </c>
       <c r="I151" s="30"/>
     </row>
-    <row r="152" spans="1:9" ht="45">
+    <row r="152" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="28" t="s">
         <v>156</v>
       </c>
@@ -8865,7 +8869,7 @@
       </c>
       <c r="I152" s="30"/>
     </row>
-    <row r="153" spans="1:9" ht="180">
+    <row r="153" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A153" s="28" t="s">
         <v>157</v>
       </c>
@@ -8890,7 +8894,7 @@
       </c>
       <c r="I153" s="30"/>
     </row>
-    <row r="154" spans="1:9" ht="45">
+    <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="28" t="s">
         <v>158</v>
       </c>
@@ -8915,7 +8919,7 @@
       </c>
       <c r="I154" s="30"/>
     </row>
-    <row r="155" spans="1:9" ht="30">
+    <row r="155" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="28" t="s">
         <v>159</v>
       </c>
@@ -8940,7 +8944,7 @@
       </c>
       <c r="I155" s="30"/>
     </row>
-    <row r="156" spans="1:9" ht="30">
+    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="28" t="s">
         <v>160</v>
       </c>
@@ -8965,7 +8969,7 @@
       </c>
       <c r="I156" s="30"/>
     </row>
-    <row r="157" spans="1:9" ht="30">
+    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="28" t="s">
         <v>806</v>
       </c>
@@ -8990,7 +8994,7 @@
       </c>
       <c r="I157" s="30"/>
     </row>
-    <row r="158" spans="1:9" ht="45">
+    <row r="158" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="28" t="s">
         <v>807</v>
       </c>
@@ -9017,7 +9021,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="330">
+    <row r="159" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A159" s="28" t="s">
         <v>915</v>
       </c>
@@ -9042,7 +9046,7 @@
       </c>
       <c r="I159" s="30"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="28" t="s">
         <v>808</v>
       </c>
@@ -9067,7 +9071,7 @@
       </c>
       <c r="I160" s="30"/>
     </row>
-    <row r="161" spans="1:9" ht="30">
+    <row r="161" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="28" t="s">
         <v>809</v>
       </c>
@@ -9092,7 +9096,7 @@
       </c>
       <c r="I161" s="30"/>
     </row>
-    <row r="162" spans="1:9" ht="30">
+    <row r="162" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="28" t="s">
         <v>810</v>
       </c>
@@ -9117,7 +9121,7 @@
       </c>
       <c r="I162" s="30"/>
     </row>
-    <row r="163" spans="1:9" ht="30">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="28" t="s">
         <v>811</v>
       </c>
@@ -9142,7 +9146,7 @@
       </c>
       <c r="I163" s="30"/>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="28" t="s">
         <v>812</v>
       </c>
@@ -9167,7 +9171,7 @@
       </c>
       <c r="I164" s="30"/>
     </row>
-    <row r="165" spans="1:9" ht="30">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="28" t="s">
         <v>813</v>
       </c>
@@ -9192,7 +9196,7 @@
       </c>
       <c r="I165" s="30"/>
     </row>
-    <row r="166" spans="1:9" ht="30">
+    <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="28" t="s">
         <v>814</v>
       </c>
@@ -9217,7 +9221,7 @@
       </c>
       <c r="I166" s="30"/>
     </row>
-    <row r="167" spans="1:9" ht="30">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="28" t="s">
         <v>815</v>
       </c>
@@ -9242,7 +9246,7 @@
       </c>
       <c r="I167" s="30"/>
     </row>
-    <row r="168" spans="1:9" ht="30">
+    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="28" t="s">
         <v>816</v>
       </c>
@@ -9267,7 +9271,7 @@
       </c>
       <c r="I168" s="30"/>
     </row>
-    <row r="169" spans="1:9" ht="30">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="28" t="s">
         <v>817</v>
       </c>
@@ -9292,7 +9296,7 @@
       </c>
       <c r="I169" s="30"/>
     </row>
-    <row r="170" spans="1:9" ht="30">
+    <row r="170" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="28" t="s">
         <v>818</v>
       </c>
@@ -9317,7 +9321,7 @@
       </c>
       <c r="I170" s="30"/>
     </row>
-    <row r="171" spans="1:9" ht="30">
+    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="28" t="s">
         <v>819</v>
       </c>
@@ -9342,7 +9346,7 @@
       </c>
       <c r="I171" s="30"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="28" t="s">
         <v>820</v>
       </c>
@@ -9367,7 +9371,7 @@
       </c>
       <c r="I172" s="30"/>
     </row>
-    <row r="173" spans="1:9" ht="30">
+    <row r="173" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="28" t="s">
         <v>821</v>
       </c>
@@ -9392,7 +9396,7 @@
       </c>
       <c r="I173" s="30"/>
     </row>
-    <row r="174" spans="1:9" ht="30">
+    <row r="174" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="28" t="s">
         <v>822</v>
       </c>
@@ -9417,7 +9421,7 @@
       </c>
       <c r="I174" s="30"/>
     </row>
-    <row r="175" spans="1:9" ht="30">
+    <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="28" t="s">
         <v>161</v>
       </c>
@@ -9442,7 +9446,7 @@
       </c>
       <c r="I175" s="30"/>
     </row>
-    <row r="176" spans="1:9" ht="30">
+    <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="28" t="s">
         <v>162</v>
       </c>
@@ -9467,7 +9471,7 @@
       </c>
       <c r="I176" s="30"/>
     </row>
-    <row r="177" spans="1:9" ht="210">
+    <row r="177" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A177" s="28" t="s">
         <v>163</v>
       </c>
@@ -9492,7 +9496,7 @@
       </c>
       <c r="I177" s="30"/>
     </row>
-    <row r="178" spans="1:9" ht="45">
+    <row r="178" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="28" t="s">
         <v>164</v>
       </c>
@@ -9517,7 +9521,7 @@
       </c>
       <c r="I178" s="30"/>
     </row>
-    <row r="179" spans="1:9" ht="30">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="28" t="s">
         <v>165</v>
       </c>
@@ -9542,7 +9546,7 @@
       </c>
       <c r="I179" s="30"/>
     </row>
-    <row r="180" spans="1:9" ht="30">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="28" t="s">
         <v>166</v>
       </c>
@@ -9567,7 +9571,7 @@
       </c>
       <c r="I180" s="30"/>
     </row>
-    <row r="181" spans="1:9" ht="30">
+    <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="28" t="s">
         <v>167</v>
       </c>
@@ -9592,7 +9596,7 @@
       </c>
       <c r="I181" s="30"/>
     </row>
-    <row r="182" spans="1:9" ht="30">
+    <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="28" t="s">
         <v>180</v>
       </c>
@@ -9617,7 +9621,7 @@
       </c>
       <c r="I182" s="30"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="28" t="s">
         <v>181</v>
       </c>
@@ -9642,7 +9646,7 @@
       </c>
       <c r="I183" s="30"/>
     </row>
-    <row r="184" spans="1:9" ht="30">
+    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="28" t="s">
         <v>182</v>
       </c>
@@ -9667,7 +9671,7 @@
       </c>
       <c r="I184" s="30"/>
     </row>
-    <row r="185" spans="1:9" ht="30">
+    <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="28" t="s">
         <v>183</v>
       </c>
@@ -9692,7 +9696,7 @@
       </c>
       <c r="I185" s="30"/>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="28" t="s">
         <v>184</v>
       </c>
@@ -9717,7 +9721,7 @@
       </c>
       <c r="I186" s="30"/>
     </row>
-    <row r="187" spans="1:9" ht="30">
+    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="28" t="s">
         <v>185</v>
       </c>
@@ -9742,7 +9746,7 @@
       </c>
       <c r="I187" s="30"/>
     </row>
-    <row r="188" spans="1:9" ht="30">
+    <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="28" t="s">
         <v>186</v>
       </c>
@@ -9767,7 +9771,7 @@
       </c>
       <c r="I188" s="30"/>
     </row>
-    <row r="189" spans="1:9" ht="45">
+    <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="28" t="s">
         <v>187</v>
       </c>
@@ -9792,7 +9796,7 @@
       </c>
       <c r="I189" s="30"/>
     </row>
-    <row r="190" spans="1:9" ht="45">
+    <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="28" t="s">
         <v>188</v>
       </c>
@@ -9817,7 +9821,7 @@
       </c>
       <c r="I190" s="30"/>
     </row>
-    <row r="191" spans="1:9" ht="45">
+    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="28" t="s">
         <v>189</v>
       </c>
@@ -9842,7 +9846,7 @@
       </c>
       <c r="I191" s="30"/>
     </row>
-    <row r="192" spans="1:9" ht="45">
+    <row r="192" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="28" t="s">
         <v>190</v>
       </c>
@@ -9867,7 +9871,7 @@
       </c>
       <c r="I192" s="30"/>
     </row>
-    <row r="193" spans="1:9" ht="45">
+    <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="28" t="s">
         <v>191</v>
       </c>
@@ -9892,7 +9896,7 @@
       </c>
       <c r="I193" s="30"/>
     </row>
-    <row r="194" spans="1:9" ht="60">
+    <row r="194" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="28" t="s">
         <v>192</v>
       </c>
@@ -9917,7 +9921,7 @@
       </c>
       <c r="I194" s="30"/>
     </row>
-    <row r="195" spans="1:9" ht="30">
+    <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="28" t="s">
         <v>193</v>
       </c>
@@ -9942,7 +9946,7 @@
       </c>
       <c r="I195" s="30"/>
     </row>
-    <row r="196" spans="1:9" ht="60">
+    <row r="196" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="28" t="s">
         <v>194</v>
       </c>
@@ -9967,7 +9971,7 @@
       </c>
       <c r="I196" s="30"/>
     </row>
-    <row r="197" spans="1:9" ht="30">
+    <row r="197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="28" t="s">
         <v>195</v>
       </c>
@@ -9992,7 +9996,7 @@
       </c>
       <c r="I197" s="30"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
+    <row r="198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="28" t="s">
         <v>196</v>
       </c>
@@ -10017,7 +10021,7 @@
       </c>
       <c r="I198" s="30"/>
     </row>
-    <row r="199" spans="1:9" ht="30">
+    <row r="199" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="28" t="s">
         <v>197</v>
       </c>
@@ -10042,7 +10046,7 @@
       </c>
       <c r="I199" s="30"/>
     </row>
-    <row r="200" spans="1:9" ht="30">
+    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="28" t="s">
         <v>198</v>
       </c>
@@ -10067,7 +10071,7 @@
       </c>
       <c r="I200" s="30"/>
     </row>
-    <row r="201" spans="1:9" ht="30">
+    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="28" t="s">
         <v>199</v>
       </c>
@@ -10092,7 +10096,7 @@
       </c>
       <c r="I201" s="30"/>
     </row>
-    <row r="202" spans="1:9" ht="90">
+    <row r="202" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A202" s="28" t="s">
         <v>200</v>
       </c>
@@ -10117,7 +10121,7 @@
       </c>
       <c r="I202" s="30"/>
     </row>
-    <row r="203" spans="1:9" ht="345">
+    <row r="203" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A203" s="28" t="s">
         <v>201</v>
       </c>
@@ -10142,7 +10146,7 @@
       </c>
       <c r="I203" s="30"/>
     </row>
-    <row r="204" spans="1:9" ht="30">
+    <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="28" t="s">
         <v>202</v>
       </c>
@@ -10167,7 +10171,7 @@
       </c>
       <c r="I204" s="30"/>
     </row>
-    <row r="205" spans="1:9" ht="30">
+    <row r="205" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="28" t="s">
         <v>203</v>
       </c>
@@ -10192,7 +10196,7 @@
       </c>
       <c r="I205" s="30"/>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="28" t="s">
         <v>204</v>
       </c>
@@ -10217,7 +10221,7 @@
       </c>
       <c r="I206" s="30"/>
     </row>
-    <row r="207" spans="1:9" ht="45">
+    <row r="207" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="28" t="s">
         <v>205</v>
       </c>
@@ -10244,7 +10248,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="30">
+    <row r="208" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="28" t="s">
         <v>206</v>
       </c>
@@ -10271,7 +10275,7 @@
       </c>
       <c r="I208" s="30"/>
     </row>
-    <row r="209" spans="1:9" ht="30">
+    <row r="209" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="28" t="s">
         <v>207</v>
       </c>
@@ -10296,7 +10300,7 @@
       </c>
       <c r="I209" s="30"/>
     </row>
-    <row r="210" spans="1:9" ht="45">
+    <row r="210" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="28" t="s">
         <v>210</v>
       </c>
@@ -10321,7 +10325,7 @@
       </c>
       <c r="I210" s="30"/>
     </row>
-    <row r="211" spans="1:9" ht="30">
+    <row r="211" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="28" t="s">
         <v>211</v>
       </c>
@@ -10346,7 +10350,7 @@
       </c>
       <c r="I211" s="30"/>
     </row>
-    <row r="212" spans="1:9" ht="30">
+    <row r="212" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="28" t="s">
         <v>212</v>
       </c>
@@ -10371,7 +10375,7 @@
       </c>
       <c r="I212" s="30"/>
     </row>
-    <row r="213" spans="1:9" ht="135">
+    <row r="213" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A213" s="28" t="s">
         <v>213</v>
       </c>
@@ -10396,7 +10400,7 @@
       </c>
       <c r="I213" s="30"/>
     </row>
-    <row r="214" spans="1:9" ht="45">
+    <row r="214" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="28" t="s">
         <v>214</v>
       </c>
@@ -10421,7 +10425,7 @@
       </c>
       <c r="I214" s="30"/>
     </row>
-    <row r="215" spans="1:9" ht="45">
+    <row r="215" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="28" t="s">
         <v>215</v>
       </c>
@@ -10446,7 +10450,7 @@
       </c>
       <c r="I215" s="30"/>
     </row>
-    <row r="216" spans="1:9" ht="30">
+    <row r="216" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="28" t="s">
         <v>216</v>
       </c>
@@ -10471,7 +10475,7 @@
       </c>
       <c r="I216" s="30"/>
     </row>
-    <row r="217" spans="1:9" ht="30">
+    <row r="217" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="28" t="s">
         <v>217</v>
       </c>
@@ -10496,7 +10500,7 @@
       </c>
       <c r="I217" s="30"/>
     </row>
-    <row r="218" spans="1:9" ht="30">
+    <row r="218" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="28" t="s">
         <v>218</v>
       </c>
@@ -10521,7 +10525,7 @@
       </c>
       <c r="I218" s="30"/>
     </row>
-    <row r="219" spans="1:9" ht="30">
+    <row r="219" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="28" t="s">
         <v>219</v>
       </c>
@@ -10546,7 +10550,7 @@
       </c>
       <c r="I219" s="30"/>
     </row>
-    <row r="220" spans="1:9" ht="30">
+    <row r="220" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="28" t="s">
         <v>220</v>
       </c>
@@ -10571,7 +10575,7 @@
       </c>
       <c r="I220" s="30"/>
     </row>
-    <row r="221" spans="1:9" ht="30">
+    <row r="221" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="28" t="s">
         <v>221</v>
       </c>
@@ -10596,7 +10600,7 @@
       </c>
       <c r="I221" s="30"/>
     </row>
-    <row r="222" spans="1:9" ht="30">
+    <row r="222" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="28" t="s">
         <v>222</v>
       </c>
@@ -10621,7 +10625,7 @@
       </c>
       <c r="I222" s="30"/>
     </row>
-    <row r="223" spans="1:9" ht="30">
+    <row r="223" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="28" t="s">
         <v>223</v>
       </c>
@@ -10646,7 +10650,7 @@
       </c>
       <c r="I223" s="30"/>
     </row>
-    <row r="224" spans="1:9" ht="30">
+    <row r="224" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="28" t="s">
         <v>224</v>
       </c>
@@ -10671,7 +10675,7 @@
       </c>
       <c r="I224" s="30"/>
     </row>
-    <row r="225" spans="1:9" ht="30">
+    <row r="225" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="28" t="s">
         <v>225</v>
       </c>
@@ -10696,7 +10700,7 @@
       </c>
       <c r="I225" s="30"/>
     </row>
-    <row r="226" spans="1:9" ht="30">
+    <row r="226" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="28" t="s">
         <v>226</v>
       </c>
@@ -10721,7 +10725,7 @@
       </c>
       <c r="I226" s="30"/>
     </row>
-    <row r="227" spans="1:9" ht="120">
+    <row r="227" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A227" s="28" t="s">
         <v>227</v>
       </c>
@@ -10746,7 +10750,7 @@
       </c>
       <c r="I227" s="30"/>
     </row>
-    <row r="228" spans="1:9" ht="45">
+    <row r="228" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A228" s="28" t="s">
         <v>228</v>
       </c>
@@ -10771,7 +10775,7 @@
       </c>
       <c r="I228" s="30"/>
     </row>
-    <row r="229" spans="1:9" ht="45">
+    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="28" t="s">
         <v>229</v>
       </c>
@@ -10796,7 +10800,7 @@
       </c>
       <c r="I229" s="30"/>
     </row>
-    <row r="230" spans="1:9" ht="30">
+    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="28" t="s">
         <v>230</v>
       </c>
@@ -10821,7 +10825,7 @@
       </c>
       <c r="I230" s="30"/>
     </row>
-    <row r="231" spans="1:9" ht="30">
+    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="28" t="s">
         <v>231</v>
       </c>
@@ -10846,7 +10850,7 @@
       </c>
       <c r="I231" s="30"/>
     </row>
-    <row r="232" spans="1:9" ht="45">
+    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="28" t="s">
         <v>232</v>
       </c>
@@ -10854,7 +10858,7 @@
         <v>411</v>
       </c>
       <c r="C232" s="19" t="s">
-        <v>932</v>
+        <v>946</v>
       </c>
       <c r="D232" s="28"/>
       <c r="E232" s="28" t="s">
@@ -10871,7 +10875,7 @@
       </c>
       <c r="I232" s="30"/>
     </row>
-    <row r="233" spans="1:9" ht="30">
+    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="28" t="s">
         <v>233</v>
       </c>
@@ -10896,7 +10900,7 @@
       </c>
       <c r="I233" s="30"/>
     </row>
-    <row r="234" spans="1:9" ht="45">
+    <row r="234" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A234" s="28" t="s">
         <v>208</v>
       </c>
@@ -10921,7 +10925,7 @@
       </c>
       <c r="I234" s="30"/>
     </row>
-    <row r="235" spans="1:9" ht="45">
+    <row r="235" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A235" s="28" t="s">
         <v>209</v>
       </c>
@@ -10946,7 +10950,7 @@
       </c>
       <c r="I235" s="30"/>
     </row>
-    <row r="236" spans="1:9" ht="45">
+    <row r="236" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="28" t="s">
         <v>855</v>
       </c>
@@ -10971,7 +10975,7 @@
       </c>
       <c r="I236" s="30"/>
     </row>
-    <row r="237" spans="1:9" ht="60">
+    <row r="237" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A237" s="28" t="s">
         <v>856</v>
       </c>
@@ -10996,7 +11000,7 @@
       </c>
       <c r="I237" s="30"/>
     </row>
-    <row r="238" spans="1:9" ht="30">
+    <row r="238" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="28" t="s">
         <v>234</v>
       </c>
@@ -11021,7 +11025,7 @@
       </c>
       <c r="I238" s="30"/>
     </row>
-    <row r="239" spans="1:9" ht="30">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="28" t="s">
         <v>235</v>
       </c>
@@ -11046,7 +11050,7 @@
       </c>
       <c r="I239" s="30"/>
     </row>
-    <row r="240" spans="1:9" ht="30">
+    <row r="240" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="28" t="s">
         <v>236</v>
       </c>
@@ -11071,7 +11075,7 @@
       </c>
       <c r="I240" s="30"/>
     </row>
-    <row r="241" spans="1:9" ht="75">
+    <row r="241" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A241" s="28" t="s">
         <v>237</v>
       </c>
@@ -11096,7 +11100,7 @@
       </c>
       <c r="I241" s="30"/>
     </row>
-    <row r="242" spans="1:9" ht="75">
+    <row r="242" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A242" s="28" t="s">
         <v>238</v>
       </c>
@@ -11121,7 +11125,7 @@
       </c>
       <c r="I242" s="30"/>
     </row>
-    <row r="243" spans="1:9" ht="45">
+    <row r="243" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A243" s="28" t="s">
         <v>239</v>
       </c>
@@ -11146,7 +11150,7 @@
       </c>
       <c r="I243" s="30"/>
     </row>
-    <row r="244" spans="1:9" ht="30">
+    <row r="244" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="28" t="s">
         <v>240</v>
       </c>
@@ -11171,7 +11175,7 @@
       </c>
       <c r="I244" s="30"/>
     </row>
-    <row r="245" spans="1:9" ht="30">
+    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="28" t="s">
         <v>241</v>
       </c>
@@ -11196,7 +11200,7 @@
       </c>
       <c r="I245" s="30"/>
     </row>
-    <row r="246" spans="1:9" ht="45">
+    <row r="246" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="28" t="s">
         <v>242</v>
       </c>
@@ -11221,7 +11225,7 @@
       </c>
       <c r="I246" s="30"/>
     </row>
-    <row r="247" spans="1:9" ht="45">
+    <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="28" t="s">
         <v>243</v>
       </c>
@@ -11246,7 +11250,7 @@
       </c>
       <c r="I247" s="30"/>
     </row>
-    <row r="248" spans="1:9" ht="135">
+    <row r="248" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A248" s="28" t="s">
         <v>244</v>
       </c>
@@ -11271,7 +11275,7 @@
       </c>
       <c r="I248" s="30"/>
     </row>
-    <row r="249" spans="1:9" ht="45">
+    <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="28" t="s">
         <v>245</v>
       </c>
@@ -11296,7 +11300,7 @@
       </c>
       <c r="I249" s="30"/>
     </row>
-    <row r="250" spans="1:9" ht="30">
+    <row r="250" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="28" t="s">
         <v>246</v>
       </c>
@@ -11321,7 +11325,7 @@
       </c>
       <c r="I250" s="30"/>
     </row>
-    <row r="251" spans="1:9" ht="270">
+    <row r="251" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A251" s="28" t="s">
         <v>247</v>
       </c>
@@ -11346,7 +11350,7 @@
       </c>
       <c r="I251" s="30"/>
     </row>
-    <row r="252" spans="1:9" ht="45">
+    <row r="252" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="28" t="s">
         <v>248</v>
       </c>
@@ -11371,7 +11375,7 @@
       </c>
       <c r="I252" s="30"/>
     </row>
-    <row r="253" spans="1:9" ht="30">
+    <row r="253" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" s="28" t="s">
         <v>249</v>
       </c>
@@ -11396,7 +11400,7 @@
       </c>
       <c r="I253" s="30"/>
     </row>
-    <row r="254" spans="1:9" ht="30">
+    <row r="254" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="28" t="s">
         <v>250</v>
       </c>
@@ -11421,7 +11425,7 @@
       </c>
       <c r="I254" s="30"/>
     </row>
-    <row r="255" spans="1:9" ht="30">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="28" t="s">
         <v>251</v>
       </c>
@@ -11446,7 +11450,7 @@
       </c>
       <c r="I255" s="30"/>
     </row>
-    <row r="256" spans="1:9" ht="30">
+    <row r="256" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="28" t="s">
         <v>252</v>
       </c>
@@ -11471,7 +11475,7 @@
       </c>
       <c r="I256" s="30"/>
     </row>
-    <row r="257" spans="1:9" ht="30">
+    <row r="257" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" s="28" t="s">
         <v>253</v>
       </c>
@@ -11496,7 +11500,7 @@
       </c>
       <c r="I257" s="30"/>
     </row>
-    <row r="258" spans="1:9" ht="30">
+    <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="28" t="s">
         <v>254</v>
       </c>
@@ -11521,7 +11525,7 @@
       </c>
       <c r="I258" s="30"/>
     </row>
-    <row r="259" spans="1:9" ht="30">
+    <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="28" t="s">
         <v>255</v>
       </c>
@@ -11546,7 +11550,7 @@
       </c>
       <c r="I259" s="30"/>
     </row>
-    <row r="260" spans="1:9" ht="90">
+    <row r="260" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A260" s="28" t="s">
         <v>256</v>
       </c>
@@ -11571,7 +11575,7 @@
       </c>
       <c r="I260" s="30"/>
     </row>
-    <row r="261" spans="1:9" ht="315">
+    <row r="261" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A261" s="28" t="s">
         <v>257</v>
       </c>
@@ -11596,7 +11600,7 @@
       </c>
       <c r="I261" s="30"/>
     </row>
-    <row r="262" spans="1:9" ht="30">
+    <row r="262" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="28" t="s">
         <v>258</v>
       </c>
@@ -11621,7 +11625,7 @@
       </c>
       <c r="I262" s="30"/>
     </row>
-    <row r="263" spans="1:9" ht="30">
+    <row r="263" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="28" t="s">
         <v>259</v>
       </c>
@@ -11646,7 +11650,7 @@
       </c>
       <c r="I263" s="30"/>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="28" t="s">
         <v>260</v>
       </c>
@@ -11671,7 +11675,7 @@
       </c>
       <c r="I264" s="30"/>
     </row>
-    <row r="265" spans="1:9" ht="45">
+    <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="28" t="s">
         <v>261</v>
       </c>
@@ -11698,7 +11702,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="30">
+    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="28" t="s">
         <v>262</v>
       </c>
@@ -11725,7 +11729,7 @@
       </c>
       <c r="I266" s="30"/>
     </row>
-    <row r="267" spans="1:9" ht="30">
+    <row r="267" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="28" t="s">
         <v>263</v>
       </c>
@@ -11750,7 +11754,7 @@
       </c>
       <c r="I267" s="30"/>
     </row>
-    <row r="268" spans="1:9" ht="30">
+    <row r="268" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="28" t="s">
         <v>264</v>
       </c>
@@ -11775,7 +11779,7 @@
       </c>
       <c r="I268" s="30"/>
     </row>
-    <row r="269" spans="1:9" ht="45">
+    <row r="269" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="28" t="s">
         <v>267</v>
       </c>
@@ -11800,7 +11804,7 @@
       </c>
       <c r="I269" s="30"/>
     </row>
-    <row r="270" spans="1:9" ht="30">
+    <row r="270" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="28" t="s">
         <v>268</v>
       </c>
@@ -11825,7 +11829,7 @@
       </c>
       <c r="I270" s="30"/>
     </row>
-    <row r="271" spans="1:9" ht="30">
+    <row r="271" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="28" t="s">
         <v>269</v>
       </c>
@@ -11850,7 +11854,7 @@
       </c>
       <c r="I271" s="30"/>
     </row>
-    <row r="272" spans="1:9" ht="120">
+    <row r="272" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A272" s="28" t="s">
         <v>270</v>
       </c>
@@ -11875,7 +11879,7 @@
       </c>
       <c r="I272" s="30"/>
     </row>
-    <row r="273" spans="1:9" ht="45">
+    <row r="273" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="28" t="s">
         <v>271</v>
       </c>
@@ -11900,7 +11904,7 @@
       </c>
       <c r="I273" s="30"/>
     </row>
-    <row r="274" spans="1:9" ht="45">
+    <row r="274" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A274" s="28" t="s">
         <v>272</v>
       </c>
@@ -11925,7 +11929,7 @@
       </c>
       <c r="I274" s="30"/>
     </row>
-    <row r="275" spans="1:9" ht="30">
+    <row r="275" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="28" t="s">
         <v>273</v>
       </c>
@@ -11950,7 +11954,7 @@
       </c>
       <c r="I275" s="30"/>
     </row>
-    <row r="276" spans="1:9" ht="30">
+    <row r="276" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="28" t="s">
         <v>274</v>
       </c>
@@ -11975,7 +11979,7 @@
       </c>
       <c r="I276" s="30"/>
     </row>
-    <row r="277" spans="1:9" ht="30">
+    <row r="277" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="28" t="s">
         <v>275</v>
       </c>
@@ -11983,7 +11987,7 @@
         <v>419</v>
       </c>
       <c r="C277" s="19" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D277" s="28"/>
       <c r="E277" s="28" t="s">
@@ -12000,7 +12004,7 @@
       </c>
       <c r="I277" s="30"/>
     </row>
-    <row r="278" spans="1:9" ht="30">
+    <row r="278" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="28" t="s">
         <v>276</v>
       </c>
@@ -12025,7 +12029,7 @@
       </c>
       <c r="I278" s="30"/>
     </row>
-    <row r="279" spans="1:9" ht="30">
+    <row r="279" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="28" t="s">
         <v>277</v>
       </c>
@@ -12033,7 +12037,7 @@
         <v>419</v>
       </c>
       <c r="C279" s="19" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D279" s="28"/>
       <c r="E279" s="28" t="s">
@@ -12050,7 +12054,7 @@
       </c>
       <c r="I279" s="30"/>
     </row>
-    <row r="280" spans="1:9" ht="30">
+    <row r="280" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A280" s="28" t="s">
         <v>278</v>
       </c>
@@ -12075,7 +12079,7 @@
       </c>
       <c r="I280" s="30"/>
     </row>
-    <row r="281" spans="1:9" ht="30">
+    <row r="281" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" s="28" t="s">
         <v>279</v>
       </c>
@@ -12100,7 +12104,7 @@
       </c>
       <c r="I281" s="30"/>
     </row>
-    <row r="282" spans="1:9" ht="30">
+    <row r="282" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="28" t="s">
         <v>280</v>
       </c>
@@ -12108,7 +12112,7 @@
         <v>419</v>
       </c>
       <c r="C282" s="19" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D282" s="28"/>
       <c r="E282" s="28" t="s">
@@ -12125,7 +12129,7 @@
       </c>
       <c r="I282" s="30"/>
     </row>
-    <row r="283" spans="1:9" ht="30">
+    <row r="283" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="28" t="s">
         <v>281</v>
       </c>
@@ -12150,7 +12154,7 @@
       </c>
       <c r="I283" s="30"/>
     </row>
-    <row r="284" spans="1:9" ht="120">
+    <row r="284" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A284" s="28" t="s">
         <v>282</v>
       </c>
@@ -12175,7 +12179,7 @@
       </c>
       <c r="I284" s="30"/>
     </row>
-    <row r="285" spans="1:9" ht="45">
+    <row r="285" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A285" s="28" t="s">
         <v>283</v>
       </c>
@@ -12200,7 +12204,7 @@
       </c>
       <c r="I285" s="30"/>
     </row>
-    <row r="286" spans="1:9" ht="45">
+    <row r="286" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="28" t="s">
         <v>284</v>
       </c>
@@ -12225,7 +12229,7 @@
       </c>
       <c r="I286" s="30"/>
     </row>
-    <row r="287" spans="1:9" ht="30">
+    <row r="287" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="28" t="s">
         <v>285</v>
       </c>
@@ -12250,7 +12254,7 @@
       </c>
       <c r="I287" s="30"/>
     </row>
-    <row r="288" spans="1:9" ht="30">
+    <row r="288" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="28" t="s">
         <v>286</v>
       </c>
@@ -12275,7 +12279,7 @@
       </c>
       <c r="I288" s="30"/>
     </row>
-    <row r="289" spans="1:9" ht="30">
+    <row r="289" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="28" t="s">
         <v>287</v>
       </c>
@@ -12283,7 +12287,7 @@
         <v>420</v>
       </c>
       <c r="C289" s="19" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D289" s="28"/>
       <c r="E289" s="28" t="s">
@@ -12300,7 +12304,7 @@
       </c>
       <c r="I289" s="30"/>
     </row>
-    <row r="290" spans="1:9" ht="30">
+    <row r="290" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="28" t="s">
         <v>288</v>
       </c>
@@ -12325,7 +12329,7 @@
       </c>
       <c r="I290" s="30"/>
     </row>
-    <row r="291" spans="1:9" ht="45">
+    <row r="291" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A291" s="28" t="s">
         <v>265</v>
       </c>
@@ -12350,7 +12354,7 @@
       </c>
       <c r="I291" s="30"/>
     </row>
-    <row r="292" spans="1:9" ht="45">
+    <row r="292" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A292" s="28" t="s">
         <v>266</v>
       </c>
@@ -12375,7 +12379,7 @@
       </c>
       <c r="I292" s="30"/>
     </row>
-    <row r="293" spans="1:9" ht="45">
+    <row r="293" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A293" s="28" t="s">
         <v>835</v>
       </c>
@@ -12400,7 +12404,7 @@
       </c>
       <c r="I293" s="30"/>
     </row>
-    <row r="294" spans="1:9" ht="60">
+    <row r="294" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A294" s="28" t="s">
         <v>836</v>
       </c>
@@ -12425,7 +12429,7 @@
       </c>
       <c r="I294" s="30"/>
     </row>
-    <row r="295" spans="1:9" ht="45">
+    <row r="295" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="28" t="s">
         <v>289</v>
       </c>
@@ -12450,7 +12454,7 @@
       </c>
       <c r="I295" s="30"/>
     </row>
-    <row r="296" spans="1:9" ht="30">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="28" t="s">
         <v>290</v>
       </c>
@@ -12475,7 +12479,7 @@
       </c>
       <c r="I296" s="30"/>
     </row>
-    <row r="297" spans="1:9" ht="30">
+    <row r="297" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="28" t="s">
         <v>291</v>
       </c>
@@ -12500,7 +12504,7 @@
       </c>
       <c r="I297" s="30"/>
     </row>
-    <row r="298" spans="1:9" ht="30">
+    <row r="298" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="28" t="s">
         <v>292</v>
       </c>
@@ -12525,7 +12529,7 @@
       </c>
       <c r="I298" s="30"/>
     </row>
-    <row r="299" spans="1:9" ht="60">
+    <row r="299" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A299" s="28" t="s">
         <v>293</v>
       </c>
@@ -12550,7 +12554,7 @@
       </c>
       <c r="I299" s="30"/>
     </row>
-    <row r="300" spans="1:9" ht="75">
+    <row r="300" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A300" s="28" t="s">
         <v>294</v>
       </c>
@@ -12575,7 +12579,7 @@
       </c>
       <c r="I300" s="30"/>
     </row>
-    <row r="301" spans="1:9" ht="45">
+    <row r="301" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A301" s="28" t="s">
         <v>295</v>
       </c>
@@ -12600,7 +12604,7 @@
       </c>
       <c r="I301" s="30"/>
     </row>
-    <row r="302" spans="1:9" ht="30">
+    <row r="302" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A302" s="28" t="s">
         <v>296</v>
       </c>
@@ -12625,7 +12629,7 @@
       </c>
       <c r="I302" s="30"/>
     </row>
-    <row r="303" spans="1:9" ht="30">
+    <row r="303" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="28" t="s">
         <v>297</v>
       </c>
@@ -12650,7 +12654,7 @@
       </c>
       <c r="I303" s="30"/>
     </row>
-    <row r="304" spans="1:9" ht="30">
+    <row r="304" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A304" s="28" t="s">
         <v>298</v>
       </c>
@@ -12675,7 +12679,7 @@
       </c>
       <c r="I304" s="30"/>
     </row>
-    <row r="305" spans="1:9" ht="30">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" s="28" t="s">
         <v>838</v>
       </c>
@@ -12700,7 +12704,7 @@
       </c>
       <c r="I305" s="30"/>
     </row>
-    <row r="306" spans="1:9" ht="30">
+    <row r="306" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A306" s="28" t="s">
         <v>839</v>
       </c>
@@ -12725,7 +12729,7 @@
       </c>
       <c r="I306" s="30"/>
     </row>
-    <row r="307" spans="1:9" ht="45">
+    <row r="307" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A307" s="28" t="s">
         <v>299</v>
       </c>
@@ -12750,7 +12754,7 @@
       </c>
       <c r="I307" s="30"/>
     </row>
-    <row r="308" spans="1:9" ht="45">
+    <row r="308" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A308" s="28" t="s">
         <v>300</v>
       </c>
@@ -12775,7 +12779,7 @@
       </c>
       <c r="I308" s="30"/>
     </row>
-    <row r="309" spans="1:9" ht="240">
+    <row r="309" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A309" s="28" t="s">
         <v>301</v>
       </c>
@@ -12800,7 +12804,7 @@
       </c>
       <c r="I309" s="30"/>
     </row>
-    <row r="310" spans="1:9" ht="45">
+    <row r="310" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="28" t="s">
         <v>302</v>
       </c>
@@ -12825,7 +12829,7 @@
       </c>
       <c r="I310" s="30"/>
     </row>
-    <row r="311" spans="1:9" ht="30">
+    <row r="311" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A311" s="28" t="s">
         <v>303</v>
       </c>
@@ -12850,7 +12854,7 @@
       </c>
       <c r="I311" s="30"/>
     </row>
-    <row r="312" spans="1:9" ht="30">
+    <row r="312" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A312" s="28" t="s">
         <v>304</v>
       </c>
@@ -12875,7 +12879,7 @@
       </c>
       <c r="I312" s="30"/>
     </row>
-    <row r="313" spans="1:9" ht="45">
+    <row r="313" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A313" s="28" t="s">
         <v>305</v>
       </c>
@@ -12900,7 +12904,7 @@
       </c>
       <c r="I313" s="30"/>
     </row>
-    <row r="314" spans="1:9" ht="45">
+    <row r="314" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A314" s="28" t="s">
         <v>306</v>
       </c>
@@ -12925,7 +12929,7 @@
       </c>
       <c r="I314" s="30"/>
     </row>
-    <row r="315" spans="1:9" ht="135">
+    <row r="315" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A315" s="28" t="s">
         <v>307</v>
       </c>
@@ -12950,7 +12954,7 @@
       </c>
       <c r="I315" s="30"/>
     </row>
-    <row r="316" spans="1:9" ht="30">
+    <row r="316" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A316" s="28" t="s">
         <v>308</v>
       </c>
@@ -12975,7 +12979,7 @@
       </c>
       <c r="I316" s="30"/>
     </row>
-    <row r="317" spans="1:9" ht="30">
+    <row r="317" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A317" s="28" t="s">
         <v>309</v>
       </c>
@@ -13000,7 +13004,7 @@
       </c>
       <c r="I317" s="30"/>
     </row>
-    <row r="318" spans="1:9" ht="225">
+    <row r="318" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A318" s="28" t="s">
         <v>310</v>
       </c>
@@ -13025,7 +13029,7 @@
       </c>
       <c r="I318" s="30"/>
     </row>
-    <row r="319" spans="1:9" ht="30">
+    <row r="319" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A319" s="28" t="s">
         <v>311</v>
       </c>
@@ -13050,7 +13054,7 @@
       </c>
       <c r="I319" s="30"/>
     </row>
-    <row r="320" spans="1:9" ht="30">
+    <row r="320" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A320" s="28" t="s">
         <v>312</v>
       </c>
@@ -13075,7 +13079,7 @@
       </c>
       <c r="I320" s="30"/>
     </row>
-    <row r="321" spans="1:9" ht="30">
+    <row r="321" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A321" s="28" t="s">
         <v>313</v>
       </c>
@@ -13100,7 +13104,7 @@
       </c>
       <c r="I321" s="30"/>
     </row>
-    <row r="322" spans="1:9" ht="30">
+    <row r="322" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A322" s="28" t="s">
         <v>168</v>
       </c>
@@ -13125,7 +13129,7 @@
       </c>
       <c r="I322" s="30"/>
     </row>
-    <row r="323" spans="1:9" ht="30">
+    <row r="323" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A323" s="28" t="s">
         <v>169</v>
       </c>
@@ -13150,7 +13154,7 @@
       </c>
       <c r="I323" s="30"/>
     </row>
-    <row r="324" spans="1:9" ht="255">
+    <row r="324" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A324" s="28" t="s">
         <v>170</v>
       </c>
@@ -13175,7 +13179,7 @@
       </c>
       <c r="I324" s="30"/>
     </row>
-    <row r="325" spans="1:9" ht="45">
+    <row r="325" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A325" s="28" t="s">
         <v>171</v>
       </c>
@@ -13200,7 +13204,7 @@
       </c>
       <c r="I325" s="30"/>
     </row>
-    <row r="326" spans="1:9" ht="30">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" s="28" t="s">
         <v>172</v>
       </c>
@@ -13225,7 +13229,7 @@
       </c>
       <c r="I326" s="30"/>
     </row>
-    <row r="327" spans="1:9" ht="30">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" s="28" t="s">
         <v>173</v>
       </c>
@@ -13250,7 +13254,7 @@
       </c>
       <c r="I327" s="30"/>
     </row>
-    <row r="328" spans="1:9" ht="45">
+    <row r="328" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A328" s="28" t="s">
         <v>174</v>
       </c>
@@ -13277,7 +13281,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="329" spans="1:9" ht="30">
+    <row r="329" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A329" s="28" t="s">
         <v>175</v>
       </c>
@@ -13304,7 +13308,7 @@
       </c>
       <c r="I329" s="30"/>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" s="28" t="s">
         <v>176</v>
       </c>
@@ -13329,7 +13333,7 @@
       </c>
       <c r="I330" s="30"/>
     </row>
-    <row r="331" spans="1:9" ht="30">
+    <row r="331" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A331" s="28" t="s">
         <v>177</v>
       </c>
@@ -13354,7 +13358,7 @@
       </c>
       <c r="I331" s="30"/>
     </row>
-    <row r="332" spans="1:9" ht="45">
+    <row r="332" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A332" s="28" t="s">
         <v>178</v>
       </c>
@@ -13381,7 +13385,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="333" spans="1:9" ht="30">
+    <row r="333" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A333" s="28" t="s">
         <v>179</v>
       </c>
@@ -13408,7 +13412,7 @@
       </c>
       <c r="I333" s="30"/>
     </row>
-    <row r="334" spans="1:9" ht="30">
+    <row r="334" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A334" s="28" t="s">
         <v>314</v>
       </c>
@@ -13433,7 +13437,7 @@
       </c>
       <c r="I334" s="30"/>
     </row>
-    <row r="335" spans="1:9" ht="90">
+    <row r="335" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A335" s="28" t="s">
         <v>315</v>
       </c>
@@ -13458,7 +13462,7 @@
       </c>
       <c r="I335" s="30"/>
     </row>
-    <row r="336" spans="1:9" ht="345">
+    <row r="336" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A336" s="28" t="s">
         <v>316</v>
       </c>
@@ -13483,7 +13487,7 @@
       </c>
       <c r="I336" s="30"/>
     </row>
-    <row r="337" spans="1:9" ht="30">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" s="28" t="s">
         <v>317</v>
       </c>
@@ -13508,7 +13512,7 @@
       </c>
       <c r="I337" s="30"/>
     </row>
-    <row r="338" spans="1:9" ht="30">
+    <row r="338" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A338" s="28" t="s">
         <v>318</v>
       </c>
@@ -13533,7 +13537,7 @@
       </c>
       <c r="I338" s="30"/>
     </row>
-    <row r="339" spans="1:9" ht="45">
+    <row r="339" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A339" s="28" t="s">
         <v>321</v>
       </c>
@@ -13558,7 +13562,7 @@
       </c>
       <c r="I339" s="30"/>
     </row>
-    <row r="340" spans="1:9" ht="30">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="28" t="s">
         <v>322</v>
       </c>
@@ -13583,7 +13587,7 @@
       </c>
       <c r="I340" s="30"/>
     </row>
-    <row r="341" spans="1:9" ht="30">
+    <row r="341" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A341" s="28" t="s">
         <v>323</v>
       </c>
@@ -13608,7 +13612,7 @@
       </c>
       <c r="I341" s="30"/>
     </row>
-    <row r="342" spans="1:9" ht="135">
+    <row r="342" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A342" s="28" t="s">
         <v>324</v>
       </c>
@@ -13633,7 +13637,7 @@
       </c>
       <c r="I342" s="30"/>
     </row>
-    <row r="343" spans="1:9" ht="45">
+    <row r="343" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A343" s="28" t="s">
         <v>325</v>
       </c>
@@ -13658,7 +13662,7 @@
       </c>
       <c r="I343" s="30"/>
     </row>
-    <row r="344" spans="1:9" ht="45">
+    <row r="344" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A344" s="28" t="s">
         <v>326</v>
       </c>
@@ -13683,7 +13687,7 @@
       </c>
       <c r="I344" s="30"/>
     </row>
-    <row r="345" spans="1:9" ht="30">
+    <row r="345" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A345" s="28" t="s">
         <v>327</v>
       </c>
@@ -13708,7 +13712,7 @@
       </c>
       <c r="I345" s="30"/>
     </row>
-    <row r="346" spans="1:9" ht="30">
+    <row r="346" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A346" s="28" t="s">
         <v>328</v>
       </c>
@@ -13733,7 +13737,7 @@
       </c>
       <c r="I346" s="30"/>
     </row>
-    <row r="347" spans="1:9" ht="30">
+    <row r="347" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A347" s="28" t="s">
         <v>329</v>
       </c>
@@ -13741,7 +13745,7 @@
         <v>430</v>
       </c>
       <c r="C347" s="19" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D347" s="28"/>
       <c r="E347" s="28" t="s">
@@ -13758,7 +13762,7 @@
       </c>
       <c r="I347" s="30"/>
     </row>
-    <row r="348" spans="1:9" ht="30">
+    <row r="348" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A348" s="28" t="s">
         <v>330</v>
       </c>
@@ -13783,7 +13787,7 @@
       </c>
       <c r="I348" s="30"/>
     </row>
-    <row r="349" spans="1:9" ht="30">
+    <row r="349" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A349" s="28" t="s">
         <v>331</v>
       </c>
@@ -13791,7 +13795,7 @@
         <v>430</v>
       </c>
       <c r="C349" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D349" s="28"/>
       <c r="E349" s="28" t="s">
@@ -13808,7 +13812,7 @@
       </c>
       <c r="I349" s="30"/>
     </row>
-    <row r="350" spans="1:9" ht="30">
+    <row r="350" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A350" s="28" t="s">
         <v>332</v>
       </c>
@@ -13833,7 +13837,7 @@
       </c>
       <c r="I350" s="30"/>
     </row>
-    <row r="351" spans="1:9" ht="30">
+    <row r="351" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A351" s="28" t="s">
         <v>333</v>
       </c>
@@ -13858,7 +13862,7 @@
       </c>
       <c r="I351" s="30"/>
     </row>
-    <row r="352" spans="1:9" ht="30">
+    <row r="352" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A352" s="28" t="s">
         <v>334</v>
       </c>
@@ -13866,7 +13870,7 @@
         <v>430</v>
       </c>
       <c r="C352" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D352" s="28"/>
       <c r="E352" s="28" t="s">
@@ -13883,7 +13887,7 @@
       </c>
       <c r="I352" s="30"/>
     </row>
-    <row r="353" spans="1:9" ht="30">
+    <row r="353" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A353" s="28" t="s">
         <v>335</v>
       </c>
@@ -13908,7 +13912,7 @@
       </c>
       <c r="I353" s="30"/>
     </row>
-    <row r="354" spans="1:9" ht="30">
+    <row r="354" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A354" s="28" t="s">
         <v>336</v>
       </c>
@@ -13933,7 +13937,7 @@
       </c>
       <c r="I354" s="30"/>
     </row>
-    <row r="355" spans="1:9" ht="30">
+    <row r="355" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A355" s="28" t="s">
         <v>337</v>
       </c>
@@ -13958,7 +13962,7 @@
       </c>
       <c r="I355" s="30"/>
     </row>
-    <row r="356" spans="1:9" ht="90">
+    <row r="356" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A356" s="28" t="s">
         <v>338</v>
       </c>
@@ -13983,7 +13987,7 @@
       </c>
       <c r="I356" s="30"/>
     </row>
-    <row r="357" spans="1:9" ht="45">
+    <row r="357" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A357" s="28" t="s">
         <v>339</v>
       </c>
@@ -14008,7 +14012,7 @@
       </c>
       <c r="I357" s="30"/>
     </row>
-    <row r="358" spans="1:9" ht="45">
+    <row r="358" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A358" s="28" t="s">
         <v>340</v>
       </c>
@@ -14033,7 +14037,7 @@
       </c>
       <c r="I358" s="30"/>
     </row>
-    <row r="359" spans="1:9" ht="30">
+    <row r="359" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A359" s="28" t="s">
         <v>341</v>
       </c>
@@ -14058,7 +14062,7 @@
       </c>
       <c r="I359" s="30"/>
     </row>
-    <row r="360" spans="1:9" ht="30">
+    <row r="360" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A360" s="28" t="s">
         <v>342</v>
       </c>
@@ -14083,7 +14087,7 @@
       </c>
       <c r="I360" s="30"/>
     </row>
-    <row r="361" spans="1:9" ht="30">
+    <row r="361" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A361" s="28" t="s">
         <v>343</v>
       </c>
@@ -14091,7 +14095,7 @@
         <v>431</v>
       </c>
       <c r="C361" s="19" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D361" s="28"/>
       <c r="E361" s="28" t="s">
@@ -14108,7 +14112,7 @@
       </c>
       <c r="I361" s="30"/>
     </row>
-    <row r="362" spans="1:9" ht="30">
+    <row r="362" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A362" s="28" t="s">
         <v>344</v>
       </c>
@@ -14133,7 +14137,7 @@
       </c>
       <c r="I362" s="30"/>
     </row>
-    <row r="363" spans="1:9" ht="45">
+    <row r="363" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A363" s="28" t="s">
         <v>319</v>
       </c>
@@ -14158,7 +14162,7 @@
       </c>
       <c r="I363" s="30"/>
     </row>
-    <row r="364" spans="1:9" ht="45">
+    <row r="364" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A364" s="28" t="s">
         <v>320</v>
       </c>
@@ -14183,7 +14187,7 @@
       </c>
       <c r="I364" s="30"/>
     </row>
-    <row r="365" spans="1:9" ht="45">
+    <row r="365" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A365" s="28" t="s">
         <v>850</v>
       </c>
@@ -14208,7 +14212,7 @@
       </c>
       <c r="I365" s="30"/>
     </row>
-    <row r="366" spans="1:9" ht="60">
+    <row r="366" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A366" s="28" t="s">
         <v>851</v>
       </c>
@@ -14233,7 +14237,7 @@
       </c>
       <c r="I366" s="30"/>
     </row>
-    <row r="367" spans="1:9" ht="45">
+    <row r="367" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A367" s="28" t="s">
         <v>345</v>
       </c>
@@ -14258,7 +14262,7 @@
       </c>
       <c r="I367" s="30"/>
     </row>
-    <row r="368" spans="1:9">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" s="28" t="s">
         <v>346</v>
       </c>
@@ -14283,7 +14287,7 @@
       </c>
       <c r="I368" s="30"/>
     </row>
-    <row r="369" spans="1:9" ht="30">
+    <row r="369" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A369" s="28" t="s">
         <v>347</v>
       </c>
@@ -14308,7 +14312,7 @@
       </c>
       <c r="I369" s="30"/>
     </row>
-    <row r="370" spans="1:9" ht="75">
+    <row r="370" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A370" s="28" t="s">
         <v>348</v>
       </c>
@@ -14333,7 +14337,7 @@
       </c>
       <c r="I370" s="30"/>
     </row>
-    <row r="371" spans="1:9" ht="75">
+    <row r="371" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A371" s="28" t="s">
         <v>349</v>
       </c>
@@ -14358,7 +14362,7 @@
       </c>
       <c r="I371" s="30"/>
     </row>
-    <row r="372" spans="1:9" ht="60">
+    <row r="372" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A372" s="28" t="s">
         <v>350</v>
       </c>
@@ -14383,7 +14387,7 @@
       </c>
       <c r="I372" s="30"/>
     </row>
-    <row r="373" spans="1:9" ht="30">
+    <row r="373" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A373" s="28" t="s">
         <v>351</v>
       </c>
@@ -14408,7 +14412,7 @@
       </c>
       <c r="I373" s="30"/>
     </row>
-    <row r="374" spans="1:9" ht="30">
+    <row r="374" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A374" s="28" t="s">
         <v>352</v>
       </c>
@@ -14433,7 +14437,7 @@
       </c>
       <c r="I374" s="30"/>
     </row>
-    <row r="375" spans="1:9" ht="30">
+    <row r="375" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A375" s="28" t="s">
         <v>353</v>
       </c>
@@ -14458,7 +14462,7 @@
       </c>
       <c r="I375" s="30"/>
     </row>
-    <row r="376" spans="1:9" ht="45">
+    <row r="376" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A376" s="28" t="s">
         <v>354</v>
       </c>
@@ -14483,7 +14487,7 @@
       </c>
       <c r="I376" s="30"/>
     </row>
-    <row r="377" spans="1:9" ht="150">
+    <row r="377" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A377" s="28" t="s">
         <v>355</v>
       </c>
@@ -14508,7 +14512,7 @@
       </c>
       <c r="I377" s="30"/>
     </row>
-    <row r="378" spans="1:9" ht="30">
+    <row r="378" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A378" s="28" t="s">
         <v>356</v>
       </c>
@@ -14533,7 +14537,7 @@
       </c>
       <c r="I378" s="30"/>
     </row>
-    <row r="379" spans="1:9" ht="285">
+    <row r="379" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A379" s="28" t="s">
         <v>357</v>
       </c>
@@ -14558,7 +14562,7 @@
       </c>
       <c r="I379" s="30"/>
     </row>
-    <row r="380" spans="1:9" ht="45">
+    <row r="380" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A380" s="28" t="s">
         <v>358</v>
       </c>
@@ -14583,7 +14587,7 @@
       </c>
       <c r="I380" s="30"/>
     </row>
-    <row r="381" spans="1:9" ht="30">
+    <row r="381" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A381" s="28" t="s">
         <v>359</v>
       </c>
@@ -14608,7 +14612,7 @@
       </c>
       <c r="I381" s="30"/>
     </row>
-    <row r="382" spans="1:9" ht="30">
+    <row r="382" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A382" s="28" t="s">
         <v>360</v>
       </c>
@@ -14633,7 +14637,7 @@
       </c>
       <c r="I382" s="30"/>
     </row>
-    <row r="383" spans="1:9" ht="30">
+    <row r="383" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A383" s="28" t="s">
         <v>361</v>
       </c>
@@ -14658,7 +14662,7 @@
       </c>
       <c r="I383" s="30"/>
     </row>
-    <row r="384" spans="1:9" ht="30">
+    <row r="384" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A384" s="28" t="s">
         <v>362</v>
       </c>
@@ -14683,7 +14687,7 @@
       </c>
       <c r="I384" s="30"/>
     </row>
-    <row r="385" spans="1:9" ht="345">
+    <row r="385" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A385" s="28" t="s">
         <v>363</v>
       </c>
@@ -14708,7 +14712,7 @@
       </c>
       <c r="I385" s="30"/>
     </row>
-    <row r="386" spans="1:9" ht="45">
+    <row r="386" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A386" s="28" t="s">
         <v>364</v>
       </c>
@@ -14733,7 +14737,7 @@
       </c>
       <c r="I386" s="30"/>
     </row>
-    <row r="387" spans="1:9" ht="30">
+    <row r="387" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A387" s="28" t="s">
         <v>365</v>
       </c>
@@ -14758,7 +14762,7 @@
       </c>
       <c r="I387" s="30"/>
     </row>
-    <row r="388" spans="1:9" ht="30">
+    <row r="388" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A388" s="28" t="s">
         <v>366</v>
       </c>
@@ -14783,7 +14787,7 @@
       </c>
       <c r="I388" s="30"/>
     </row>
-    <row r="389" spans="1:9" ht="90">
+    <row r="389" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A389" s="28" t="s">
         <v>367</v>
       </c>
@@ -14810,7 +14814,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="390" spans="1:9" ht="30">
+    <row r="390" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A390" s="28" t="s">
         <v>368</v>
       </c>
@@ -14837,7 +14841,7 @@
       </c>
       <c r="I390" s="30"/>
     </row>
-    <row r="391" spans="1:9" ht="30">
+    <row r="391" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A391" s="28" t="s">
         <v>373</v>
       </c>
@@ -14862,7 +14866,7 @@
       </c>
       <c r="I391" s="30"/>
     </row>
-    <row r="392" spans="1:9" ht="30">
+    <row r="392" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A392" s="28" t="s">
         <v>374</v>
       </c>
@@ -14887,7 +14891,7 @@
       </c>
       <c r="I392" s="30"/>
     </row>
-    <row r="393" spans="1:9" ht="45">
+    <row r="393" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A393" s="28" t="s">
         <v>375</v>
       </c>
@@ -14914,7 +14918,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="394" spans="1:9" ht="30">
+    <row r="394" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A394" s="28" t="s">
         <v>376</v>
       </c>
@@ -14939,7 +14943,7 @@
       </c>
       <c r="I394" s="30"/>
     </row>
-    <row r="395" spans="1:9" ht="45">
+    <row r="395" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A395" s="28" t="s">
         <v>873</v>
       </c>
@@ -14964,7 +14968,7 @@
       </c>
       <c r="I395" s="30"/>
     </row>
-    <row r="396" spans="1:9" ht="45">
+    <row r="396" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A396" s="28" t="s">
         <v>876</v>
       </c>
@@ -14991,7 +14995,7 @@
       </c>
       <c r="I396" s="30"/>
     </row>
-    <row r="397" spans="1:9" ht="30">
+    <row r="397" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A397" s="28" t="s">
         <v>377</v>
       </c>
@@ -15016,7 +15020,7 @@
       </c>
       <c r="I397" s="30"/>
     </row>
-    <row r="398" spans="1:9" ht="30">
+    <row r="398" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A398" s="28" t="s">
         <v>378</v>
       </c>
@@ -15041,7 +15045,7 @@
       </c>
       <c r="I398" s="30"/>
     </row>
-    <row r="399" spans="1:9" ht="45">
+    <row r="399" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A399" s="28" t="s">
         <v>379</v>
       </c>
@@ -15049,7 +15053,7 @@
         <v>439</v>
       </c>
       <c r="C399" s="19" t="s">
-        <v>941</v>
+        <v>947</v>
       </c>
       <c r="D399" s="28"/>
       <c r="E399" s="28" t="s">
@@ -15066,7 +15070,7 @@
       </c>
       <c r="I399" s="30"/>
     </row>
-    <row r="400" spans="1:9" ht="30">
+    <row r="400" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A400" s="28" t="s">
         <v>380</v>
       </c>
@@ -15074,7 +15078,7 @@
         <v>439</v>
       </c>
       <c r="C400" s="19" t="s">
-        <v>942</v>
+        <v>948</v>
       </c>
       <c r="D400" s="28"/>
       <c r="E400" s="28" t="s">
@@ -15091,7 +15095,7 @@
       </c>
       <c r="I400" s="30"/>
     </row>
-    <row r="401" spans="1:9" ht="45">
+    <row r="401" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A401" s="28" t="s">
         <v>381</v>
       </c>
@@ -15120,7 +15124,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="402" spans="1:9" ht="75">
+    <row r="402" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A402" s="28" t="s">
         <v>766</v>
       </c>
@@ -15149,7 +15153,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="403" spans="1:9" ht="30">
+    <row r="403" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A403" s="28" t="s">
         <v>877</v>
       </c>
@@ -15176,7 +15180,7 @@
       </c>
       <c r="I403" s="30"/>
     </row>
-    <row r="404" spans="1:9" ht="45">
+    <row r="404" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A404" s="28" t="s">
         <v>878</v>
       </c>
@@ -15205,7 +15209,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="405" spans="1:9" ht="30">
+    <row r="405" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A405" s="28" t="s">
         <v>879</v>
       </c>
@@ -15232,7 +15236,7 @@
       </c>
       <c r="I405" s="19"/>
     </row>
-    <row r="406" spans="1:9" ht="45">
+    <row r="406" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A406" s="28" t="s">
         <v>880</v>
       </c>
@@ -15261,7 +15265,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="407" spans="1:9" ht="45">
+    <row r="407" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A407" s="28" t="s">
         <v>888</v>
       </c>
@@ -15290,7 +15294,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="408" spans="1:9" ht="30">
+    <row r="408" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A408" s="28" t="s">
         <v>920</v>
       </c>
@@ -15298,7 +15302,7 @@
         <v>439</v>
       </c>
       <c r="C408" s="19" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="D408" s="28" t="s">
         <v>921</v>
@@ -15317,7 +15321,7 @@
       </c>
       <c r="I408" s="30"/>
     </row>
-    <row r="409" spans="1:9" ht="45">
+    <row r="409" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A409" s="28" t="s">
         <v>881</v>
       </c>
@@ -15344,7 +15348,7 @@
       </c>
       <c r="I409" s="19"/>
     </row>
-    <row r="410" spans="1:9" ht="45">
+    <row r="410" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A410" s="28" t="s">
         <v>882</v>
       </c>
@@ -15352,7 +15356,7 @@
         <v>439</v>
       </c>
       <c r="C410" s="19" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="D410" s="21" t="s">
         <v>905</v>
@@ -15373,7 +15377,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="411" spans="1:9" ht="60">
+    <row r="411" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A411" s="28" t="s">
         <v>883</v>
       </c>
@@ -15400,7 +15404,7 @@
       </c>
       <c r="I411" s="30"/>
     </row>
-    <row r="412" spans="1:9" ht="45">
+    <row r="412" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A412" s="28" t="s">
         <v>884</v>
       </c>
@@ -15429,7 +15433,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="413" spans="1:9" ht="45">
+    <row r="413" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A413" s="28" t="s">
         <v>885</v>
       </c>
@@ -15456,7 +15460,7 @@
       </c>
       <c r="I413" s="30"/>
     </row>
-    <row r="414" spans="1:9" ht="45">
+    <row r="414" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A414" s="28" t="s">
         <v>886</v>
       </c>
@@ -15485,7 +15489,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="415" spans="1:9" ht="75">
+    <row r="415" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A415" s="28" t="s">
         <v>369</v>
       </c>
@@ -15514,7 +15518,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="416" spans="1:9" ht="75">
+    <row r="416" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A416" s="28" t="s">
         <v>370</v>
       </c>
@@ -15543,7 +15547,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="417" spans="1:9" ht="75">
+    <row r="417" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A417" s="28" t="s">
         <v>371</v>
       </c>
@@ -15572,7 +15576,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="418" spans="1:9" ht="105">
+    <row r="418" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A418" s="28" t="s">
         <v>372</v>
       </c>
@@ -15601,7 +15605,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="419" spans="1:9" ht="30">
+    <row r="419" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A419" s="21" t="s">
         <v>893</v>
       </c>
@@ -15628,15 +15632,15 @@
       </c>
       <c r="I419" s="30"/>
     </row>
-    <row r="420" spans="1:9" ht="45">
+    <row r="420" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A420" s="21" t="s">
         <v>382</v>
       </c>
       <c r="B420" s="23" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="C420" s="19" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="D420" s="28"/>
       <c r="E420" s="28" t="s">
@@ -15653,15 +15657,15 @@
       </c>
       <c r="I420" s="30"/>
     </row>
-    <row r="421" spans="1:9" ht="30">
+    <row r="421" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A421" s="28" t="s">
         <v>383</v>
       </c>
       <c r="B421" s="23" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="C421" s="19" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="D421" s="28"/>
       <c r="E421" s="28" t="s">
@@ -15678,12 +15682,12 @@
       </c>
       <c r="I421" s="30"/>
     </row>
-    <row r="422" spans="1:9" ht="360">
+    <row r="422" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A422" s="28" t="s">
         <v>384</v>
       </c>
       <c r="B422" s="23" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="C422" s="19" t="s">
         <v>712</v>
@@ -15703,27 +15707,27 @@
       </c>
       <c r="I422" s="30"/>
     </row>
-    <row r="423" spans="1:9">
+    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A423" s="3"/>
       <c r="B423" s="10"/>
     </row>
-    <row r="424" spans="1:9">
+    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A424" s="3"/>
       <c r="B424" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A238:I290 A293:I362 A395:H395 A365:I394 A126:I233 A125:H125 A20:I124 A396:I422">

</xml_diff>

<commit_message>
update RS of MS-OXWSATT,MS-OXWSCORE
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F65448-C719-4440-B0E9-7FDDA90EB6B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D05AB-C5E0-4715-84BE-FF504597B01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -3543,22 +3543,22 @@
     <t>[In Appendix C: Product Behavior] Implementation does not return the items of type t:ItemType as a t:MessageType type.(&lt;3&gt; Section 2.2.4.6:  Exchange 2007 does not return the items of type t:ItemType as a t:MessageType type. )</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does return a ItemType item.(Microsoft Exchange Server 2007 Service Pack 1 (SP1) starts to return the items of type t:ItemType as a t:MessageType type.)</t>
-  </si>
-  <si>
     <t>[In t:ItemAttachmentType Complex Type][The type of Item element is] t:ItemType ([MS-OXWSCORE] section 2.2.4.24).</t>
   </si>
   <si>
     <t>MS-OXWSATT_R444:i,MS-OXWSATT_R1:i</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXWSATT_R318015.</t>
-  </si>
-  <si>
     <t>[In t:ItemAttachmentType Complex Type] [The type of RoleMember element is] t:RoleMemberItemType ([MS-OXWSCORE] section 2.2.4.43)</t>
   </si>
   <si>
     <t>[In t:ItemAttachmentType Complex Type] [The type of Network element is] t:NetworkItemType ([MS-OXWSCORE] section 2.2.4.30)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does return the items of type t:ItemType as a t:MessageType type.(Microsoft Exchange Server 2007 Service Pack 1 (SP1) starts to return the items of type t:ItemType as a t:MessageType type.)</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSATT_R318014.</t>
   </si>
 </sst>
 </file>
@@ -3871,6 +3871,27 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3894,27 +3915,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5150,8 +5150,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M425"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:I7"/>
+    <sheetView tabSelected="1" topLeftCell="D123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I126" sqref="I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5217,16 +5217,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -5238,13 +5238,13 @@
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -5252,16 +5252,16 @@
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -5269,16 +5269,16 @@
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -5286,16 +5286,16 @@
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -5303,16 +5303,16 @@
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -5320,16 +5320,16 @@
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="48" t="s">
         <v>738</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -5337,16 +5337,16 @@
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="45" t="s">
         <v>737</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="55"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -5430,16 +5430,16 @@
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -5447,16 +5447,16 @@
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="55"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -5464,16 +5464,16 @@
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="45" t="s">
         <v>739</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -8158,7 +8158,7 @@
         <v>397</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D124" s="28"/>
       <c r="E124" s="28" t="s">
@@ -8224,7 +8224,7 @@
         <v>17</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="30">
@@ -8685,7 +8685,7 @@
         <v>397</v>
       </c>
       <c r="C145" s="19" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D145" s="28"/>
       <c r="E145" s="28" t="s">
@@ -8735,7 +8735,7 @@
         <v>397</v>
       </c>
       <c r="C147" s="19" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D147" s="28"/>
       <c r="E147" s="28" t="s">
@@ -15296,22 +15296,22 @@
       <c r="H407" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I407" s="30" t="s">
+      <c r="I407" s="19" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="408" spans="1:9" ht="45">
-      <c r="A408" s="28" t="s">
-        <v>886</v>
+      <c r="A408" s="21" t="s">
+        <v>916</v>
       </c>
       <c r="B408" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C408" s="19" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
       <c r="D408" s="21" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E408" s="28" t="s">
         <v>22</v>
@@ -15322,23 +15322,23 @@
       <c r="G408" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H408" s="28" t="s">
+      <c r="H408" s="21" t="s">
         <v>18</v>
       </c>
       <c r="I408" s="19"/>
     </row>
     <row r="409" spans="1:9" ht="45">
       <c r="A409" s="21" t="s">
-        <v>916</v>
+        <v>886</v>
       </c>
       <c r="B409" s="29" t="s">
         <v>439</v>
       </c>
       <c r="C409" s="19" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D409" s="21" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E409" s="28" t="s">
         <v>22</v>
@@ -15349,7 +15349,7 @@
       <c r="G409" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H409" s="28" t="s">
+      <c r="H409" s="21" t="s">
         <v>20</v>
       </c>
       <c r="I409" s="30" t="s">
@@ -15752,17 +15752,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A239:I291 A294:I363 A396:H396 A366:I395 A127:I234 A125:H126 A20:I124 A397:I423">

</xml_diff>

<commit_message>
update RS of MS-OXWSATT and test case code.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSATT/MS-OXWSATT_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D05AB-C5E0-4715-84BE-FF504597B01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF52601-0611-4464-A31C-7C1F5F881D16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3871,27 +3871,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3915,6 +3894,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5150,8 +5150,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I126" sqref="I126"/>
+    <sheetView tabSelected="1" topLeftCell="A405" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C409" sqref="C409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5217,16 +5217,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -5238,13 +5238,13 @@
       <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -5252,16 +5252,16 @@
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="58"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -5269,16 +5269,16 @@
       <c r="A7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -5286,16 +5286,16 @@
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -5303,16 +5303,16 @@
       <c r="A9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -5320,16 +5320,16 @@
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="56" t="s">
         <v>738</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -5337,16 +5337,16 @@
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>737</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -5430,16 +5430,16 @@
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -5447,16 +5447,16 @@
       <c r="A17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -5464,16 +5464,16 @@
       <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>739</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -15308,7 +15308,7 @@
         <v>439</v>
       </c>
       <c r="C408" s="19" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="D408" s="21" t="s">
         <v>947</v>
@@ -15335,7 +15335,7 @@
         <v>439</v>
       </c>
       <c r="C409" s="19" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
       <c r="D409" s="21" t="s">
         <v>947</v>
@@ -15752,17 +15752,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A239:I291 A294:I363 A396:H396 A366:I395 A127:I234 A125:H126 A20:I124 A397:I423">

</xml_diff>